<commit_message>
CI: Auto Update Data (#66)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/模组任务.xlsx
+++ b/Excel/模组任务.xlsx
@@ -410,7 +410,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE330"/>
+  <dimension ref="A1:AA330"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
@@ -455,7 +455,7 @@
     <row r="1">
       <c r="A1" s="5" t="inlineStr">
         <is>
-          <t>更新日期：2024.09.22 01:35:26</t>
+          <t>更新日期：2024.09.22 08:01:38</t>
         </is>
       </c>
     </row>
@@ -5638,7 +5638,7 @@
       </c>
       <c r="C286" s="4" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战寒檀并上场，且每次战斗至少释放1次“女巫之泪”&gt; 3星通关别传别传BI-2；必须编入非助战寒檀并上场，且使用寒檀至少歼灭8个敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战寒檀并上场，且每次战斗至少释放1次“女巫之泪”&gt; 3星通关别传BI-2；必须编入非助战寒檀并上场，且使用寒檀至少歼灭8个敌人</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#192)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/模组任务.xlsx
+++ b/Excel/模组任务.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA386"/>
+  <dimension ref="A1:AA392"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A300" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="D300" sqref="D300"/>
@@ -465,7 +465,7 @@
     <row r="1">
       <c r="A1" s="8" t="inlineStr">
         <is>
-          <t>更新日期：2025.05.24 13:19:10</t>
+          <t>更新日期：2025.06.10 00:49:28</t>
         </is>
       </c>
     </row>
@@ -3739,63 +3739,63 @@
       </c>
       <c r="B174" s="8" t="inlineStr">
         <is>
-          <t>MB-EX-3</t>
+          <t>LE-5</t>
         </is>
       </c>
       <c r="C174" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战山累计造成40歼灭数&gt; 3星通关别传MB-EX-3；必须编入非助战山并上场，且不编入其他近卫干员</t>
+          <t>&gt; 完成5次战斗，必须编入非助战山，且每次战斗使用山造成至少12000点伤害&gt; 3星通关插曲LE-5，必须编入非助战山并上场，且使用山歼灭至少10名敌人</t>
         </is>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="8" t="inlineStr">
         <is>
-          <t>豆苗</t>
+          <t>山</t>
         </is>
       </c>
       <c r="B175" s="8" t="inlineStr">
         <is>
-          <t>S3-7</t>
+          <t>MB-EX-3</t>
         </is>
       </c>
       <c r="C175" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战豆苗，并确定第一位部署的干员是豆苗&gt; 3星通关主题曲S3-7；必须编入非助战豆苗并上场，且至少使用1次“大家一起上”</t>
+          <t>&gt; 由非助战山累计造成40歼灭数&gt; 3星通关别传MB-EX-3；必须编入非助战山并上场，且不编入其他近卫干员</t>
         </is>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="8" t="inlineStr">
         <is>
-          <t>爱丽丝</t>
+          <t>豆苗</t>
         </is>
       </c>
       <c r="B176" s="8" t="inlineStr">
         <is>
-          <t>2-2</t>
+          <t>S3-7</t>
         </is>
       </c>
       <c r="C176" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战爱丽丝累计造成30歼灭数&gt; 3星通关主题曲2-2；必须编入非助战爱丽丝并上场，且使用爱丽丝歼灭至少2个重装防御者</t>
+          <t>&gt; 完成5次战斗；必须编入非助战豆苗，并确定第一位部署的干员是豆苗&gt; 3星通关主题曲S3-7；必须编入非助战豆苗并上场，且至少使用1次“大家一起上”</t>
         </is>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="8" t="inlineStr">
         <is>
-          <t>空弦</t>
+          <t>爱丽丝</t>
         </is>
       </c>
       <c r="B177" s="8" t="inlineStr">
         <is>
-          <t>SV-4</t>
+          <t>2-2</t>
         </is>
       </c>
       <c r="C177" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战空弦累计造成100000点伤害&gt; 3星通关插曲SV-4；必须编入非助战空弦并上场，其他成员不可编入狙击干员</t>
+          <t>&gt; 由非助战爱丽丝累计造成30歼灭数&gt; 3星通关主题曲2-2；必须编入非助战爱丽丝并上场，且使用爱丽丝歼灭至少2个重装防御者</t>
         </is>
       </c>
     </row>
@@ -3807,80 +3807,80 @@
       </c>
       <c r="B178" s="8" t="inlineStr">
         <is>
-          <t>2-9</t>
+          <t>SV-4</t>
         </is>
       </c>
       <c r="C178" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战空弦并上场，且使用空弦歼灭至少5名敌人&gt; 3星通关主题曲2-9；必须编入非助战空弦并上场，且不编入其他狙击干员</t>
+          <t>&gt; 由非助战空弦累计造成100000点伤害&gt; 3星通关插曲SV-4；必须编入非助战空弦并上场，其他成员不可编入狙击干员</t>
         </is>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="8" t="inlineStr">
         <is>
-          <t>图耶</t>
+          <t>空弦</t>
         </is>
       </c>
       <c r="B179" s="8" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>2-9</t>
         </is>
       </c>
       <c r="C179" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战图耶并上场，且每次战斗至少释放1次强心剂&gt; 3星通关主题曲4-6；必须编入非助战图耶并上场，其他成员仅可编入6名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战空弦并上场，且使用空弦歼灭至少5名敌人&gt; 3星通关主题曲2-9；必须编入非助战空弦并上场，且不编入其他狙击干员</t>
         </is>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="8" t="inlineStr">
         <is>
-          <t>炎狱炎熔</t>
+          <t>图耶</t>
         </is>
       </c>
       <c r="B180" s="8" t="inlineStr">
         <is>
-          <t>WR-4</t>
+          <t>4-6</t>
         </is>
       </c>
       <c r="C180" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战炎狱炎熔累计造成80歼灭数&gt; 3星通关别传WR-4； 必须编入非助战炎狱炎熔并上场，且使用炎狱炎熔歼灭至少8名敌人、其中包括至少1名“偷闲”</t>
+          <t>&gt; 完成5次战斗；必须编入非助战图耶并上场，且每次战斗至少释放1次强心剂&gt; 3星通关主题曲4-6；必须编入非助战图耶并上场，其他成员仅可编入6名干员</t>
         </is>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="8" t="inlineStr">
         <is>
-          <t>乌有</t>
+          <t>炎狱炎熔</t>
         </is>
       </c>
       <c r="B181" s="8" t="inlineStr">
         <is>
-          <t>3-7</t>
+          <t>WR-4</t>
         </is>
       </c>
       <c r="C181" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战乌有并部署至少2次，且使用乌有歼灭至少4名敌人&gt; 3星通关主题曲3-7；必须编入非助战乌有并上场，且使用乌有歼灭至少2个炮手</t>
+          <t>&gt; 由非助战炎狱炎熔累计造成80歼灭数&gt; 3星通关别传WR-4； 必须编入非助战炎狱炎熔并上场，且使用炎狱炎熔歼灭至少8名敌人、其中包括至少1名“偷闲”</t>
         </is>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="8" t="inlineStr">
         <is>
-          <t>嵯峨</t>
+          <t>乌有</t>
         </is>
       </c>
       <c r="B182" s="8" t="inlineStr">
         <is>
-          <t>WR-3</t>
+          <t>3-7</t>
         </is>
       </c>
       <c r="C182" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战嵯峨累计造成80000点伤害&gt; 3星通关别传WR-3；必须编入非助战嵯峨，且第一位部署嵯峨、嵯峨全程不撤退或被击倒</t>
+          <t>&gt; 完成5次战斗；必须编入非助战乌有并部署至少2次，且使用乌有歼灭至少4名敌人&gt; 3星通关主题曲3-7；必须编入非助战乌有并上场，且使用乌有歼灭至少2个炮手</t>
         </is>
       </c>
     </row>
@@ -3892,29 +3892,29 @@
       </c>
       <c r="B183" s="8" t="inlineStr">
         <is>
-          <t>WR-1</t>
+          <t>WR-3</t>
         </is>
       </c>
       <c r="C183" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战嵯峨，并确定第一位部署的干员是嵯峨&gt; 3星通关别传WR-1；必须编入非助战嵯峨并上场，其他成员仅可编入2名干员</t>
+          <t>&gt; 由非助战嵯峨累计造成80000点伤害&gt; 3星通关别传WR-3；必须编入非助战嵯峨，且第一位部署嵯峨、嵯峨全程不撤退或被击倒</t>
         </is>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="8" t="inlineStr">
         <is>
-          <t>夕</t>
+          <t>嵯峨</t>
         </is>
       </c>
       <c r="B184" s="8" t="inlineStr">
         <is>
-          <t>1-6</t>
+          <t>WR-1</t>
         </is>
       </c>
       <c r="C184" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中累计召唤非助战夕的召唤物20回&gt; 使用至多2人（包含助战）的队伍3星通关主题曲1-6；必须编入非助战夕并上场，其他成员仅可编入重装干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战嵯峨，并确定第一位部署的干员是嵯峨&gt; 3星通关别传WR-1；必须编入非助战嵯峨并上场，其他成员仅可编入2名干员</t>
         </is>
       </c>
     </row>
@@ -3926,80 +3926,80 @@
       </c>
       <c r="B185" s="8" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>1-6</t>
         </is>
       </c>
       <c r="C185" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战夕累计造成80歼灭数&gt; 3星通关主题曲4-3；必须编入非助战夕并上场，其他成员仅可编入先锋干员</t>
+          <t>&gt; 战斗中累计召唤非助战夕的召唤物20回&gt; 使用至多2人（包含助战）的队伍3星通关主题曲1-6；必须编入非助战夕并上场，其他成员仅可编入重装干员</t>
         </is>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="8" t="inlineStr">
         <is>
-          <t>战车</t>
+          <t>夕</t>
         </is>
       </c>
       <c r="B186" s="8" t="inlineStr">
         <is>
-          <t>S2-3</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C186" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战战车累计造成150000点伤害&gt; 使用至多2人（包含助战）的队伍3星通关主题曲S2-3；必须编入非助战战车并上场，其他成员仅可编入重装干员</t>
+          <t>&gt; 由非助战夕累计造成80歼灭数&gt; 3星通关主题曲4-3；必须编入非助战夕并上场，其他成员仅可编入先锋干员</t>
         </is>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="8" t="inlineStr">
         <is>
-          <t>闪击</t>
+          <t>战车</t>
         </is>
       </c>
       <c r="B187" s="8" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>S2-3</t>
         </is>
       </c>
       <c r="C187" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战闪击累计造成30歼灭数&gt; 3星通关主题曲3-4；必须编入非助战闪击并上场，且使用闪击歼灭至少2名屠夫</t>
+          <t>&gt; 由非助战战车累计造成150000点伤害&gt; 使用至多2人（包含助战）的队伍3星通关主题曲S2-3；必须编入非助战战车并上场，其他成员仅可编入重装干员</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="8" t="inlineStr">
         <is>
-          <t>霜华</t>
+          <t>闪击</t>
         </is>
       </c>
       <c r="B188" s="8" t="inlineStr">
         <is>
-          <t>4-4</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="C188" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战霜华累计造成100000点伤害※迎宾踏垫造成的伤害可计数&gt; 3星通关主题曲4-4；必须编入非助战霜华并上场，且使用霜华歼灭弑君者※允许使用迎宾踏垫歼灭弑君者</t>
+          <t>&gt; 由非助战闪击累计造成30歼灭数&gt; 3星通关主题曲3-4；必须编入非助战闪击并上场，且使用闪击歼灭至少2名屠夫</t>
         </is>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="8" t="inlineStr">
         <is>
-          <t>灰烬</t>
+          <t>霜华</t>
         </is>
       </c>
       <c r="B189" s="8" t="inlineStr">
         <is>
-          <t>SV-8</t>
+          <t>4-4</t>
         </is>
       </c>
       <c r="C189" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战灰烬累计造成100000点伤害&gt; 3星通关插曲SV-8；必须编入非助战灰烬并上场，且使用灰烬歼灭至少2名囊海爬行者</t>
+          <t>&gt; 由非助战霜华累计造成100000点伤害※迎宾踏垫造成的伤害可计数&gt; 3星通关主题曲4-4；必须编入非助战霜华并上场，且使用霜华歼灭弑君者※允许使用迎宾踏垫歼灭弑君者</t>
         </is>
       </c>
     </row>
@@ -4011,63 +4011,63 @@
       </c>
       <c r="B190" s="8" t="inlineStr">
         <is>
-          <t>1-12</t>
+          <t>SV-8</t>
         </is>
       </c>
       <c r="C190" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战灰烬累计歼灭10个精英敌人&gt; 3星通关主题曲1-12；必须编入非助战灰烬并上场，且使用灰烬歼灭W</t>
+          <t>&gt; 由非助战灰烬累计造成100000点伤害&gt; 3星通关插曲SV-8；必须编入非助战灰烬并上场，且使用灰烬歼灭至少2名囊海爬行者</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="8" t="inlineStr">
         <is>
-          <t>暴雨</t>
+          <t>灰烬</t>
         </is>
       </c>
       <c r="B191" s="8" t="inlineStr">
         <is>
-          <t>2-7</t>
+          <t>1-12</t>
         </is>
       </c>
       <c r="C191" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战暴雨累计使用应急迷彩30次&gt; 3星通关主题曲2-7；必须编入非助战暴雨并上场，且所有干员不被击倒</t>
+          <t>&gt; 由非助战灰烬累计歼灭10个精英敌人&gt; 3星通关主题曲1-12；必须编入非助战灰烬并上场，且使用灰烬歼灭W</t>
         </is>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="8" t="inlineStr">
         <is>
-          <t>熔泉</t>
+          <t>暴雨</t>
         </is>
       </c>
       <c r="B192" s="8" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>2-7</t>
         </is>
       </c>
       <c r="C192" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战熔泉累计歼灭20个萨卡兹敌人&gt; 3星通关主题曲4-6；必须编入非助战熔泉并上场，其他成员仅可编入6名干员</t>
+          <t>&gt; 战斗中非助战暴雨累计使用应急迷彩30次&gt; 3星通关主题曲2-7；必须编入非助战暴雨并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="8" t="inlineStr">
         <is>
-          <t>异客</t>
+          <t>熔泉</t>
         </is>
       </c>
       <c r="B193" s="8" t="inlineStr">
         <is>
-          <t>2-2</t>
+          <t>4-6</t>
         </is>
       </c>
       <c r="C193" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战异客累计使用辉煌裂片30次&gt; 3星通关主题曲2-2；必须编入非助战异客并上场，其他成员仅可编入先锋和重装干员</t>
+          <t>&gt; 由非助战熔泉累计歼灭20个萨卡兹敌人&gt; 3星通关主题曲4-6；必须编入非助战熔泉并上场，其他成员仅可编入6名干员</t>
         </is>
       </c>
     </row>
@@ -4079,46 +4079,46 @@
       </c>
       <c r="B194" s="8" t="inlineStr">
         <is>
-          <t>5-10</t>
+          <t>2-2</t>
         </is>
       </c>
       <c r="C194" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战异客并上场，且使用异客造成至少30000点伤害&gt; 3星通关主题曲5-10；必须编入非助战异客并上场，且使用异客歼灭至少2个粉碎攻坚手</t>
+          <t>&gt; 战斗中非助战异客累计使用辉煌裂片30次&gt; 3星通关主题曲2-2；必须编入非助战异客并上场，其他成员仅可编入先锋和重装干员</t>
         </is>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="8" t="inlineStr">
         <is>
-          <t>赤冬</t>
+          <t>异客</t>
         </is>
       </c>
       <c r="B195" s="8" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>5-10</t>
         </is>
       </c>
       <c r="C195" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战赤冬累计使用信影流·十文字胜5次&gt; 3星通关主题曲3-8；必须编入非助战赤冬并上场，且使用赤冬歼灭碎骨</t>
+          <t>&gt; 完成5次战斗；必须编入非助战异客并上场，且使用异客造成至少30000点伤害&gt; 3星通关主题曲5-10；必须编入非助战异客并上场，且使用异客歼灭至少2个粉碎攻坚手</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="8" t="inlineStr">
         <is>
-          <t>歌蕾蒂娅</t>
+          <t>赤冬</t>
         </is>
       </c>
       <c r="B196" s="8" t="inlineStr">
         <is>
-          <t>SV-EX-5</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C196" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战歌蕾蒂娅并上场，且每次战斗至少释放1次缺水的碎漩狂舞&gt; 3星通关插曲SV-EX-5；必须编入非助战歌蕾蒂娅，且至少使1个富营养的收割者坠落地穴</t>
+          <t>&gt; 战斗中非助战赤冬累计使用信影流·十文字胜5次&gt; 3星通关主题曲3-8；必须编入非助战赤冬并上场，且使用赤冬歼灭碎骨</t>
         </is>
       </c>
     </row>
@@ -4130,29 +4130,29 @@
       </c>
       <c r="B197" s="8" t="inlineStr">
         <is>
-          <t>SN-EX-3</t>
+          <t>SV-EX-5</t>
         </is>
       </c>
       <c r="C197" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战歌蕾蒂娅，且每次战斗至少使2名敌人坠落地穴&gt; 3星通关插曲SN-EX-3；必须编入非助战歌蕾蒂娅并上场，且使用至少2次缺水的掌握怒海或缺水的碎漩狂舞</t>
+          <t>&gt; 完成5次战斗；必须编入非助战歌蕾蒂娅并上场，且每次战斗至少释放1次缺水的碎漩狂舞&gt; 3星通关插曲SV-EX-5；必须编入非助战歌蕾蒂娅，且至少使1个富营养的收割者坠落地穴</t>
         </is>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="8" t="inlineStr">
         <is>
-          <t>凯尔希</t>
+          <t>歌蕾蒂娅</t>
         </is>
       </c>
       <c r="B198" s="8" t="inlineStr">
         <is>
-          <t>5-10</t>
+          <t>SN-EX-3</t>
         </is>
       </c>
       <c r="C198" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战凯尔希累计造成150000点伤害※Mon3tr造成的伤害会计数&gt; 3星通关主题曲5-10；必须编入非助战凯尔希并上场，且使用4次指令：熔毁</t>
+          <t>&gt; 完成5次战斗；必须编入非助战歌蕾蒂娅，且每次战斗至少使2名敌人坠落地穴&gt; 3星通关插曲SN-EX-3；必须编入非助战歌蕾蒂娅并上场，且使用至少2次缺水的掌握怒海或缺水的碎漩狂舞</t>
         </is>
       </c>
     </row>
@@ -4169,31 +4169,31 @@
       </c>
       <c r="C199" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战凯尔希累计使用指令：熔毁10次&gt; 3星通关主题曲5-10；必须编入非助战凯尔希并上场，且使用Mon3tr歼灭梅菲斯特</t>
+          <t>&gt; 由非助战凯尔希累计造成150000点伤害※Mon3tr造成的伤害会计数&gt; 3星通关主题曲5-10；必须编入非助战凯尔希并上场，且使用4次指令：熔毁</t>
         </is>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="8" t="inlineStr">
         <is>
-          <t>浊心斯卡蒂</t>
+          <t>凯尔希</t>
         </is>
       </c>
       <c r="B200" s="8" t="inlineStr">
         <is>
-          <t>SV-5</t>
+          <t>5-10</t>
         </is>
       </c>
       <c r="C200" s="6" t="inlineStr">
         <is>
-          <t>&gt; 携带非助战浊心斯卡蒂完成5次战斗，且每次战斗至少发动一次“同葬无光之愿”&gt; 3星通关插曲SV-5；必须编入非助战浊心斯卡蒂并上场，且队伍中不能有医疗干员</t>
+          <t>&gt; 战斗中非助战凯尔希累计使用指令：熔毁10次&gt; 3星通关主题曲5-10；必须编入非助战凯尔希并上场，且使用Mon3tr歼灭梅菲斯特</t>
         </is>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="8" t="inlineStr">
         <is>
-          <t>深靛</t>
+          <t>浊心斯卡蒂</t>
         </is>
       </c>
       <c r="B201" s="8" t="inlineStr">
@@ -4203,58 +4203,58 @@
       </c>
       <c r="C201" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战深靛累计造成60000点伤害&gt; 3星通关插曲SV-5；必须编入非助战深靛并上场，且使用2次光影迷宫</t>
+          <t>&gt; 携带非助战浊心斯卡蒂完成5次战斗，且每次战斗至少发动一次“同葬无光之愿”&gt; 3星通关插曲SV-5；必须编入非助战浊心斯卡蒂并上场，且队伍中不能有医疗干员</t>
         </is>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="8" t="inlineStr">
         <is>
-          <t>贝娜</t>
+          <t>深靛</t>
         </is>
       </c>
       <c r="B202" s="8" t="inlineStr">
         <is>
-          <t>2-3</t>
+          <t>SV-5</t>
         </is>
       </c>
       <c r="C202" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战贝娜并上场，且每次战斗至少释放1次快速修剪&gt; 3星通关主题曲2-3；必须编入非助战贝娜并上场，且使用贝娜歼灭至少1个重装防御者</t>
+          <t>&gt; 由非助战深靛累计造成60000点伤害&gt; 3星通关插曲SV-5；必须编入非助战深靛并上场，且使用2次光影迷宫</t>
         </is>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="8" t="inlineStr">
         <is>
-          <t>绮良</t>
+          <t>贝娜</t>
         </is>
       </c>
       <c r="B203" s="8" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="C203" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战绮良累计使用锚点捕捉5次&gt; 3星通关主题曲3-1；必须编入非助战绮良并上场，且使用绮良歼灭20个敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战贝娜并上场，且每次战斗至少释放1次快速修剪&gt; 3星通关主题曲2-3；必须编入非助战贝娜并上场，且使用贝娜歼灭至少1个重装防御者</t>
         </is>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="8" t="inlineStr">
         <is>
-          <t>卡涅利安</t>
+          <t>绮良</t>
         </is>
       </c>
       <c r="B204" s="8" t="inlineStr">
         <is>
-          <t>7-3</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="C204" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战卡涅利安累计造成120000点伤害&gt; 3星通关主题曲7-3；必须编入非助战卡涅利安并上场，且不编入重装干员</t>
+          <t>&gt; 战斗中非助战绮良累计使用锚点捕捉5次&gt; 3星通关主题曲3-1；必须编入非助战绮良并上场，且使用绮良歼灭20个敌人</t>
         </is>
       </c>
     </row>
@@ -4266,29 +4266,29 @@
       </c>
       <c r="B205" s="8" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>7-3</t>
         </is>
       </c>
       <c r="C205" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战卡涅利安累计造成80歼灭数&gt; 3星通关主题曲4-6；必须编入非助战卡涅利安并上场，其他成员仅可编入6名干员</t>
+          <t>&gt; 由非助战卡涅利安累计造成120000点伤害&gt; 3星通关主题曲7-3；必须编入非助战卡涅利安并上场，且不编入重装干员</t>
         </is>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="8" t="inlineStr">
         <is>
-          <t>帕拉斯</t>
+          <t>卡涅利安</t>
         </is>
       </c>
       <c r="B206" s="8" t="inlineStr">
         <is>
-          <t>3-6</t>
+          <t>4-6</t>
         </is>
       </c>
       <c r="C206" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战帕拉斯累计造成50歼灭数&gt; 使用至多2人（包含助战）的队伍3星通关主题曲3-6；必须编入非助战帕拉斯并上场，其他成员仅可编入医疗干员</t>
+          <t>&gt; 由非助战卡涅利安累计造成80歼灭数&gt; 3星通关主题曲4-6；必须编入非助战卡涅利安并上场，其他成员仅可编入6名干员</t>
         </is>
       </c>
     </row>
@@ -4300,63 +4300,63 @@
       </c>
       <c r="B207" s="8" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>3-6</t>
         </is>
       </c>
       <c r="C207" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战帕拉斯累计使用英勇的祝福5次&gt; 3星通关主题曲4-3；必须编入非助战帕拉斯并上场，其他成员仅可编入重装干员</t>
+          <t>&gt; 由非助战帕拉斯累计造成50歼灭数&gt; 使用至多2人（包含助战）的队伍3星通关主题曲3-6；必须编入非助战帕拉斯并上场，其他成员仅可编入医疗干员</t>
         </is>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="8" t="inlineStr">
         <is>
-          <t>龙舌兰</t>
+          <t>帕拉斯</t>
         </is>
       </c>
       <c r="B208" s="8" t="inlineStr">
         <is>
-          <t>7-11</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C208" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战龙舌兰累计造成30歼灭数&gt; 3星通关主题曲7-11；必须编入非助战龙舌兰并上场，且使用2次剑走偏锋</t>
+          <t>&gt; 战斗中非助战帕拉斯累计使用英勇的祝福5次&gt; 3星通关主题曲4-3；必须编入非助战帕拉斯并上场，其他成员仅可编入重装干员</t>
         </is>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="8" t="inlineStr">
         <is>
-          <t>羽毛笔</t>
+          <t>龙舌兰</t>
         </is>
       </c>
       <c r="B209" s="8" t="inlineStr">
         <is>
-          <t>11-6</t>
+          <t>7-11</t>
         </is>
       </c>
       <c r="C209" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战羽毛笔并上场，且使用羽毛笔造成至少12000点伤害&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战羽毛笔并上场，且使用羽毛笔至少歼灭15个敌人</t>
+          <t>&gt; 由非助战龙舌兰累计造成30歼灭数&gt; 3星通关主题曲7-11；必须编入非助战龙舌兰并上场，且使用2次剑走偏锋</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="8" t="inlineStr">
         <is>
-          <t>水月</t>
+          <t>羽毛笔</t>
         </is>
       </c>
       <c r="B210" s="8" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>11-6</t>
         </is>
       </c>
       <c r="C210" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战水月累计造成150000点伤害&gt; 3星通关主题曲4-3；必须编入非助战水月并上场，且使用水月歼灭至少2名萨卡兹狙击手</t>
+          <t>&gt; 完成5次战斗；必须编入非助战羽毛笔并上场，且使用羽毛笔造成至少12000点伤害&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战羽毛笔并上场，且使用羽毛笔至少歼灭15个敌人</t>
         </is>
       </c>
     </row>
@@ -4368,80 +4368,80 @@
       </c>
       <c r="B211" s="8" t="inlineStr">
         <is>
-          <t>4-5</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C211" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战水月累计造成50歼灭数&gt; 3星通关主题曲4-5；必须编入非助战水月并上场，且使用水月歼灭10个敌人</t>
+          <t>&gt; 由非助战水月累计造成150000点伤害&gt; 3星通关主题曲4-3；必须编入非助战水月并上场，且使用水月歼灭至少2名萨卡兹狙击手</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="8" t="inlineStr">
         <is>
-          <t>假日威龙陈</t>
+          <t>水月</t>
         </is>
       </c>
       <c r="B212" s="8" t="inlineStr">
         <is>
-          <t>9-13</t>
+          <t>4-5</t>
         </is>
       </c>
       <c r="C212" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战假日威龙陈累计造成120000伤害&gt; 3星通关主题曲9-13标准实战环境；必须编入非助战假日威龙陈并上场，且使用假日威龙陈至少歼灭20个敌人</t>
+          <t>&gt; 由非助战水月累计造成50歼灭数&gt; 3星通关主题曲4-5；必须编入非助战水月并上场，且使用水月歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="8" t="inlineStr">
         <is>
-          <t>罗比菈塔</t>
+          <t>假日威龙陈</t>
         </is>
       </c>
       <c r="B213" s="8" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>9-13</t>
         </is>
       </c>
       <c r="C213" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战罗比菈塔累计部署支援装置25个&gt; 3星通关主题曲3-8；必须编入非助战罗比菈塔并上场，且所有干员不被击倒</t>
+          <t>&gt; 由非助战假日威龙陈累计造成120000伤害&gt; 3星通关主题曲9-13标准实战环境；必须编入非助战假日威龙陈并上场，且使用假日威龙陈至少歼灭20个敌人</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="8" t="inlineStr">
         <is>
-          <t>桑葚</t>
+          <t>罗比菈塔</t>
         </is>
       </c>
       <c r="B214" s="8" t="inlineStr">
         <is>
-          <t>SV-5</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C214" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战桑葚并上场，且每次战斗至少释放1次安全区域&gt; 3星通关插曲SV-5；必须编入非助战桑葚并上场，其他成员仅可编入7名干员</t>
+          <t>&gt; 战斗中非助战罗比菈塔累计部署支援装置25个&gt; 3星通关主题曲3-8；必须编入非助战罗比菈塔并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="8" t="inlineStr">
         <is>
-          <t>琴柳</t>
+          <t>桑葚</t>
         </is>
       </c>
       <c r="B215" s="8" t="inlineStr">
         <is>
-          <t>9-2</t>
+          <t>SV-5</t>
         </is>
       </c>
       <c r="C215" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战琴柳累计使用信仰传承10次&gt; 3星通关主题曲9-2；必须编入非助战琴柳并上场，且不编入其他先锋干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战桑葚并上场，且每次战斗至少释放1次安全区域&gt; 3星通关插曲SV-5；必须编入非助战桑葚并上场，其他成员仅可编入7名干员</t>
         </is>
       </c>
     </row>
@@ -4453,46 +4453,46 @@
       </c>
       <c r="B216" s="8" t="inlineStr">
         <is>
-          <t>5-3</t>
+          <t>9-2</t>
         </is>
       </c>
       <c r="C216" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战琴柳并上场，且每次战斗至少释放1次光辉旗帜&gt; 3星通关主题曲5-3；必须编入非助战琴柳并上场，且至少使用3次光辉旗帜</t>
+          <t>&gt; 战斗中非助战琴柳累计使用信仰传承10次&gt; 3星通关主题曲9-2；必须编入非助战琴柳并上场，且不编入其他先锋干员</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="8" t="inlineStr">
         <is>
-          <t>灰毫</t>
+          <t>琴柳</t>
         </is>
       </c>
       <c r="B217" s="8" t="inlineStr">
         <is>
-          <t>7-9</t>
+          <t>5-3</t>
         </is>
       </c>
       <c r="C217" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战灰毫累计造成100000点伤害&gt; 3星通关主题曲7-9；必须编入非助战灰毫并上场，且使用灰毫歼灭至少2名游击队传令兵</t>
+          <t>&gt; 完成5次战斗；必须编入非助战琴柳并上场，且每次战斗至少释放1次光辉旗帜&gt; 3星通关主题曲5-3；必须编入非助战琴柳并上场，且至少使用3次光辉旗帜</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="8" t="inlineStr">
         <is>
-          <t>远牙</t>
+          <t>灰毫</t>
         </is>
       </c>
       <c r="B218" s="8" t="inlineStr">
         <is>
-          <t>S2-2</t>
+          <t>7-9</t>
         </is>
       </c>
       <c r="C218" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战远牙累计造成80歼灭数&gt; 3星通关主题曲S2-2；必须编入非助战远牙并上场，且远牙使用光羽箭至少歼灭8名敌人</t>
+          <t>&gt; 由非助战灰毫累计造成100000点伤害&gt; 3星通关主题曲7-9；必须编入非助战灰毫并上场，且使用灰毫歼灭至少2名游击队传令兵</t>
         </is>
       </c>
     </row>
@@ -4504,97 +4504,97 @@
       </c>
       <c r="B219" s="8" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>S2-2</t>
         </is>
       </c>
       <c r="C219" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战远牙并上场，且每次战斗至少释放2次光羽箭&gt; 3星通关主题曲2-5；必须编入非助战远牙并上场，且使用远牙歼灭至少2名高阶术师</t>
+          <t>&gt; 由非助战远牙累计造成80歼灭数&gt; 3星通关主题曲S2-2；必须编入非助战远牙并上场，且远牙使用光羽箭至少歼灭8名敌人</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="8" t="inlineStr">
         <is>
-          <t>布丁</t>
+          <t>远牙</t>
         </is>
       </c>
       <c r="B220" s="8" t="inlineStr">
         <is>
-          <t>2-10</t>
+          <t>2-5</t>
         </is>
       </c>
       <c r="C220" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战布丁累计造成150000点伤害&gt; 3星通关主题曲2-10；必须编入非助战布丁并上场，且布丁使用技能扩散电流至少歼灭2个重装防御者</t>
+          <t>&gt; 完成5次战斗；必须编入非助战远牙并上场，且每次战斗至少释放2次光羽箭&gt; 3星通关主题曲2-5；必须编入非助战远牙并上场，且使用远牙歼灭至少2名高阶术师</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="8" t="inlineStr">
         <is>
-          <t>蜜莓</t>
+          <t>布丁</t>
         </is>
       </c>
       <c r="B221" s="8" t="inlineStr">
         <is>
-          <t>GA-2</t>
+          <t>2-10</t>
         </is>
       </c>
       <c r="C221" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战蜜莓累计使用振奋8次&gt; 3星通关别传GA-2；必须编入非助战蜜莓并上场，且不编入其他医疗干员</t>
+          <t>&gt; 由非助战布丁累计造成150000点伤害&gt; 3星通关主题曲2-10；必须编入非助战布丁并上场，且布丁使用技能扩散电流至少歼灭2个重装防御者</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="8" t="inlineStr">
         <is>
-          <t>野鬃</t>
+          <t>蜜莓</t>
         </is>
       </c>
       <c r="B222" s="8" t="inlineStr">
         <is>
-          <t>MN-2</t>
+          <t>GA-2</t>
         </is>
       </c>
       <c r="C222" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战野鬃，并确定第一位部署的干员是野鬃&gt; 3星通关别传MN-2；必须编入非助战野鬃并上场，其他成员不可编入先锋干员</t>
+          <t>&gt; 战斗中非助战蜜莓累计使用振奋8次&gt; 3星通关别传GA-2；必须编入非助战蜜莓并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="8" t="inlineStr">
         <is>
-          <t>蚀清</t>
+          <t>野鬃</t>
         </is>
       </c>
       <c r="B223" s="8" t="inlineStr">
         <is>
-          <t>BI-6</t>
+          <t>MN-2</t>
         </is>
       </c>
       <c r="C223" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战蚀清累计造成100000点伤害&gt; 3星通关别传BI-6；必须编入非助战蚀清并上场，且至少使用2次传导蚀滞弹</t>
+          <t>&gt; 完成5次战斗；必须编入非助战野鬃，并确定第一位部署的干员是野鬃&gt; 3星通关别传MN-2；必须编入非助战野鬃并上场，其他成员不可编入先锋干员</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="8" t="inlineStr">
         <is>
-          <t>焰尾</t>
+          <t>蚀清</t>
         </is>
       </c>
       <c r="B224" s="8" t="inlineStr">
         <is>
-          <t>NL-5</t>
+          <t>BI-6</t>
         </is>
       </c>
       <c r="C224" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战焰尾并上场，且每次战斗至少释放2次焰心&gt; 3星通关别传NL-5；必须编入非助战焰尾，且第一位部署焰尾、焰尾全程不撤退或被击倒</t>
+          <t>&gt; 由非助战蚀清累计造成100000点伤害&gt; 3星通关别传BI-6；必须编入非助战蚀清并上场，且至少使用2次传导蚀滞弹</t>
         </is>
       </c>
     </row>
@@ -4606,29 +4606,29 @@
       </c>
       <c r="B225" s="8" t="inlineStr">
         <is>
-          <t>NL-3</t>
+          <t>NL-5</t>
         </is>
       </c>
       <c r="C225" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战焰尾累计造成40000点伤害&gt; 3星通关别传NL-3；必须编入非助战焰尾并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战焰尾并上场，且每次战斗至少释放2次焰心&gt; 3星通关别传NL-5；必须编入非助战焰尾，且第一位部署焰尾、焰尾全程不撤退或被击倒</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="8" t="inlineStr">
         <is>
-          <t>耀骑士临光</t>
+          <t>焰尾</t>
         </is>
       </c>
       <c r="B226" s="8" t="inlineStr">
         <is>
-          <t>MN-8</t>
+          <t>NL-3</t>
         </is>
       </c>
       <c r="C226" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战耀骑士临光累计造成100歼灭数&gt; 3星通关别传MN-8；必须编入非助战耀骑士临光并上场，且使用耀骑士临光歼灭至少1个腐败骑士或凋零骑士</t>
+          <t>&gt; 由非助战焰尾累计造成40000点伤害&gt; 3星通关别传NL-3；必须编入非助战焰尾并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
@@ -4640,63 +4640,63 @@
       </c>
       <c r="B227" s="8" t="inlineStr">
         <is>
-          <t>NL-10</t>
+          <t>MN-8</t>
         </is>
       </c>
       <c r="C227" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战耀骑士临光并上场，且每次战斗至少释放1次耀阳颔首&gt; 3星通关别传NL-10；必须编入非助战耀骑士临光并上场，且使用耀骑士临光击败血骑士狄开俄波利斯</t>
+          <t>&gt; 由非助战耀骑士临光累计造成100歼灭数&gt; 3星通关别传MN-8；必须编入非助战耀骑士临光并上场，且使用耀骑士临光歼灭至少1个腐败骑士或凋零骑士</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="8" t="inlineStr">
         <is>
-          <t>耶拉</t>
+          <t>耀骑士临光</t>
         </is>
       </c>
       <c r="B228" s="8" t="inlineStr">
         <is>
-          <t>BI-7</t>
+          <t>NL-10</t>
         </is>
       </c>
       <c r="C228" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战耶拉累计造成80000点伤害&gt; 3星通关别传BI-7；必须编入非助战耶拉并上场，且至少使用2次心随意动</t>
+          <t>&gt; 完成5次战斗；必须编入非助战耀骑士临光并上场，且每次战斗至少释放1次耀阳颔首&gt; 3星通关别传NL-10；必须编入非助战耀骑士临光并上场，且使用耀骑士临光击败血骑士狄开俄波利斯</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="8" t="inlineStr">
         <is>
-          <t>极光</t>
+          <t>耶拉</t>
         </is>
       </c>
       <c r="B229" s="8" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>BI-7</t>
         </is>
       </c>
       <c r="C229" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战极光累计造成40000点伤害&gt; 3星通关主题曲3-8；必须编入非助战极光并上场，且使用极光歼灭碎骨</t>
+          <t>&gt; 由非助战耶拉累计造成80000点伤害&gt; 3星通关别传BI-7；必须编入非助战耶拉并上场，且至少使用2次心随意动</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="8" t="inlineStr">
         <is>
-          <t>灵知</t>
+          <t>极光</t>
         </is>
       </c>
       <c r="B230" s="8" t="inlineStr">
         <is>
-          <t>BI-7</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C230" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战灵知并上场，且每次战斗至少释放1次失温症&gt; 3星通关别传BI-7，必须编入非助战灵知并上场，且不编入其他辅助干员</t>
+          <t>&gt; 由非助战极光累计造成40000点伤害&gt; 3星通关主题曲3-8；必须编入非助战极光并上场，且使用极光歼灭碎骨</t>
         </is>
       </c>
     </row>
@@ -4708,70 +4708,70 @@
       </c>
       <c r="B231" s="8" t="inlineStr">
         <is>
-          <t>5-6</t>
+          <t>BI-7</t>
         </is>
       </c>
       <c r="C231" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战灵知累计使用10次失温症&gt; 3星通关主题曲5-6；必须编入非助战灵知并上场，且使用灵知击败至少5个法术大师A1</t>
+          <t>&gt; 完成5次战斗；必须编入非助战灵知并上场，且每次战斗至少释放1次失温症&gt; 3星通关别传BI-7，必须编入非助战灵知并上场，且不编入其他辅助干员</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="8" t="inlineStr">
         <is>
-          <t>九色鹿</t>
+          <t>灵知</t>
         </is>
       </c>
       <c r="B232" s="8" t="inlineStr">
         <is>
-          <t>IW-3</t>
+          <t>5-6</t>
         </is>
       </c>
       <c r="C232" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战九色鹿累计使用仙山去远8次&gt; 3星通关别传IW-3；必须编入非助战九色鹿并上场，且不编入其他辅助干员</t>
+          <t>&gt; 战斗中非助战灵知累计使用10次失温症&gt; 3星通关主题曲5-6；必须编入非助战灵知并上场，且使用灵知击败至少5个法术大师A1</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="8" t="inlineStr">
         <is>
-          <t>寒芒克洛丝</t>
+          <t>九色鹿</t>
         </is>
       </c>
       <c r="B233" s="8" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>IW-3</t>
         </is>
       </c>
       <c r="C233" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战寒芒克洛丝累计使用封喉5次&gt; 3星通关主题曲3-8；必须编入非助战寒芒克洛丝并上场，且使用寒芒克洛丝歼灭碎骨</t>
+          <t>&gt; 战斗中非助战九色鹿累计使用仙山去远8次&gt; 3星通关别传IW-3；必须编入非助战九色鹿并上场，且不编入其他辅助干员</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="8" t="inlineStr">
         <is>
-          <t>夜半</t>
+          <t>寒芒克洛丝</t>
         </is>
       </c>
       <c r="B234" s="8" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C234" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战夜半累计使用安眠10次&gt; 3星通关主题曲3-1；必须编入非助战夜半并上场，且至少使用3次安眠</t>
+          <t>&gt; 战斗中非助战寒芒克洛丝累计使用封喉5次&gt; 3星通关主题曲3-8；必须编入非助战寒芒克洛丝并上场，且使用寒芒克洛丝歼灭碎骨</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="8" t="inlineStr">
         <is>
-          <t>老鲤</t>
+          <t>夜半</t>
         </is>
       </c>
       <c r="B235" s="8" t="inlineStr">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="C235" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战老鲤累计造成80歼灭数&gt; 3星通关主题曲3-1；必须编入非助战老鲤并上场，其他成员仅可编入狙击、先锋与医疗干员</t>
+          <t>&gt; 战斗中非助战夜半累计使用安眠10次&gt; 3星通关主题曲3-1；必须编入非助战夜半并上场，且至少使用3次安眠</t>
         </is>
       </c>
     </row>
@@ -4793,114 +4793,114 @@
       </c>
       <c r="B236" s="8" t="inlineStr">
         <is>
-          <t>IW-EX-1</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="C236" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战老鲤并上场，且每次战斗至少释放1次贵客盈门&gt; 3星通关别传IW-EX-1；必须编入非助战老鲤并上场，且使用老鲤至少歼灭10个敌人</t>
+          <t>&gt; 由非助战老鲤累计造成80歼灭数&gt; 3星通关主题曲3-1；必须编入非助战老鲤并上场，其他成员仅可编入狙击、先锋与医疗干员</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="8" t="inlineStr">
         <is>
-          <t>令</t>
+          <t>老鲤</t>
         </is>
       </c>
       <c r="B237" s="8" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>IW-EX-1</t>
         </is>
       </c>
       <c r="C237" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战令并上场，且使用令与令的召唤物歼灭至少7名敌人&gt; 3星通关主题曲3-4；必须编入非助战令并上场，且整场战斗仅部署过令与至多4位其他干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战老鲤并上场，且每次战斗至少释放1次贵客盈门&gt; 3星通关别传IW-EX-1；必须编入非助战老鲤并上场，且使用老鲤至少歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="8" t="inlineStr">
         <is>
-          <t>夏栎</t>
+          <t>令</t>
         </is>
       </c>
       <c r="B238" s="8" t="inlineStr">
         <is>
-          <t>9-2</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="C238" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战夏栎累计使用生灵的回响8次&gt; 3星通关主题曲9-2标准实战环境；必须编入非助战夏栎并上场，且不编入其他医疗干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战令并上场，且使用令与令的召唤物歼灭至少7名敌人&gt; 3星通关主题曲3-4；必须编入非助战令并上场，且整场战斗仅部署过令与至多4位其他干员</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="8" t="inlineStr">
         <is>
-          <t>澄闪</t>
+          <t>夏栎</t>
         </is>
       </c>
       <c r="B239" s="8" t="inlineStr">
         <is>
-          <t>R8-8</t>
+          <t>9-2</t>
         </is>
       </c>
       <c r="C239" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战澄闪累计造成100000点伤害&gt; 3星通关主题曲R8-8；必须编入非助战澄闪并上场，且使用澄闪歼灭至少2名帝国炮火先兆者</t>
+          <t>&gt; 战斗中非助战夏栎累计使用生灵的回响8次&gt; 3星通关主题曲9-2标准实战环境；必须编入非助战夏栎并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="8" t="inlineStr">
         <is>
-          <t>见行者</t>
+          <t>澄闪</t>
         </is>
       </c>
       <c r="B240" s="8" t="inlineStr">
         <is>
-          <t>GA-EX-1</t>
+          <t>R8-8</t>
         </is>
       </c>
       <c r="C240" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战见行者并上场，且每次战斗至少释放2次惊爆射击&gt; 3星通关别传GA-EX-1；必须编入非助战见行者，且本场战斗至少使3个寻路者精锐狙击手坠落地穴</t>
+          <t>&gt; 由非助战澄闪累计造成100000点伤害&gt; 3星通关主题曲R8-8；必须编入非助战澄闪并上场，且使用澄闪歼灭至少2名帝国炮火先兆者</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="8" t="inlineStr">
         <is>
-          <t>风丸</t>
+          <t>见行者</t>
         </is>
       </c>
       <c r="B241" s="8" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>GA-EX-1</t>
         </is>
       </c>
       <c r="C241" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战风丸累计使用纸艺·双影10次&gt; 3星通关主题曲3-1；必须编入非助战风丸并上场，且使用风丸歼灭至少30名敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战见行者并上场，且每次战斗至少释放2次惊爆射击&gt; 3星通关别传GA-EX-1；必须编入非助战见行者，且本场战斗至少使3个寻路者精锐狙击手坠落地穴</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="8" t="inlineStr">
         <is>
-          <t>菲亚梅塔</t>
+          <t>风丸</t>
         </is>
       </c>
       <c r="B242" s="8" t="inlineStr">
         <is>
-          <t>GA-4</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="C242" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战菲亚梅塔并上场，且使用菲亚梅塔歼灭至少10个敌人&gt; 3星通关别传GA-4；必须编入非助战菲亚梅塔并上场，且队伍中不能有其他狙击干员</t>
+          <t>&gt; 由非助战风丸累计使用纸艺·双影10次&gt; 3星通关主题曲3-1；必须编入非助战风丸并上场，且使用风丸歼灭至少30名敌人</t>
         </is>
       </c>
     </row>
@@ -4912,80 +4912,80 @@
       </c>
       <c r="B243" s="8" t="inlineStr">
         <is>
-          <t>S5-9</t>
+          <t>GA-4</t>
         </is>
       </c>
       <c r="C243" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战菲亚梅塔累计造成180000点伤害&gt; 3星通关主题曲S5-9；必须编入非助战菲亚梅塔并上场，且使用菲亚梅塔造成至少60000点伤害</t>
+          <t>&gt; 完成5次战斗；必须编入非助战菲亚梅塔并上场，且使用菲亚梅塔歼灭至少10个敌人&gt; 3星通关别传GA-4；必须编入非助战菲亚梅塔并上场，且队伍中不能有其他狙击干员</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="8" t="inlineStr">
         <is>
-          <t>褐果</t>
+          <t>菲亚梅塔</t>
         </is>
       </c>
       <c r="B244" s="8" t="inlineStr">
         <is>
-          <t>SV-3</t>
+          <t>S5-9</t>
         </is>
       </c>
       <c r="C244" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战褐果并上场，且每次战斗至少释放1次厚土迸发&gt; 3星通关插曲SV-3；必须编入非助战褐果并上场，且不编入其他医疗干员</t>
+          <t>&gt; 由非助战菲亚梅塔累计造成180000点伤害&gt; 3星通关主题曲S5-9；必须编入非助战菲亚梅塔并上场，且使用菲亚梅塔造成至少60000点伤害</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="8" t="inlineStr">
         <is>
-          <t>海蒂</t>
+          <t>褐果</t>
         </is>
       </c>
       <c r="B245" s="8" t="inlineStr">
         <is>
-          <t>9-7</t>
+          <t>SV-3</t>
         </is>
       </c>
       <c r="C245" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战海蒂累计使用8次“虚构故事·怒士”&gt; 3星通关主题曲9-7标准实战环境；必须编入非助战海蒂并上场，且海蒂使用至少3次“虚构故事·锈城”</t>
+          <t>&gt; 完成5次战斗；必须编入非助战褐果并上场，且每次战斗至少释放1次厚土迸发&gt; 3星通关插曲SV-3；必须编入非助战褐果并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="8" t="inlineStr">
         <is>
-          <t>洛洛</t>
+          <t>海蒂</t>
         </is>
       </c>
       <c r="B246" s="8" t="inlineStr">
         <is>
-          <t>RI-EX-4</t>
+          <t>9-7</t>
         </is>
       </c>
       <c r="C246" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战洛洛累计使用自负此轭10次&gt; 3星通关别传RI-EX-4；必须编入非助战洛洛并上场，且使用洛洛歼灭至少2名提亚卡乌冠军</t>
+          <t>&gt; 战斗中非助战海蒂累计使用8次“虚构故事·怒士”&gt; 3星通关主题曲9-7标准实战环境；必须编入非助战海蒂并上场，且海蒂使用至少3次“虚构故事·锈城”</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="8" t="inlineStr">
         <is>
-          <t>号角</t>
+          <t>洛洛</t>
         </is>
       </c>
       <c r="B247" s="8" t="inlineStr">
         <is>
-          <t>7-15</t>
+          <t>RI-EX-4</t>
         </is>
       </c>
       <c r="C247" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战号角累计使用终极防线10次&gt; 3星通关主题曲7-15；必须编入非助战号角并上场，且使用号角至少歼灭10个敌人</t>
+          <t>&gt; 战斗中非助战洛洛累计使用自负此轭10次&gt; 3星通关别传RI-EX-4；必须编入非助战洛洛并上场，且使用洛洛歼灭至少2名提亚卡乌冠军</t>
         </is>
       </c>
     </row>
@@ -4997,46 +4997,46 @@
       </c>
       <c r="B248" s="8" t="inlineStr">
         <is>
-          <t>9-5</t>
+          <t>7-15</t>
         </is>
       </c>
       <c r="C248" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战号角累计造成100000点伤害&gt; 3星通关主题曲9-5标准实战环境；必须编入非助战号角并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 战斗中非助战号角累计使用终极防线10次&gt; 3星通关主题曲7-15；必须编入非助战号角并上场，且使用号角至少歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="8" t="inlineStr">
         <is>
-          <t>掠风</t>
+          <t>号角</t>
         </is>
       </c>
       <c r="B249" s="8" t="inlineStr">
         <is>
-          <t>11-9</t>
+          <t>9-5</t>
         </is>
       </c>
       <c r="C249" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战掠风累计使用此身为源10次&gt; 3星通关主题曲11-9标准实战环境；必须编入非助战掠风并上场，其他成员仅可编入术师、重装与医疗干员</t>
+          <t>&gt; 由非助战号角累计造成100000点伤害&gt; 3星通关主题曲9-5标准实战环境；必须编入非助战号角并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="8" t="inlineStr">
         <is>
-          <t>流明</t>
+          <t>掠风</t>
         </is>
       </c>
       <c r="B250" s="8" t="inlineStr">
         <is>
-          <t>6-9</t>
+          <t>11-9</t>
         </is>
       </c>
       <c r="C250" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战流明并上场，且每次战斗至少释放2次灯火不灭&gt; 3星通关主题曲6-9；且仅可编入非助战流明1名医疗干员并上场</t>
+          <t>&gt; 战斗中非助战掠风累计使用此身为源10次&gt; 3星通关主题曲11-9标准实战环境；必须编入非助战掠风并上场，其他成员仅可编入术师、重装与医疗干员</t>
         </is>
       </c>
     </row>
@@ -5048,29 +5048,29 @@
       </c>
       <c r="B251" s="8" t="inlineStr">
         <is>
-          <t>OF-5</t>
+          <t>6-9</t>
         </is>
       </c>
       <c r="C251" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战流明累计使用沛霖10次&gt; 3星通关别传OF-5；必须编入非助战流明并上场，且不编入其他医疗干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战流明并上场，且每次战斗至少释放2次灯火不灭&gt; 3星通关主题曲6-9；且仅可编入非助战流明1名医疗干员并上场</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="8" t="inlineStr">
         <is>
-          <t>艾丽妮</t>
+          <t>流明</t>
         </is>
       </c>
       <c r="B252" s="8" t="inlineStr">
         <is>
-          <t>SV-EX-1</t>
+          <t>OF-5</t>
         </is>
       </c>
       <c r="C252" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战艾丽妮累计造成100000点伤害&gt; 3星通关插曲SV-EX-1；必须编入非助战艾丽妮并上场，且使用2次判决</t>
+          <t>&gt; 战斗中非助战流明累计使用沛霖10次&gt; 3星通关别传OF-5；必须编入非助战流明并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
@@ -5082,29 +5082,29 @@
       </c>
       <c r="B253" s="8" t="inlineStr">
         <is>
-          <t>SV-4</t>
+          <t>SV-EX-1</t>
         </is>
       </c>
       <c r="C253" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战艾丽妮使用技能累计造成50歼灭数&gt; 3星通关插曲SV-4；必须编入非助战艾丽妮并上场，且使用艾丽妮歼灭15个敌人</t>
+          <t>&gt; 由非助战艾丽妮累计造成100000点伤害&gt; 3星通关插曲SV-EX-1；必须编入非助战艾丽妮并上场，且使用2次判决</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="8" t="inlineStr">
         <is>
-          <t>归溟幽灵鲨</t>
+          <t>艾丽妮</t>
         </is>
       </c>
       <c r="B254" s="8" t="inlineStr">
         <is>
-          <t>SV-EX-1</t>
+          <t>SV-4</t>
         </is>
       </c>
       <c r="C254" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战归溟幽灵鲨累计造成30歼灭数&gt; 3星通关插曲SV-EX-1；必须编入非助战归溟幽灵鲨并上场，且使用归溟幽灵鲨歼灭至少1个囊海爬行者</t>
+          <t>&gt; 由非助战艾丽妮使用技能累计造成50歼灭数&gt; 3星通关插曲SV-4；必须编入非助战艾丽妮并上场，且使用艾丽妮歼灭15个敌人</t>
         </is>
       </c>
     </row>
@@ -5116,63 +5116,63 @@
       </c>
       <c r="B255" s="8" t="inlineStr">
         <is>
-          <t>S4-1</t>
+          <t>SV-EX-1</t>
         </is>
       </c>
       <c r="C255" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战归溟幽灵鲨并上场，且每次战斗至少释放1次生存的重压&gt; 3星通关主题曲S4-1；必须编入非助战归溟幽灵鲨并上场，且使用归溟幽灵鲨歼灭10个敌人</t>
+          <t>&gt; 由非助战归溟幽灵鲨累计造成30歼灭数&gt; 3星通关插曲SV-EX-1；必须编入非助战归溟幽灵鲨并上场，且使用归溟幽灵鲨歼灭至少1个囊海爬行者</t>
         </is>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="8" t="inlineStr">
         <is>
-          <t>埃拉托</t>
+          <t>归溟幽灵鲨</t>
         </is>
       </c>
       <c r="B256" s="8" t="inlineStr">
         <is>
-          <t>S5-9</t>
+          <t>S4-1</t>
         </is>
       </c>
       <c r="C256" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战埃拉托累计使用英雄赞歌5次&gt; 3星通关主题曲S5-9；必须编入非助战埃拉托并上场，其他成员不可编入狙击干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战归溟幽灵鲨并上场，且每次战斗至少释放1次生存的重压&gt; 3星通关主题曲S4-1；必须编入非助战归溟幽灵鲨并上场，且使用归溟幽灵鲨歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="8" t="inlineStr">
         <is>
-          <t>濯尘芙蓉</t>
+          <t>埃拉托</t>
         </is>
       </c>
       <c r="B257" s="8" t="inlineStr">
         <is>
-          <t>LE-4</t>
+          <t>S5-9</t>
         </is>
       </c>
       <c r="C257" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战濯尘芙蓉累计使用抚业之触10次&gt; 3星通关别传LE-4；必须编入非助战濯尘芙蓉并上场，且至少使用2次抚业之触</t>
+          <t>&gt; 战斗中非助战埃拉托累计使用英雄赞歌5次&gt; 3星通关主题曲S5-9；必须编入非助战埃拉托并上场，其他成员不可编入狙击干员</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="8" t="inlineStr">
         <is>
-          <t>黑键</t>
+          <t>濯尘芙蓉</t>
         </is>
       </c>
       <c r="B258" s="8" t="inlineStr">
         <is>
-          <t>3-7</t>
+          <t>LE-4</t>
         </is>
       </c>
       <c r="C258" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战黑键累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲3-7；必须编入非助战黑键并上场，且使用黑键歼灭至少1个重装防御组长</t>
+          <t>&gt; 战斗中非助战濯尘芙蓉累计使用抚业之触10次&gt; 3星通关别传LE-4；必须编入非助战濯尘芙蓉并上场，且至少使用2次抚业之触</t>
         </is>
       </c>
     </row>
@@ -5184,12 +5184,12 @@
       </c>
       <c r="B259" s="8" t="inlineStr">
         <is>
-          <t>3-6</t>
+          <t>3-7</t>
         </is>
       </c>
       <c r="C259" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战黑键并上场，且使用黑键歼灭至少6个敌人&gt; 3星通关主题曲3-6；必须编入非助战黑键并上场，且使用黑键歼灭屠宰老手</t>
+          <t>&gt; 由非助战黑键累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲3-7；必须编入非助战黑键并上场，且使用黑键歼灭至少1个重装防御组长</t>
         </is>
       </c>
     </row>
@@ -5201,835 +5201,835 @@
       </c>
       <c r="B260" s="8" t="inlineStr">
         <is>
-          <t>11-12</t>
+          <t>3-6</t>
         </is>
       </c>
       <c r="C260" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战黑键累计使用寂静之声10次&gt; 3星通关主题曲11-12标准实战环境；必须编入非助战黑键并上场，且使用黑键歼灭至少2名伦蒂尼姆城防自行炮</t>
+          <t>&gt; 完成5次战斗；必须编入非助战黑键并上场，且使用黑键歼灭至少6个敌人&gt; 3星通关主题曲3-6；必须编入非助战黑键并上场，且使用黑键歼灭屠宰老手</t>
         </is>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="8" t="inlineStr">
         <is>
-          <t>星源</t>
+          <t>黑键</t>
         </is>
       </c>
       <c r="B261" s="8" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>11-12</t>
         </is>
       </c>
       <c r="C261" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战星源累计造成40歼灭数&gt; 3星通关主题曲4-3；必须编入非助战星源并上场，其他成员仅可编入重装干员</t>
+          <t>&gt; 战斗中非助战黑键累计使用寂静之声10次&gt; 3星通关主题曲11-12标准实战环境；必须编入非助战黑键并上场，且使用黑键歼灭至少2名伦蒂尼姆城防自行炮</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="8" t="inlineStr">
         <is>
-          <t>承曦格雷伊</t>
+          <t>星源</t>
         </is>
       </c>
       <c r="B262" s="8" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C262" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战承曦格雷伊累计使用晨曦信标10次&gt; 3星通关主题曲1-3；必须编入非助战承曦格雷伊并上场，其他成员仅可编入先锋干员</t>
+          <t>&gt; 由非助战星源累计造成40歼灭数&gt; 3星通关主题曲4-3；必须编入非助战星源并上场，其他成员仅可编入重装干员</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="8" t="inlineStr">
         <is>
-          <t>多萝西</t>
+          <t>承曦格雷伊</t>
         </is>
       </c>
       <c r="B263" s="8" t="inlineStr">
         <is>
-          <t>4-5</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="C263" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战多萝西累计部署共振装置50个&gt; 3星通关主题曲4-5；必须编入非助战多萝西并上场，其他成员仅可编入3名干员</t>
+          <t>&gt; 战斗中非助战承曦格雷伊累计使用晨曦信标10次&gt; 3星通关主题曲1-3；必须编入非助战承曦格雷伊并上场，其他成员仅可编入先锋干员</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="8" t="inlineStr">
         <is>
-          <t>至简</t>
+          <t>多萝西</t>
         </is>
       </c>
       <c r="B264" s="8" t="inlineStr">
         <is>
-          <t>IC-8</t>
+          <t>MB-EX-1</t>
         </is>
       </c>
       <c r="C264" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战至简累计使用神工意匠20次&gt; 3星通关别传IC-8；必须编入非助战至简并上场，且使用至简歼灭至少2名蜜酿级醒酒助手</t>
+          <t>&gt; 由非助战多萝西累计造成120000点伤害&gt; 3星通关插曲MB-EX-1，必须编入非助战多萝西并上场，其他成员仅可编入近卫干员</t>
         </is>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="8" t="inlineStr">
         <is>
-          <t>晓歌</t>
+          <t>多萝西</t>
         </is>
       </c>
       <c r="B265" s="8" t="inlineStr">
         <is>
-          <t>5-3</t>
+          <t>4-5</t>
         </is>
       </c>
       <c r="C265" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中累计部署非助战晓歌12次&gt; 3星通关主题曲5-3；必须编入非助战晓歌并上场，且使用晓歌歼灭至少3个特战术师或特战术师组长</t>
+          <t>&gt; 战斗中非助战多萝西累计部署共振装置50个&gt; 3星通关主题曲4-5；必须编入非助战多萝西并上场，其他成员仅可编入3名干员</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="8" t="inlineStr">
         <is>
-          <t>鸿雪</t>
+          <t>至简</t>
         </is>
       </c>
       <c r="B266" s="8" t="inlineStr">
         <is>
-          <t>9-7</t>
+          <t>IC-8</t>
         </is>
       </c>
       <c r="C266" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战鸿雪并上场，且每次战斗至少释放1次锐笔速写&gt; 3星通关主题曲9-7标准实战环境，必须编入非助战鸿雪并上场，且使用鸿雪歼灭至少10名敌人，其中包括至少1个深池重甲卫士</t>
+          <t>&gt; 战斗中非助战至简累计使用神工意匠20次&gt; 3星通关别传IC-8；必须编入非助战至简并上场，且使用至简歼灭至少2名蜜酿级醒酒助手</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="8" t="inlineStr">
         <is>
-          <t>鸿雪</t>
+          <t>晓歌</t>
         </is>
       </c>
       <c r="B267" s="8" t="inlineStr">
         <is>
-          <t>2-10</t>
+          <t>5-3</t>
         </is>
       </c>
       <c r="C267" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中累计部署非助战鸿雪的“打字机”10次&gt; 3星通关主题曲2-10；必须编入非助战鸿雪并上场，且使用鸿雪或“打字机”歼灭碎骨</t>
+          <t>&gt; 战斗中累计部署非助战晓歌12次&gt; 3星通关主题曲5-3；必须编入非助战晓歌并上场，且使用晓歌歼灭至少3个特战术师或特战术师组长</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="8" t="inlineStr">
         <is>
-          <t>百炼嘉维尔</t>
+          <t>鸿雪</t>
         </is>
       </c>
       <c r="B268" s="8" t="inlineStr">
         <is>
-          <t>9-2</t>
+          <t>9-7</t>
         </is>
       </c>
       <c r="C268" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战百炼嘉维尔累计使用链锯强袭10次&gt; 3星通关主题曲9-2标准实战环境；必须编入非助战百炼嘉维尔并上场，且使用百炼嘉维尔至少歼灭15个敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战鸿雪并上场，且每次战斗至少释放1次锐笔速写&gt; 3星通关主题曲9-7标准实战环境，必须编入非助战鸿雪并上场，且使用鸿雪歼灭至少10名敌人，其中包括至少1个深池重甲卫士</t>
         </is>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="8" t="inlineStr">
         <is>
-          <t>但书</t>
+          <t>鸿雪</t>
         </is>
       </c>
       <c r="B269" s="8" t="inlineStr">
         <is>
-          <t>4-7</t>
+          <t>2-10</t>
         </is>
       </c>
       <c r="C269" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战但书累计使用致胜立论14次&gt; 3星通关主题曲4-7；必须编入非助战但书并上场，且使用但书至少歼灭3只高能源石虫</t>
+          <t>&gt; 战斗中累计部署非助战鸿雪的“打字机”10次&gt; 3星通关主题曲2-10；必须编入非助战鸿雪并上场，且使用鸿雪或“打字机”歼灭碎骨</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="8" t="inlineStr">
         <is>
-          <t>玛恩纳</t>
+          <t>百炼嘉维尔</t>
         </is>
       </c>
       <c r="B270" s="8" t="inlineStr">
         <is>
-          <t>11-15</t>
+          <t>9-2</t>
         </is>
       </c>
       <c r="C270" s="6" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战玛恩纳累计造成120000点伤害&gt; 3星通关主题曲11-15标准实战环境；必须编入非助战玛恩纳并上场，且使用2次未照耀的荣光</t>
+          <t>&gt; 战斗中非助战百炼嘉维尔累计使用链锯强袭10次&gt; 3星通关主题曲9-2标准实战环境；必须编入非助战百炼嘉维尔并上场，且使用百炼嘉维尔至少歼灭15个敌人</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="8" t="inlineStr">
         <is>
-          <t>罗小黑</t>
+          <t>但书</t>
         </is>
       </c>
       <c r="B271" s="8" t="inlineStr">
         <is>
-          <t>IW-4</t>
+          <t>4-7</t>
         </is>
       </c>
       <c r="C271" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战罗小黑并上场，且每次战斗至少释放1次碎金为刃&gt; 3星通关别传IW-4；必须编入非助战罗小黑并上场，其他成员仅可编入6名干员</t>
+          <t>&gt; 战斗中非助战但书累计使用致胜立论14次&gt; 3星通关主题曲4-7；必须编入非助战但书并上场，且使用但书至少歼灭3只高能源石虫</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="8" t="inlineStr">
         <is>
-          <t>海沫</t>
+          <t>玛恩纳</t>
         </is>
       </c>
       <c r="B272" s="8" t="inlineStr">
         <is>
-          <t>SN-2</t>
+          <t>11-15</t>
         </is>
       </c>
       <c r="C272" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战海沫并上场，且使用海沫造成至少12000点伤害&gt; 3星通关插曲SN-2；必须携带并部署非助战海沫，其他成员仅可编入2名干员</t>
+          <t>&gt; 使用非助战玛恩纳累计造成120000点伤害&gt; 3星通关主题曲11-15标准实战环境；必须编入非助战玛恩纳并上场，且使用2次未照耀的荣光</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="8" t="inlineStr">
         <is>
-          <t>铅踝</t>
+          <t>罗小黑</t>
         </is>
       </c>
       <c r="B273" s="8" t="inlineStr">
         <is>
-          <t>S3-5</t>
+          <t>IW-4</t>
         </is>
       </c>
       <c r="C273" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战铅踝累计造成30歼灭数&gt; 3星通关主题曲S3-5；必须编入非助战铅踝并上场，且使用铅踝歼灭至少2个隐形弩手</t>
+          <t>&gt; 完成5次战斗；必须编入非助战罗小黑并上场，且每次战斗至少释放1次碎金为刃&gt; 3星通关别传IW-4；必须编入非助战罗小黑并上场，其他成员仅可编入6名干员</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="8" t="inlineStr">
         <is>
-          <t>达格达</t>
+          <t>海沫</t>
         </is>
       </c>
       <c r="B274" s="8" t="inlineStr">
         <is>
-          <t>11-5</t>
+          <t>SN-2</t>
         </is>
       </c>
       <c r="C274" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战达格达累计造成30歼灭数&gt; 3星通关主题曲11-5标准实战环境；必须编入非助战达格达并上场，且使用达格达至少歼灭10个敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战海沫并上场，且使用海沫造成至少12000点伤害&gt; 3星通关插曲SN-2；必须携带并部署非助战海沫，其他成员仅可编入2名干员</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="8" t="inlineStr">
         <is>
-          <t>白铁</t>
+          <t>铅踝</t>
         </is>
       </c>
       <c r="B275" s="8" t="inlineStr">
         <is>
-          <t>11-6</t>
+          <t>S3-5</t>
         </is>
       </c>
       <c r="C275" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战白铁累计部署支援装置25个&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战白铁并上场，且使用白铁或白铁的支援装置歼灭至少15名萨卡兹枯朽战士</t>
+          <t>&gt; 由非助战铅踝累计造成30歼灭数&gt; 3星通关主题曲S3-5；必须编入非助战铅踝并上场，且使用铅踝歼灭至少2个隐形弩手</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="8" t="inlineStr">
         <is>
-          <t>白铁</t>
+          <t>达格达</t>
         </is>
       </c>
       <c r="B276" s="8" t="inlineStr">
         <is>
-          <t>9-6</t>
+          <t>11-5</t>
         </is>
       </c>
       <c r="C276" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战白铁累计使用8次“铁钳号·原型机”&gt; 3星通关主题曲9-6标准实战环境；必须编入非助战白铁并上场，且使用白铁至少歼灭10个敌人</t>
+          <t>&gt; 由非助战达格达累计造成30歼灭数&gt; 3星通关主题曲11-5标准实战环境；必须编入非助战达格达并上场，且使用达格达至少歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="8" t="inlineStr">
         <is>
-          <t>石英</t>
+          <t>白铁</t>
         </is>
       </c>
       <c r="B277" s="8" t="inlineStr">
         <is>
-          <t>DH-4</t>
+          <t>11-6</t>
         </is>
       </c>
       <c r="C277" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成3次战斗；必须编入非助战石英并上场，且每次战斗至少释放1次全力相搏&gt; 3星通关别传DH-4；必须编入非助战石英并上场，并使用石英至少击败2名控潮术师</t>
+          <t>&gt; 战斗中非助战白铁累计部署支援装置25个&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战白铁并上场，且使用白铁或白铁的支援装置歼灭至少15名萨卡兹枯朽战士</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="8" t="inlineStr">
         <is>
-          <t>雪绒</t>
+          <t>白铁</t>
         </is>
       </c>
       <c r="B278" s="8" t="inlineStr">
         <is>
-          <t>2-3</t>
+          <t>9-6</t>
         </is>
       </c>
       <c r="C278" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战雪绒累计使用坠雪10次&gt; 3星通关主题曲2-3；必须编入非助战雪绒并上场，且使用雪绒歼灭至少2名重装防御者</t>
+          <t>&gt; 战斗中非助战白铁累计使用8次“铁钳号·原型机”&gt; 3星通关主题曲9-6标准实战环境；必须编入非助战白铁并上场，且使用白铁至少歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="8" t="inlineStr">
         <is>
-          <t>子月</t>
+          <t>石英</t>
         </is>
       </c>
       <c r="B279" s="8" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>DH-4</t>
         </is>
       </c>
       <c r="C279" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战子月累计造成30歼灭数&gt; 3星通关主题曲2-5；必须编入非助战子月并上场，且使用子月歼灭至少2个高阶术师</t>
+          <t>&gt; 完成3次战斗；必须编入非助战石英并上场，且每次战斗至少释放1次全力相搏&gt; 3星通关别传DH-4；必须编入非助战石英并上场，并使用石英至少击败2名控潮术师</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="8" t="inlineStr">
         <is>
-          <t>伺夜</t>
+          <t>雪绒</t>
         </is>
       </c>
       <c r="B280" s="8" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="C280" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战伺夜并上场，且每次战斗至少释放1次领袖的尊严&gt; 3星通关主题曲3-8；必须编入非助战伺夜并上场，且使用伺夜歼灭碎骨</t>
+          <t>&gt; 战斗中非助战雪绒累计使用坠雪10次&gt; 3星通关主题曲2-3；必须编入非助战雪绒并上场，且使用雪绒歼灭至少2名重装防御者</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="8" t="inlineStr">
         <is>
-          <t>伺夜</t>
+          <t>子月</t>
         </is>
       </c>
       <c r="B281" s="8" t="inlineStr">
         <is>
-          <t>IS-6</t>
+          <t>2-5</t>
         </is>
       </c>
       <c r="C281" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战伺夜，并确定第一位部署的干员是伺夜&gt; 3星通关别传IS-6；必须编入非助战伺夜并上场，且至少使用3次领袖的尊严</t>
+          <t>&gt; 由非助战子月累计造成30歼灭数&gt; 3星通关主题曲2-5；必须编入非助战子月并上场，且使用子月歼灭至少2个高阶术师</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="8" t="inlineStr">
         <is>
-          <t>斥罪</t>
+          <t>伺夜</t>
         </is>
       </c>
       <c r="B282" s="8" t="inlineStr">
         <is>
-          <t>CB-4</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C282" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战斥罪累计造成40歼灭数&gt; 3星通关别传CB-4；必须携带并部署非助战斥罪，其他成员仅可编入4名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战伺夜并上场，且每次战斗至少释放1次领袖的尊严&gt; 3星通关主题曲3-8；必须编入非助战伺夜并上场，且使用伺夜歼灭碎骨</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="8" t="inlineStr">
         <is>
-          <t>斥罪</t>
+          <t>伺夜</t>
         </is>
       </c>
       <c r="B283" s="8" t="inlineStr">
         <is>
-          <t>IS-7</t>
+          <t>IS-6</t>
         </is>
       </c>
       <c r="C283" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战斥罪累计使用披荆斩棘5次&gt; 3星通关别传IS-7；必须编入非助战斥罪并上场，且不编入其他医疗干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战伺夜，并确定第一位部署的干员是伺夜&gt; 3星通关别传IS-6；必须编入非助战伺夜并上场，且至少使用3次领袖的尊严</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="8" t="inlineStr">
         <is>
-          <t>缄默德克萨斯</t>
+          <t>斥罪</t>
         </is>
       </c>
       <c r="B284" s="8" t="inlineStr">
         <is>
-          <t>CB-8</t>
+          <t>CB-4</t>
         </is>
       </c>
       <c r="C284" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战缄默德克萨斯累计歼灭10个精英或领袖敌人&gt; 3星通关别传CB-8；必须编入非助战缄默德克萨斯并上场，且使用缄默德克萨斯歼灭至少2个灰尾</t>
+          <t>&gt; 由非助战斥罪累计造成40歼灭数&gt; 3星通关别传CB-4；必须携带并部署非助战斥罪，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="8" t="inlineStr">
         <is>
-          <t>谜图</t>
+          <t>斥罪</t>
         </is>
       </c>
       <c r="B285" s="8" t="inlineStr">
         <is>
-          <t>9-4</t>
+          <t>IS-7</t>
         </is>
       </c>
       <c r="C285" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战谜图并上场，且使用谜图歼灭至少3个敌人&gt; 3星通关主题曲9-4标准实战环境；必须编入非助战谜图并上场，其他成员不可编入先锋干员</t>
+          <t>&gt; 战斗中非助战斥罪累计使用披荆斩棘5次&gt; 3星通关别传IS-7；必须编入非助战斥罪并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="8" t="inlineStr">
         <is>
-          <t>和弦</t>
+          <t>缄默德克萨斯</t>
         </is>
       </c>
       <c r="B286" s="8" t="inlineStr">
         <is>
-          <t>6-5</t>
+          <t>CB-8</t>
         </is>
       </c>
       <c r="C286" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战和弦并上场，且每次战斗至少释放一次沉溺之灾&gt; 3星通关主题曲6-5；必须编入非助战和弦并上场，且使用和弦歼灭至少2个宿主重装士兵</t>
+          <t>&gt; 由非助战缄默德克萨斯累计歼灭10个精英或领袖敌人&gt; 3星通关别传CB-8；必须编入非助战缄默德克萨斯并上场，且使用缄默德克萨斯歼灭至少2个灰尾</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="8" t="inlineStr">
         <is>
-          <t>焰影苇草</t>
+          <t>谜图</t>
         </is>
       </c>
       <c r="B287" s="8" t="inlineStr">
         <is>
-          <t>11-6</t>
+          <t>9-4</t>
         </is>
       </c>
       <c r="C287" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战焰影苇草累计使用枯荣共息10次&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战焰影苇草并上场，且使用焰影苇草至少歼灭40个敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战谜图并上场，且使用谜图歼灭至少3个敌人&gt; 3星通关主题曲9-4标准实战环境；必须编入非助战谜图并上场，其他成员不可编入先锋干员</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="8" t="inlineStr">
         <is>
-          <t>截云</t>
+          <t>和弦</t>
         </is>
       </c>
       <c r="B288" s="8" t="inlineStr">
         <is>
-          <t>S2-2</t>
+          <t>6-5</t>
         </is>
       </c>
       <c r="C288" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战截云累计造成100000点伤害&gt; 3星通关主题曲S2-2；必须编入非助战截云并上场，且使用截云至少歼灭10名敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战和弦并上场，且每次战斗至少释放一次沉溺之灾&gt; 3星通关主题曲6-5；必须编入非助战和弦并上场，且使用和弦歼灭至少2个宿主重装士兵</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="8" t="inlineStr">
         <is>
-          <t>火哨</t>
+          <t>焰影苇草</t>
         </is>
       </c>
       <c r="B289" s="8" t="inlineStr">
         <is>
-          <t>S4-6</t>
+          <t>11-6</t>
         </is>
       </c>
       <c r="C289" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战火哨累计使用焦土8次&gt; 3星通关主题曲S4-6；必须携带并部署非助战火哨，其他成员仅可编入远程位干员</t>
+          <t>&gt; 战斗中非助战焰影苇草累计使用枯荣共息10次&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战焰影苇草并上场，且使用焰影苇草至少歼灭40个敌人</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="8" t="inlineStr">
         <is>
-          <t>林</t>
+          <t>截云</t>
         </is>
       </c>
       <c r="B290" s="8" t="inlineStr">
         <is>
-          <t>11-6</t>
+          <t>S2-2</t>
         </is>
       </c>
       <c r="C290" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战林累计歼灭80个敌人&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战林并上场，且不编入重装干员</t>
+          <t>&gt; 由非助战截云累计造成100000点伤害&gt; 3星通关主题曲S2-2；必须编入非助战截云并上场，且使用截云至少歼灭10名敌人</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="8" t="inlineStr">
         <is>
-          <t>林</t>
+          <t>火哨</t>
         </is>
       </c>
       <c r="B291" s="8" t="inlineStr">
         <is>
-          <t>6-5</t>
+          <t>S4-6</t>
         </is>
       </c>
       <c r="C291" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战林并上场，且每次战斗至少释放1次流光乍裂&gt; 3星通关主题曲6-5；必须携带且部署非助战林，且至少释放3次流光乍裂</t>
+          <t>&gt; 战斗中非助战火哨累计使用焦土8次&gt; 3星通关主题曲S4-6；必须携带并部署非助战火哨，其他成员仅可编入远程位干员</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="8" t="inlineStr">
         <is>
-          <t>重岳</t>
+          <t>林</t>
         </is>
       </c>
       <c r="B292" s="8" t="inlineStr">
         <is>
-          <t>WB-7</t>
+          <t>11-6</t>
         </is>
       </c>
       <c r="C292" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战重岳累计造成120000点伤害&gt; 3星通关别传WB-7；必须携带并部署非助战重岳，其他成员仅可编入4名干员</t>
+          <t>&gt; 由非助战林累计歼灭80个敌人&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战林并上场，且不编入重装干员</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="8" t="inlineStr">
         <is>
-          <t>重岳</t>
+          <t>林</t>
         </is>
       </c>
       <c r="B293" s="8" t="inlineStr">
         <is>
-          <t>GA-5</t>
+          <t>6-5</t>
         </is>
       </c>
       <c r="C293" s="6" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战重岳累计使用50次我无&gt; 3星通关别传GA-5；必须携带且部署非助战重岳，其他成员仅可编入4名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战林并上场，且每次战斗至少释放1次流光乍裂&gt; 3星通关主题曲6-5；必须携带且部署非助战林，且至少释放3次流光乍裂</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="8" t="inlineStr">
         <is>
-          <t>铎铃</t>
+          <t>重岳</t>
         </is>
       </c>
       <c r="B294" s="8" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>WB-7</t>
         </is>
       </c>
       <c r="C294" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战铎铃累计使用乡心无改6次&gt; 3星通关主题曲2-1；必须编入非助战铎铃并上场，且使用3次乡心无改</t>
+          <t>&gt; 由非助战重岳累计造成120000点伤害&gt; 3星通关别传WB-7；必须携带并部署非助战重岳，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="8" t="inlineStr">
         <is>
-          <t>仇白</t>
+          <t>重岳</t>
         </is>
       </c>
       <c r="B295" s="8" t="inlineStr">
         <is>
-          <t>WB-7</t>
+          <t>GA-5</t>
         </is>
       </c>
       <c r="C295" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战仇白累计造成40歼灭数&gt; 3星通关别传WB-7；必须编入非助战仇白并上场，并使用仇白至少击败3名“破坚”</t>
+          <t>&gt; 使用非助战重岳累计使用50次我无&gt; 3星通关别传GA-5；必须携带且部署非助战重岳，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="8" t="inlineStr">
         <is>
-          <t>火龙S黑角</t>
+          <t>铎铃</t>
         </is>
       </c>
       <c r="B296" s="8" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="C296" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战火龙S黑角累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲3-8；必须编入非助战火龙S黑角并上场，且使用火龙S黑角歼灭碎骨</t>
+          <t>&gt; 战斗中非助战铎铃累计使用乡心无改6次&gt; 3星通关主题曲2-1；必须编入非助战铎铃并上场，且使用3次乡心无改</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="8" t="inlineStr">
         <is>
-          <t>麒麟R夜刀</t>
+          <t>仇白</t>
         </is>
       </c>
       <c r="B297" s="8" t="inlineStr">
         <is>
-          <t>3-7</t>
+          <t>WB-7</t>
         </is>
       </c>
       <c r="C297" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；每次战斗至少部署3次非助战的麒麟R夜刀&gt; 3星通关主题曲3-7；必须编入非助战麒麟R夜刀并上场，且使用麒麟R夜刀歼灭至少2名炮手</t>
+          <t>&gt; 由非助战仇白累计造成40歼灭数&gt; 3星通关别传WB-7；必须编入非助战仇白并上场，并使用仇白至少击败3名“破坚”</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="8" t="inlineStr">
         <is>
-          <t>休谟斯</t>
+          <t>火龙S黑角</t>
         </is>
       </c>
       <c r="B298" s="8" t="inlineStr">
         <is>
-          <t>7-8</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C298" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战休谟斯并上场，且每次战斗至少释放1次高效处理&gt; 3星通关主题曲7-8；必须编入非助战休谟斯并上场，其他成员仅可编入近战位干员</t>
+          <t>&gt; 由非助战火龙S黑角累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲3-8；必须编入非助战火龙S黑角并上场，且使用火龙S黑角歼灭碎骨</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="8" t="inlineStr">
         <is>
-          <t>摩根</t>
+          <t>麒麟R夜刀</t>
         </is>
       </c>
       <c r="B299" s="8" t="inlineStr">
         <is>
-          <t>4-5</t>
+          <t>3-7</t>
         </is>
       </c>
       <c r="C299" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战摩根累计造成80000点伤害&gt; 3星通关主题曲4-5，必须编入非助战摩根并上场，且使用摩根至少歼灭10名敌人</t>
+          <t>&gt; 完成5次战斗；每次战斗至少部署3次非助战的麒麟R夜刀&gt; 3星通关主题曲3-7；必须编入非助战麒麟R夜刀并上场，且使用麒麟R夜刀歼灭至少2名炮手</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="8" t="inlineStr">
         <is>
-          <t>洋灰</t>
+          <t>休谟斯</t>
         </is>
       </c>
       <c r="B300" s="8" t="inlineStr">
         <is>
-          <t>IW-EX-6</t>
+          <t>7-8</t>
         </is>
       </c>
       <c r="C300" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战洋灰并上场，且每次战斗至少释放1次结构加固&gt; 3星通关别传IW-EX-6，必须编入非助战洋灰并上场，且不编入其他重装干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战休谟斯并上场，且每次战斗至少释放1次高效处理&gt; 3星通关主题曲7-8；必须编入非助战休谟斯并上场，其他成员仅可编入近战位干员</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="8" t="inlineStr">
         <is>
-          <t>伊内丝</t>
+          <t>摩根</t>
         </is>
       </c>
       <c r="B301" s="8" t="inlineStr">
         <is>
-          <t>12-12</t>
+          <t>4-5</t>
         </is>
       </c>
       <c r="C301" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中累计部署非助战伊内丝12次&gt; 3星通关主题曲12-12标准实战环境；必须编入非助战伊内丝并上场，且至少使用3次暗夜无明</t>
+          <t>&gt; 由非助战摩根累计造成80000点伤害&gt; 3星通关主题曲4-5，必须编入非助战摩根并上场，且使用摩根至少歼灭10名敌人</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="8" t="inlineStr">
         <is>
-          <t>玫拉</t>
+          <t>洋灰</t>
         </is>
       </c>
       <c r="B302" s="8" t="inlineStr">
         <is>
-          <t>S3-5</t>
+          <t>IW-EX-6</t>
         </is>
       </c>
       <c r="C302" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战玫拉并上场，且每次战斗至少释放1次临界爆发&gt; 3星通关主题曲S3-5；必须编入非助战玫拉并上场，其他成员仅可编入6名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战洋灰并上场，且每次战斗至少释放1次结构加固&gt; 3星通关别传IW-EX-6，必须编入非助战洋灰并上场，且不编入其他重装干员</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="8" t="inlineStr">
         <is>
-          <t>淬羽赫默</t>
+          <t>伊内丝</t>
         </is>
       </c>
       <c r="B303" s="8" t="inlineStr">
         <is>
-          <t>6-3</t>
+          <t>12-12</t>
         </is>
       </c>
       <c r="C303" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战淬羽赫默累计使用无畏者协议8次&gt; 3星通关主题曲6-3；必须编入非助战淬羽赫默并上场，且所有干员不被击倒</t>
+          <t>&gt; 战斗中累计部署非助战伊内丝12次&gt; 3星通关主题曲12-12标准实战环境；必须编入非助战伊内丝并上场，且至少使用3次暗夜无明</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="8" t="inlineStr">
         <is>
-          <t>淬羽赫默</t>
+          <t>玫拉</t>
         </is>
       </c>
       <c r="B304" s="8" t="inlineStr">
         <is>
-          <t>WB-5</t>
+          <t>S3-5</t>
         </is>
       </c>
       <c r="C304" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战淬羽赫默并上场，且每次战斗至少释放1次无畏者协议&gt; 3星通关插曲WB-5；必须编入非助战淬羽赫默并上场，且所有干员不被击倒</t>
+          <t>&gt; 完成5次战斗；必须编入非助战玫拉并上场，且每次战斗至少释放1次临界爆发&gt; 3星通关主题曲S3-5；必须编入非助战玫拉并上场，其他成员仅可编入6名干员</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="8" t="inlineStr">
         <is>
-          <t>霍尔海雅</t>
+          <t>淬羽赫默</t>
         </is>
       </c>
       <c r="B305" s="8" t="inlineStr">
         <is>
-          <t>OF-7</t>
+          <t>6-3</t>
         </is>
       </c>
       <c r="C305" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战霍尔海雅累计造成120000点伤害&gt; 3星通关别传OF-7；必须编入非助战霍尔海雅并上场，且至少使用2次博览者的狂语</t>
+          <t>&gt; 战斗中非助战淬羽赫默累计使用无畏者协议8次&gt; 3星通关主题曲6-3；必须编入非助战淬羽赫默并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="8" t="inlineStr">
         <is>
-          <t>霍尔海雅</t>
+          <t>淬羽赫默</t>
         </is>
       </c>
       <c r="B306" s="8" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>WB-5</t>
         </is>
       </c>
       <c r="C306" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战霍尔海雅并上场，且每次战斗至少释放1次博览者的狂语&gt; 3星通关主题曲4-3；必须编入非助战霍尔海雅并上场，且使用霍尔海雅至少歼灭10个敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战淬羽赫默并上场，且每次战斗至少释放1次无畏者协议&gt; 3星通关插曲WB-5；必须编入非助战淬羽赫默并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="8" t="inlineStr">
         <is>
-          <t>缪尔赛思</t>
+          <t>霍尔海雅</t>
         </is>
       </c>
       <c r="B307" s="8" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>OF-7</t>
         </is>
       </c>
       <c r="C307" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战缪尔赛思，并确定第一位部署的干员是缪尔赛思&gt; 3星通关主题曲3-4；必须编入非助战缪尔赛思并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 由非助战霍尔海雅累计造成120000点伤害&gt; 3星通关别传OF-7；必须编入非助战霍尔海雅并上场，且至少使用2次博览者的狂语</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="8" t="inlineStr">
         <is>
-          <t>缪尔赛思</t>
+          <t>霍尔海雅</t>
         </is>
       </c>
       <c r="B308" s="8" t="inlineStr">
         <is>
-          <t>6-12</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C308" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战缪尔赛思并上场，且每次战斗至少释放1次生态耦合&gt; 3星通关主题曲6-12；必须编入非助战缪尔赛思并上场，且使用2次生态耦合</t>
+          <t>&gt; 完成5次战斗；必须编入非助战霍尔海雅并上场，且每次战斗至少释放1次博览者的狂语&gt; 3星通关主题曲4-3；必须编入非助战霍尔海雅并上场，且使用霍尔海雅至少歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="8" t="inlineStr">
         <is>
-          <t>隐现</t>
+          <t>缪尔赛思</t>
         </is>
       </c>
       <c r="B309" s="8" t="inlineStr">
@@ -6039,1316 +6039,1418 @@
       </c>
       <c r="C309" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战隐现累计造成30歼灭数&gt; 3星通关主题曲3-4；必须编入非助战隐现并上场，且不编入其他狙击干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战缪尔赛思，并确定第一位部署的干员是缪尔赛思&gt; 3星通关主题曲3-4；必须编入非助战缪尔赛思并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="8" t="inlineStr">
         <is>
-          <t>空构</t>
+          <t>缪尔赛思</t>
         </is>
       </c>
       <c r="B310" s="8" t="inlineStr">
         <is>
-          <t>DM-2</t>
+          <t>6-12</t>
         </is>
       </c>
       <c r="C310" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战空构累计造成60000点伤害&gt; 3星通关插曲DM-2；必须编入非助战空构并上场，且至少使用1次临场铳械改装</t>
+          <t>&gt; 完成5次战斗；必须编入非助战缪尔赛思并上场，且每次战斗至少释放1次生态耦合&gt; 3星通关主题曲6-12；必须编入非助战缪尔赛思并上场，且使用2次生态耦合</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="8" t="inlineStr">
         <is>
-          <t>圣约送葬人</t>
+          <t>隐现</t>
         </is>
       </c>
       <c r="B311" s="8" t="inlineStr">
         <is>
-          <t>7-14</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="C311" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战圣约送葬人累计造成80000点伤害&gt; 3星通关主题曲7-14；必须编入非助战圣约送葬人并上场，且使用圣约送葬人歼灭至少2名游击队盾卫</t>
+          <t>&gt; 由非助战隐现累计造成30歼灭数&gt; 3星通关主题曲3-4；必须编入非助战隐现并上场，且不编入其他狙击干员</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="8" t="inlineStr">
         <is>
-          <t>寒檀</t>
+          <t>空构</t>
         </is>
       </c>
       <c r="B312" s="8" t="inlineStr">
         <is>
-          <t>BI-2</t>
+          <t>DM-2</t>
         </is>
       </c>
       <c r="C312" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战寒檀并上场，且每次战斗至少释放1次“女巫之泪”&gt; 3星通关别传BI-2；必须编入非助战寒檀并上场，且使用寒檀至少歼灭8个敌人</t>
+          <t>&gt; 由非助战空构累计造成60000点伤害&gt; 3星通关插曲DM-2；必须编入非助战空构并上场，且至少使用1次临场铳械改装</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="8" t="inlineStr">
         <is>
-          <t>提丰</t>
+          <t>圣约送葬人</t>
         </is>
       </c>
       <c r="B313" s="8" t="inlineStr">
         <is>
-          <t>S2-1</t>
+          <t>7-14</t>
         </is>
       </c>
       <c r="C313" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战提丰累计造成120000点伤害&gt; 3星通关主题曲S2-1；必须编入非助战提丰并上场，其他成员仅可编入近战位干员</t>
+          <t>&gt; 由非助战圣约送葬人累计造成80000点伤害&gt; 3星通关主题曲7-14；必须编入非助战圣约送葬人并上场，且使用圣约送葬人歼灭至少2名游击队盾卫</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="8" t="inlineStr">
         <is>
-          <t>凛视</t>
+          <t>寒檀</t>
         </is>
       </c>
       <c r="B314" s="8" t="inlineStr">
         <is>
-          <t>7-13</t>
+          <t>BI-2</t>
         </is>
       </c>
       <c r="C314" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战凛视累计造成30次凋亡爆发&gt; 3星通关主题曲7-13；必须编入非助战凛视并上场，且凛视造成至少1次凋亡爆发</t>
+          <t>&gt; 完成5次战斗；必须编入非助战寒檀并上场，且每次战斗至少释放1次“女巫之泪”&gt; 3星通关别传BI-2；必须编入非助战寒檀并上场，且使用寒檀至少歼灭8个敌人</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="8" t="inlineStr">
         <is>
-          <t>苍苔</t>
+          <t>提丰</t>
         </is>
       </c>
       <c r="B315" s="8" t="inlineStr">
         <is>
-          <t>9-3</t>
+          <t>S2-1</t>
         </is>
       </c>
       <c r="C315" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战苍苔并上场，且每次战斗至少释放1次土石的恒心&gt; 3星通关主题曲9-3标准实战环境；必须编入非助战苍苔并上场，且所有干员不被击倒</t>
+          <t>&gt; 由非助战提丰累计造成120000点伤害&gt; 3星通关主题曲S2-1；必须编入非助战提丰并上场，其他成员仅可编入近战位干员</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="8" t="inlineStr">
         <is>
-          <t>青枳</t>
+          <t>凛视</t>
         </is>
       </c>
       <c r="B316" s="8" t="inlineStr">
         <is>
-          <t>OF-5</t>
+          <t>7-13</t>
         </is>
       </c>
       <c r="C316" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战青枳，并确定第一位部署的干员是青枳&gt; 3星通关别传OF-5；必须编入非助战青枳并上场，且不编入其他先锋干员</t>
+          <t>&gt; 由非助战凛视累计造成30次凋亡爆发&gt; 3星通关主题曲7-13；必须编入非助战凛视并上场，且凛视造成至少1次凋亡爆发</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="8" t="inlineStr">
         <is>
-          <t>琳琅诗怀雅</t>
+          <t>苍苔</t>
         </is>
       </c>
       <c r="B317" s="8" t="inlineStr">
         <is>
-          <t>5-2</t>
+          <t>9-3</t>
         </is>
       </c>
       <c r="C317" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战琳琅诗怀雅累计造成60000点伤害※香槟炸弹造成的伤害也会参与计数&gt; 3星通关主题曲5-2；必须编入非助战琳琅诗怀雅并上场，且使用琳琅诗怀雅至少歼灭15个敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战苍苔并上场，且每次战斗至少释放1次土石的恒心&gt; 3星通关主题曲9-3标准实战环境；必须编入非助战苍苔并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="8" t="inlineStr">
         <is>
-          <t>琳琅诗怀雅</t>
+          <t>青枳</t>
         </is>
       </c>
       <c r="B318" s="8" t="inlineStr">
         <is>
-          <t>11-16</t>
+          <t>OF-5</t>
         </is>
       </c>
       <c r="C318" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战琳琅诗怀雅累计造成40歼灭数&gt; 3星通关主题曲11-16标准实战环境；必须编入非助战琳琅诗怀雅并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战青枳，并确定第一位部署的干员是青枳&gt; 3星通关别传OF-5；必须编入非助战青枳并上场，且不编入其他先锋干员</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="8" t="inlineStr">
         <is>
-          <t>纯烬艾雅法拉</t>
+          <t>琳琅诗怀雅</t>
         </is>
       </c>
       <c r="B319" s="8" t="inlineStr">
         <is>
-          <t>FC-5</t>
+          <t>5-2</t>
         </is>
       </c>
       <c r="C319" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战纯烬艾雅法拉并上场，且每次战斗至少释放1次火山回响&gt; 3星通关别传FC-5；必须编入非助战纯烬艾雅法拉并上场，且不编入其他医疗干员</t>
+          <t>&gt; 由非助战琳琅诗怀雅累计造成60000点伤害※香槟炸弹造成的伤害也会参与计数&gt; 3星通关主题曲5-2；必须编入非助战琳琅诗怀雅并上场，且使用琳琅诗怀雅至少歼灭15个敌人</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="8" t="inlineStr">
         <is>
-          <t>冰酿</t>
+          <t>琳琅诗怀雅</t>
         </is>
       </c>
       <c r="B320" s="8" t="inlineStr">
         <is>
-          <t>S3-3</t>
+          <t>11-16</t>
         </is>
       </c>
       <c r="C320" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战冰酿累计造成80000伤害&gt; 3星通关主题曲S3-3；必须编入非助战冰酿并上场，且使用冰酿至少歼灭8个敌人</t>
+          <t>&gt; 由非助战琳琅诗怀雅累计造成40歼灭数&gt; 3星通关主题曲11-16标准实战环境；必须编入非助战琳琅诗怀雅并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="8" t="inlineStr">
         <is>
-          <t>杏仁</t>
+          <t>纯烬艾雅法拉</t>
         </is>
       </c>
       <c r="B321" s="8" t="inlineStr">
         <is>
-          <t>BI-2</t>
+          <t>FC-5</t>
         </is>
       </c>
       <c r="C321" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战杏仁累计使用强力牵引10次&gt; 3星通关别传BI-2；必须编入非助战杏仁并上场，且至少使用2次强力牵引</t>
+          <t>&gt; 完成5次战斗；必须编入非助战纯烬艾雅法拉并上场，且每次战斗至少释放1次火山回响&gt; 3星通关别传FC-5；必须编入非助战纯烬艾雅法拉并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="8" t="inlineStr">
         <is>
-          <t>涤火杰西卡</t>
+          <t>冰酿</t>
         </is>
       </c>
       <c r="B322" s="8" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>S3-3</t>
         </is>
       </c>
       <c r="C322" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战涤火杰西卡累计造成30歼灭数&gt; 3星通关主题曲3-8；必须编入非助战涤火杰西卡并上场，且使用涤火杰西卡歼灭碎骨</t>
+          <t>&gt; 由非助战冰酿累计造成80000伤害&gt; 3星通关主题曲S3-3；必须编入非助战冰酿并上场，且使用冰酿至少歼灭8个敌人</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="8" t="inlineStr">
         <is>
-          <t>维荻</t>
+          <t>杏仁</t>
         </is>
       </c>
       <c r="B323" s="8" t="inlineStr">
         <is>
-          <t>9-3</t>
+          <t>BI-2</t>
         </is>
       </c>
       <c r="C323" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战维荻累计造成60000点伤害&gt; 3星通关主题曲9-3标准实战环境；必须编入非助战维荻并上场，且至少使用2次双刃毒藤</t>
+          <t>&gt; 战斗中非助战杏仁累计使用强力牵引10次&gt; 3星通关别传BI-2；必须编入非助战杏仁并上场，且至少使用2次强力牵引</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="8" t="inlineStr">
         <is>
-          <t>戴菲恩</t>
+          <t>涤火杰西卡</t>
         </is>
       </c>
       <c r="B324" s="8" t="inlineStr">
         <is>
-          <t>WD-6</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C324" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战戴菲恩累计造成30歼灭数&gt; 3星通关插曲WD-6；必须携带且部署非助战戴菲恩，且至少使用2次抢攻</t>
+          <t>&gt; 由非助战涤火杰西卡累计造成30歼灭数&gt; 3星通关主题曲3-8；必须编入非助战涤火杰西卡并上场，且使用涤火杰西卡歼灭碎骨</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="8" t="inlineStr">
         <is>
-          <t>刺玫</t>
+          <t>维荻</t>
         </is>
       </c>
       <c r="B325" s="8" t="inlineStr">
         <is>
-          <t>IC-2</t>
+          <t>9-3</t>
         </is>
       </c>
       <c r="C325" s="6" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战刺玫累计使用荆藤庇荫10次&gt; 3星通关别传IC-2；必须编入非助战刺玫并上场，且不编入其他医疗干员</t>
+          <t>&gt; 由非助战维荻累计造成60000点伤害&gt; 3星通关主题曲9-3标准实战环境；必须编入非助战维荻并上场，且至少使用2次双刃毒藤</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="8" t="inlineStr">
         <is>
-          <t>赫德雷</t>
+          <t>戴菲恩</t>
         </is>
       </c>
       <c r="B326" s="8" t="inlineStr">
         <is>
-          <t>IW-7</t>
+          <t>WD-6</t>
         </is>
       </c>
       <c r="C326" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战赫德雷累计歼灭5个精英或领袖敌人&gt; 3星通关别传IW-7；必须编入非助战赫德雷并上场，并使用赫德雷至少击败2名沉沙</t>
+          <t>&gt; 由非助战戴菲恩累计造成30歼灭数&gt; 3星通关插曲WD-6；必须携带且部署非助战戴菲恩，且至少使用2次抢攻</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="8" t="inlineStr">
         <is>
-          <t>深律</t>
+          <t>刺玫</t>
         </is>
       </c>
       <c r="B327" s="8" t="inlineStr">
         <is>
-          <t>LE-4</t>
+          <t>IC-2</t>
         </is>
       </c>
       <c r="C327" s="6" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战深律并上场，且每次战斗至少释放1次沉音宁神&gt; 3星通关别传LE-4；必须编入非助战深律并上场，且所有干员不被击倒</t>
+          <t>&gt; 战斗中非助战刺玫累计使用荆藤庇荫10次&gt; 3星通关别传IC-2；必须编入非助战刺玫并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="8" t="inlineStr">
         <is>
-          <t>止颂</t>
+          <t>赫德雷</t>
         </is>
       </c>
       <c r="B328" s="8" t="inlineStr">
         <is>
-          <t>7-11</t>
+          <t>IW-7</t>
         </is>
       </c>
       <c r="C328" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战止颂累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲7-11；必须编入非助战止颂并上场，且使用止颂歼灭至少2名雇佣军萨卡兹战士</t>
+          <t>&gt; 由非助战赫德雷累计歼灭5个精英或领袖敌人&gt; 3星通关别传IW-7；必须编入非助战赫德雷并上场，并使用赫德雷至少击败2名沉沙</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="8" t="inlineStr">
         <is>
-          <t>止颂</t>
+          <t>深律</t>
         </is>
       </c>
       <c r="B329" s="8" t="inlineStr">
         <is>
-          <t>TW-5</t>
+          <t>LE-4</t>
         </is>
       </c>
       <c r="C329" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战止颂累计造成120000点伤害&gt; 3星通关别传TW-5；必须编入非助战止颂并上场，且使用止颂击败至少6名敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战深律并上场，且每次战斗至少释放1次沉音宁神&gt; 3星通关别传LE-4；必须编入非助战深律并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="8" t="inlineStr">
         <is>
-          <t>薇薇安娜</t>
+          <t>止颂</t>
         </is>
       </c>
       <c r="B330" s="8" t="inlineStr">
         <is>
-          <t>MN-3</t>
+          <t>7-11</t>
         </is>
       </c>
       <c r="C330" s="6" t="inlineStr">
         <is>
-          <t>&gt; 由非助战薇薇安娜累计歼灭10个精英或领袖敌人&gt; 3星通关别传MN-3；必须编入非助战薇薇安娜并上场，且使用薇薇安娜歼灭“锈铜”奥尔默·英格拉</t>
+          <t>&gt; 由非助战止颂累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲7-11；必须编入非助战止颂并上场，且使用止颂歼灭至少2名雇佣军萨卡兹战士</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="7" t="inlineStr">
         <is>
-          <t>塑心</t>
+          <t>止颂</t>
         </is>
       </c>
       <c r="B331" s="7" t="inlineStr">
         <is>
-          <t>GA-7</t>
+          <t>TW-5</t>
         </is>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>&gt; 由非助战塑心累计造成75000点凋亡损伤&gt; 3星通关别传GA-7；必须编入非助战塑心并上场，且塑心造成至少15000点凋亡损伤</t>
+          <t>&gt; 由非助战止颂累计造成120000点伤害&gt; 3星通关别传TW-5；必须编入非助战止颂并上场，且使用止颂击败至少6名敌人</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="7" t="inlineStr">
         <is>
-          <t>哈洛德</t>
+          <t>薇薇安娜</t>
         </is>
       </c>
       <c r="B332" s="7" t="inlineStr">
         <is>
-          <t>9-13</t>
+          <t>MN-3</t>
         </is>
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战哈洛德累计使用重症优先8次&gt; 3星通关主题曲9-13标准实战环境；必须编入非助战哈洛德并上场，且所有干员不被击倒</t>
+          <t>&gt; 由非助战薇薇安娜累计歼灭10个精英或领袖敌人&gt; 3星通关别传MN-3；必须编入非助战薇薇安娜并上场，且使用薇薇安娜歼灭“锈铜”奥尔默·英格拉</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="7" t="inlineStr">
         <is>
-          <t>烈夏</t>
+          <t>塑心</t>
         </is>
       </c>
       <c r="B333" s="7" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>GA-7</t>
         </is>
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>&gt; 由非助战烈夏累计造成30歼灭数&gt; 3星通关主题曲4-3；必须编入非助战烈夏并上场，且不编入其他近卫干员</t>
+          <t>&gt; 由非助战塑心累计造成75000点凋亡损伤&gt; 3星通关别传GA-7；必须编入非助战塑心并上场，且塑心造成至少15000点凋亡损伤</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="7" t="inlineStr">
         <is>
-          <t>锏</t>
+          <t>哈洛德</t>
         </is>
       </c>
       <c r="B334" s="7" t="inlineStr">
         <is>
-          <t>BI-6</t>
+          <t>9-13</t>
         </is>
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战锏并上场，且每次战斗至少释放1次归于宁静&gt; 3星通关别传BI-6；必须编入非助战锏并上场，且使用锏至少歼灭10个敌人</t>
+          <t>&gt; 战斗中非助战哈洛德累计使用重症优先8次&gt; 3星通关主题曲9-13标准实战环境；必须编入非助战哈洛德并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="7" t="inlineStr">
         <is>
-          <t>莱伊</t>
+          <t>烈夏</t>
         </is>
       </c>
       <c r="B335" s="7" t="inlineStr">
         <is>
-          <t>S9-1</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>&gt; 由非助战莱伊累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲S9-1标准实战环境；必须编入非助战莱伊并上场，且使用莱伊使用至少2次“得见光芒”</t>
+          <t>&gt; 由非助战烈夏累计造成30歼灭数&gt; 3星通关主题曲4-3；必须编入非助战烈夏并上场，且不编入其他近卫干员</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="7" t="inlineStr">
         <is>
-          <t>万顷</t>
+          <t>锏</t>
         </is>
       </c>
       <c r="B336" s="7" t="inlineStr">
         <is>
-          <t>9-13</t>
+          <t>BI-6</t>
         </is>
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战万顷累计使用支援号令·γ型10次&gt; 3星通关主题曲9-13标准实战环境；必须编入非助战万顷并上场，且至少使用2次应东风</t>
+          <t>&gt; 完成5次战斗；必须编入非助战锏并上场，且每次战斗至少释放1次归于宁静&gt; 3星通关别传BI-6；必须编入非助战锏并上场，且使用锏至少歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="7" t="inlineStr">
         <is>
-          <t>小满</t>
+          <t>莱伊</t>
         </is>
       </c>
       <c r="B337" s="7" t="inlineStr">
         <is>
-          <t>9-11</t>
+          <t>S9-1</t>
         </is>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>&gt; 由非助战小满累计造成60000点伤害&gt; 3星通关主题曲9-11标准实战环境；必须编入非助战小满并上场，且至少使用2次乡音沉沉</t>
+          <t>&gt; 由非助战莱伊累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲S9-1标准实战环境；必须编入非助战莱伊并上场，且使用莱伊使用至少2次“得见光芒”</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="7" t="inlineStr">
         <is>
-          <t>左乐</t>
+          <t>万顷</t>
         </is>
       </c>
       <c r="B338" s="7" t="inlineStr">
         <is>
-          <t>WB-5</t>
+          <t>9-13</t>
         </is>
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>&gt; 由非助战左乐累计造成40歼灭数&gt; 3星通关别传WB-5；必须编入非助战左乐并上场，且使用左乐至少歼灭8个敌人</t>
+          <t>&gt; 战斗中非助战万顷累计使用支援号令·γ型10次&gt; 3星通关主题曲9-13标准实战环境；必须编入非助战万顷并上场，且至少使用2次应东风</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="7" t="inlineStr">
         <is>
-          <t>左乐</t>
+          <t>小满</t>
         </is>
       </c>
       <c r="B339" s="7" t="inlineStr">
         <is>
-          <t>RI-7</t>
+          <t>9-11</t>
         </is>
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战左乐累计造成100000点伤害&gt; 3星通关别传RI-7；必须携带且部署非助战左乐，且至少释放3次佑序有炎</t>
+          <t>&gt; 由非助战小满累计造成60000点伤害&gt; 3星通关主题曲9-11标准实战环境；必须编入非助战小满并上场，且至少使用2次乡音沉沉</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="7" t="inlineStr">
         <is>
-          <t>黍</t>
+          <t>左乐</t>
         </is>
       </c>
       <c r="B340" s="7" t="inlineStr">
         <is>
-          <t>11-11</t>
+          <t>WB-5</t>
         </is>
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战黍并上场，且每次战斗至少释放1次离离枯荣&gt; 3星通关主题曲11-11标准实战环境；必须编入非助战黍并上场，且所有干员不被击倒</t>
+          <t>&gt; 由非助战左乐累计造成40歼灭数&gt; 3星通关别传WB-5；必须编入非助战左乐并上场，且使用左乐至少歼灭8个敌人</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="7" t="inlineStr">
         <is>
-          <t>红隼</t>
+          <t>左乐</t>
         </is>
       </c>
       <c r="B341" s="7" t="inlineStr">
         <is>
-          <t>11-18</t>
+          <t>RI-7</t>
         </is>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战红隼并上场，且每次战斗至少释放2次醉刃乱舞&gt; 3星通关主题曲11-18标准实战环境；必须编入非助战红隼，且第一位部署红隼、红隼全程不撤退或被击倒</t>
+          <t>&gt; 使用非助战左乐累计造成100000点伤害&gt; 3星通关别传RI-7；必须携带且部署非助战左乐，且至少释放3次佑序有炎</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="7" t="inlineStr">
         <is>
-          <t>导火索</t>
+          <t>黍</t>
         </is>
       </c>
       <c r="B342" s="7" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>11-11</t>
         </is>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>&gt; 由非助战导火索累计造成80000点伤害&gt; 3星通关主题曲3-1；必须编入非助战导火索并上场，且使用导火索至少歼灭30个敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战黍并上场，且每次战斗至少释放1次离离枯荣&gt; 3星通关主题曲11-11标准实战环境；必须编入非助战黍并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="7" t="inlineStr">
         <is>
-          <t>双月</t>
+          <t>红隼</t>
         </is>
       </c>
       <c r="B343" s="7" t="inlineStr">
         <is>
-          <t>3-7</t>
+          <t>11-18</t>
         </is>
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战双月累计使用全知者的战术10次&gt; 3星通关主题曲3-7；必须编入非助战双月并上场，且至少使用2次全知者的战术</t>
+          <t>&gt; 完成5次战斗；必须编入非助战红隼并上场，且每次战斗至少释放2次醉刃乱舞&gt; 3星通关主题曲11-18标准实战环境；必须编入非助战红隼，且第一位部署红隼、红隼全程不撤退或被击倒</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="7" t="inlineStr">
         <is>
-          <t>医生</t>
+          <t>导火索</t>
         </is>
       </c>
       <c r="B344" s="7" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战医生累计使用激素手枪8次&gt; 3星通关主题曲2-5；必须编入非助战医生并上场，且不编入医疗干员</t>
+          <t>&gt; 由非助战导火索累计造成80000点伤害&gt; 3星通关主题曲3-1；必须编入非助战导火索并上场，且使用导火索至少歼灭30个敌人</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="7" t="inlineStr">
         <is>
-          <t>艾拉</t>
+          <t>双月</t>
         </is>
       </c>
       <c r="B345" s="7" t="inlineStr">
         <is>
-          <t>DM-EX-1</t>
+          <t>3-7</t>
         </is>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战艾拉累计部署雷鸣地雷30个&gt; 3星通关插曲DM-EX-1；必须编入非助战艾拉并上场，且使用艾拉歼灭至少2名萨卡兹穿刺手</t>
+          <t>&gt; 战斗中非助战双月累计使用全知者的战术10次&gt; 3星通关主题曲3-7；必须编入非助战双月并上场，且至少使用2次全知者的战术</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="7" t="inlineStr">
         <is>
-          <t>露托</t>
+          <t>医生</t>
         </is>
       </c>
       <c r="B346" s="7" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>2-5</t>
         </is>
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战露托累计使用强磁防卫8次&gt; 3星通关主题曲3-1；必须编入非助战露托并上场，且不编入其他重装干员</t>
+          <t>&gt; 战斗中非助战医生累计使用激素手枪8次&gt; 3星通关主题曲2-5；必须编入非助战医生并上场，且不编入医疗干员</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="7" t="inlineStr">
         <is>
-          <t>奥达</t>
+          <t>艾拉</t>
         </is>
       </c>
       <c r="B347" s="7" t="inlineStr">
         <is>
-          <t>S3-6</t>
+          <t>DM-EX-1</t>
         </is>
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战奥达累计使用4次锻锤之力&gt; 3星通关主题曲S3-6；必须携带且部署非助战奥达，其他成员仅可编入4名干员</t>
+          <t>&gt; 战斗中非助战艾拉累计部署雷鸣地雷30个&gt; 3星通关插曲DM-EX-1；必须编入非助战艾拉并上场，且使用艾拉歼灭至少2名萨卡兹穿刺手</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="7" t="inlineStr">
         <is>
-          <t>阿罗玛</t>
+          <t>露托</t>
         </is>
       </c>
       <c r="B348" s="7" t="inlineStr">
         <is>
-          <t>GT-HX-3</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战阿罗玛并上场，且每次战斗至少释放1次小心地滑&gt; 3星通关别传GT-HX-3；必须编入非助战阿罗玛并上场，且使用阿罗玛至少歼灭20个敌人</t>
+          <t>&gt; 战斗中非助战露托累计使用强磁防卫8次&gt; 3星通关主题曲3-1；必须编入非助战露托并上场，且不编入其他重装干员</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="7" t="inlineStr">
         <is>
-          <t>阿斯卡纶</t>
+          <t>奥达</t>
         </is>
       </c>
       <c r="B349" s="7" t="inlineStr">
         <is>
-          <t>11-6</t>
+          <t>S3-6</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>&gt; 由非助战阿斯卡纶累计造成180000点伤害&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战阿斯卡纶并上场，且使用阿斯卡纶至少歼灭30个敌人</t>
+          <t>&gt; 使用非助战奥达累计使用4次锻锤之力&gt; 3星通关主题曲S3-6；必须携带且部署非助战奥达，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="7" t="inlineStr">
         <is>
-          <t>历阵锐枪芬</t>
+          <t>阿罗玛</t>
         </is>
       </c>
       <c r="B350" s="7" t="inlineStr">
         <is>
-          <t>4-2</t>
+          <t>GT-HX-3</t>
         </is>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战历阵锐枪芬，并确定第一位部署的干员是历阵锐枪芬&gt; 3星通关主题曲4-2；必须编入非助战历阵锐枪芬并上场，且不编入其他先锋干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战阿罗玛并上场，且每次战斗至少释放1次小心地滑&gt; 3星通关别传GT-HX-3；必须编入非助战阿罗玛并上场，且使用阿罗玛至少歼灭20个敌人</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="7" t="inlineStr">
         <is>
-          <t>魔王</t>
+          <t>阿斯卡纶</t>
         </is>
       </c>
       <c r="B351" s="7" t="inlineStr">
         <is>
-          <t>14-5</t>
+          <t>11-6</t>
         </is>
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>&gt; 携带非助战魔王完成5次战斗，且每次战斗至少发动一次“编织重构现世”&gt; 3星通关主题曲14-5标准实战环境；必须编入非助战魔王并上场，其他成员仅可编入近战位干员</t>
+          <t>&gt; 由非助战阿斯卡纶累计造成180000点伤害&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战阿斯卡纶并上场，且使用阿斯卡纶至少歼灭30个敌人</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="7" t="inlineStr">
         <is>
-          <t>逻各斯</t>
+          <t>阿斯卡纶</t>
         </is>
       </c>
       <c r="B352" s="7" t="inlineStr">
         <is>
-          <t>14-9</t>
+          <t>5-10</t>
         </is>
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>&gt; 由非助战逻各斯累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲14-9标准实战环境；必须编入非助战逻各斯并上场，且使用逻各斯至少歼灭7个敌人</t>
+          <t>&gt; 战斗中非助战阿斯卡纶累计使用“降临”5次&gt; 3星通关主题曲5-10，必须编入非助战阿斯卡纶并上场，其他成员不可编入特种干员</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="7" t="inlineStr">
         <is>
-          <t>逻各斯</t>
+          <t>历阵锐枪芬</t>
         </is>
       </c>
       <c r="B353" s="7" t="inlineStr">
         <is>
-          <t>11-6</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>&gt; 由非助战逻各斯累计造成100000点伤害&gt; 3星通关主题曲11-6标准实战环境，必须编入非助战逻各斯并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战历阵锐枪芬，并确定第一位部署的干员是历阵锐枪芬&gt; 3星通关主题曲4-2；必须编入非助战历阵锐枪芬并上场，且不编入其他先锋干员</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="7" t="inlineStr">
         <is>
-          <t>维什戴尔</t>
+          <t>魔王</t>
         </is>
       </c>
       <c r="B354" s="7" t="inlineStr">
         <is>
-          <t>DM-5</t>
+          <t>14-5</t>
         </is>
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>&gt; 由非助战维什戴尔累计造成120000伤害&gt; 3星通关插曲DM-5；必须编入非助战维什戴尔并上场，且使用维什戴尔至少歼灭20个敌人</t>
+          <t>&gt; 携带非助战魔王完成5次战斗，且每次战斗至少发动一次“编织重构现世”&gt; 3星通关主题曲14-5标准实战环境；必须编入非助战魔王并上场，其他成员仅可编入近战位干员</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="7" t="inlineStr">
         <is>
-          <t>阿米娅(医疗)</t>
+          <t>逻各斯</t>
         </is>
       </c>
       <c r="B355" s="7" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>14-9</t>
         </is>
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战医疗职业的阿米娅累计使用慈悲愿景5次&gt; 3星通关主题曲3-8；必须编入非助战医疗职业的阿米娅并上场，且不编入其他医疗干员</t>
+          <t>&gt; 由非助战逻各斯累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲14-9标准实战环境；必须编入非助战逻各斯并上场，且使用逻各斯至少歼灭7个敌人</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="7" t="inlineStr">
         <is>
-          <t>深巡</t>
+          <t>逻各斯</t>
         </is>
       </c>
       <c r="B356" s="7" t="inlineStr">
         <is>
-          <t>SN-5</t>
+          <t>11-6</t>
         </is>
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战深巡累计使用行动能力剥夺8次&gt; 3星通关插曲SN-5，必须编入非助战深巡并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 由非助战逻各斯累计造成100000点伤害&gt; 3星通关主题曲11-6标准实战环境，必须编入非助战逻各斯并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="7" t="inlineStr">
         <is>
-          <t>海霓</t>
+          <t>维什戴尔</t>
         </is>
       </c>
       <c r="B357" s="7" t="inlineStr">
         <is>
-          <t>SV-4</t>
+          <t>DM-5</t>
         </is>
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战海霓累计使用阻滞性显色剂8次&gt; 3星通关插曲SV-4；必须编入非助战海霓并上场，且不编入其他辅助干员</t>
+          <t>&gt; 由非助战维什戴尔累计造成120000伤害&gt; 3星通关插曲DM-5；必须编入非助战维什戴尔并上场，且使用维什戴尔至少歼灭20个敌人</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="7" t="inlineStr">
         <is>
-          <t>乌尔比安</t>
+          <t>阿米娅(医疗)</t>
         </is>
       </c>
       <c r="B358" s="7" t="inlineStr">
         <is>
-          <t>SV-6</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战乌尔比安累计使用必须开辟的通路10次&gt; 3星通关插曲SV-6；必须编入非助战乌尔比安并上场，并使用乌尔比安至少击败2名囊海爬行者</t>
+          <t>&gt; 战斗中非助战医疗职业的阿米娅累计使用慈悲愿景5次&gt; 3星通关主题曲3-8；必须编入非助战医疗职业的阿米娅并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="7" t="inlineStr">
         <is>
-          <t>渡桥</t>
+          <t>深巡</t>
         </is>
       </c>
       <c r="B359" s="7" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>SN-5</t>
         </is>
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战渡桥累计使用承压功率8次&gt; 3星通关主题曲3-1；必须编入非助战渡桥并上场，且至少使用3次承压功率</t>
+          <t>&gt; 战斗中非助战深巡累计使用行动能力剥夺8次&gt; 3星通关插曲SN-5，必须编入非助战深巡并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="7" t="inlineStr">
         <is>
-          <t>锡人</t>
+          <t>海霓</t>
         </is>
       </c>
       <c r="B360" s="7" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>SV-4</t>
         </is>
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战锡人累计使用8次“大拉里”&gt; 3星通关主题曲4-3，必须编入非助战锡人并上场，且队伍中不能有其他医疗干员</t>
+          <t>&gt; 战斗中非助战海霓累计使用阻滞性显色剂8次&gt; 3星通关插曲SV-4；必须编入非助战海霓并上场，且不编入其他辅助干员</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="7" t="inlineStr">
         <is>
-          <t>衡沙</t>
+          <t>乌尔比安</t>
         </is>
       </c>
       <c r="B361" s="7" t="inlineStr">
         <is>
-          <t>DV-2</t>
+          <t>SV-6</t>
         </is>
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>&gt; 战斗中累计召唤非助战衡沙的召唤物20回&gt; 3星通关别传DV-2；必须编入非助战衡沙并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 战斗中非助战乌尔比安累计使用必须开辟的通路10次&gt; 3星通关插曲SV-6；必须编入非助战乌尔比安并上场，并使用乌尔比安至少击败2名囊海爬行者</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="7" t="inlineStr">
         <is>
-          <t>佩佩</t>
+          <t>渡桥</t>
         </is>
       </c>
       <c r="B362" s="7" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>&gt; 由非助战佩佩累计造成40歼灭数&gt; 3星通关主题曲3-8；必须编入非助战佩佩并上场，且使用佩佩歼灭碎骨</t>
+          <t>&gt; 战斗中非助战渡桥累计使用承压功率8次&gt; 3星通关主题曲3-1；必须编入非助战渡桥并上场，且至少使用3次承压功率</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="7" t="inlineStr">
         <is>
-          <t>森西</t>
+          <t>锡人</t>
         </is>
       </c>
       <c r="B363" s="7" t="inlineStr">
         <is>
-          <t>1-12</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战森西累计使用团体魔物大餐6次&gt; 3星通关主题曲1-12；必须编入非助战森西并上场，且所有干员不被击倒</t>
+          <t>&gt; 战斗中非助战锡人累计使用8次“大拉里”&gt; 3星通关主题曲4-3，必须编入非助战锡人并上场，且队伍中不能有其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="7" t="inlineStr">
         <is>
-          <t>齐尔查克</t>
+          <t>衡沙</t>
         </is>
       </c>
       <c r="B364" s="7" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>DV-2</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战齐尔查克累计使用随机应变6次&gt; 3星通关主题曲4-3；必须编入非助战齐尔查克并上场，其他成员不可编入先锋干员</t>
+          <t>&gt; 战斗中累计召唤非助战衡沙的召唤物20回&gt; 3星通关别传DV-2；必须编入非助战衡沙并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="7" t="inlineStr">
         <is>
-          <t>莱欧斯</t>
+          <t>佩佩</t>
         </is>
       </c>
       <c r="B365" s="7" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战莱欧斯并上场，且每次战斗至少释放1次威吓战法&gt; 3星通关主题曲2-4；必须编入非助战莱欧斯并上场，并使用莱欧斯至少击败1名高阶术师</t>
+          <t>&gt; 由非助战佩佩累计造成40歼灭数&gt; 3星通关主题曲3-8；必须编入非助战佩佩并上场，且使用佩佩歼灭碎骨</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="7" t="inlineStr">
         <is>
-          <t>玛露西尔</t>
+          <t>森西</t>
         </is>
       </c>
       <c r="B366" s="7" t="inlineStr">
         <is>
-          <t>5-10</t>
+          <t>1-12</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>&gt; 由非助战玛露西尔累计造成100000点伤害&gt; 3星通关主题曲5-10；必须编入非助战玛露西尔并上场，且使用玛露西尔至少歼灭10名敌人</t>
+          <t>&gt; 战斗中非助战森西累计使用团体魔物大餐6次&gt; 3星通关主题曲1-12；必须编入非助战森西并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="7" t="inlineStr">
         <is>
-          <t>凯瑟琳</t>
+          <t>齐尔查克</t>
         </is>
       </c>
       <c r="B367" s="7" t="inlineStr">
         <is>
-          <t>11-7</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战凯瑟琳累计部署15个“支援装置”&gt; 3星通关主题曲11-7标准实战环境；必须编入非助战凯瑟琳并上场，且凯瑟琳使用至少2次“战火淬炼”</t>
+          <t>&gt; 战斗中非助战齐尔查克累计使用随机应变6次&gt; 3星通关主题曲4-3；必须编入非助战齐尔查克并上场，其他成员不可编入先锋干员</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="7" t="inlineStr">
         <is>
-          <t>波卜</t>
+          <t>莱欧斯</t>
         </is>
       </c>
       <c r="B368" s="7" t="inlineStr">
         <is>
-          <t>4-8</t>
+          <t>2-4</t>
         </is>
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>&gt; 由非助战波卜累计造成30次灼燃爆发&gt; 3星通关主题曲4-8；必须编入非助战波卜并上场，且波卜使用至少2次“此路不通”</t>
+          <t>&gt; 完成5次战斗；必须编入非助战莱欧斯并上场，且每次战斗至少释放1次威吓战法&gt; 3星通关主题曲2-4；必须编入非助战莱欧斯并上场，并使用莱欧斯至少击败1名高阶术师</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="7" t="inlineStr">
         <is>
-          <t>维娜·维多利亚</t>
+          <t>玛露西尔</t>
         </is>
       </c>
       <c r="B369" s="7" t="inlineStr">
         <is>
-          <t>9-5</t>
+          <t>5-10</t>
         </is>
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>&gt; 由非助战维娜·维多利亚累计造成120000点伤害&gt; 3星通关主题曲9-5标准实战环境；必须编入非助战维娜·维多利亚并上场，其他成员仅可编入5名干员</t>
+          <t>&gt; 由非助战玛露西尔累计造成100000点伤害&gt; 3星通关主题曲5-10；必须编入非助战玛露西尔并上场，且使用玛露西尔至少歼灭10名敌人</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="7" t="inlineStr">
         <is>
-          <t>裁度</t>
+          <t>凯瑟琳</t>
         </is>
       </c>
       <c r="B370" s="7" t="inlineStr">
         <is>
-          <t>5-8</t>
+          <t>11-7</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战裁度并部署至少2次，且使用裁度击败至少4名敌人&gt; 3星通关主题曲5-8；必须编入非助战裁度并上场，且至少束缚12次敌人</t>
+          <t>&gt; 使用非助战凯瑟琳累计部署15个“支援装置”&gt; 3星通关主题曲11-7标准实战环境；必须编入非助战凯瑟琳并上场，且凯瑟琳使用至少2次“战火淬炼”</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="7" t="inlineStr">
         <is>
-          <t>弑君者</t>
+          <t>波卜</t>
         </is>
       </c>
       <c r="B371" s="7" t="inlineStr">
         <is>
-          <t>4-4</t>
+          <t>4-8</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；每次战斗至少部署3次非助战弑君者&gt; 3星通关主题曲4-4；必须编入非助战弑君者并上场，且不编入其他特种干员</t>
+          <t>&gt; 由非助战波卜累计造成30次灼燃爆发&gt; 3星通关主题曲4-8；必须编入非助战波卜并上场，且波卜使用至少2次“此路不通”</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="7" t="inlineStr">
         <is>
-          <t>弑君者</t>
+          <t>维娜·维多利亚</t>
         </is>
       </c>
       <c r="B372" s="7" t="inlineStr">
         <is>
-          <t>4-8</t>
+          <t>9-5</t>
         </is>
       </c>
       <c r="C372" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战弑君者累计使用8次烽烟行刑场&gt; 3星通关主题曲4-8；必须编入非助战弑君者并上场，且使用2次烽烟行刑场</t>
+          <t>&gt; 由非助战维娜·维多利亚累计造成120000点伤害&gt; 3星通关主题曲9-5标准实战环境；必须编入非助战维娜·维多利亚并上场，其他成员仅可编入5名干员</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="7" t="inlineStr">
         <is>
-          <t>忍冬</t>
+          <t>裁度</t>
         </is>
       </c>
       <c r="B373" s="7" t="inlineStr">
         <is>
-          <t>S2-3</t>
+          <t>5-8</t>
         </is>
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>&gt; 由非助战忍冬累计造成80000点伤害&gt; 3星通关主题曲S2-3；必须编入非助战忍冬并上场，且使用忍冬击败至少24名敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战裁度并部署至少2次，且使用裁度击败至少4名敌人&gt; 3星通关主题曲5-8；必须编入非助战裁度并上场，且至少束缚12次敌人</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="7" t="inlineStr">
         <is>
-          <t>荒芜拉普兰德</t>
+          <t>弑君者</t>
         </is>
       </c>
       <c r="B374" s="7" t="inlineStr">
         <is>
-          <t>IS-8</t>
+          <t>4-4</t>
         </is>
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>&gt; 由非助战荒芜拉普兰德累计造成150000点伤害&gt; 3星通关别传IS-8；必须编入非助战荒芜拉普兰德并上场，且荒芜拉普兰德使用至少2次逐猎狂飙或终幕·浩劫</t>
+          <t>&gt; 完成5次战斗；每次战斗至少部署3次非助战弑君者&gt; 3星通关主题曲4-4；必须编入非助战弑君者并上场，且不编入其他特种干员</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="7" t="inlineStr">
         <is>
-          <t>瑰盐</t>
+          <t>弑君者</t>
         </is>
       </c>
       <c r="B375" s="7" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>4-8</t>
         </is>
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战瑰盐累计使用绝妙的长效药呀8次&gt; 3星通关主题曲4-6；必须编入非助战瑰盐并上场，且至少使用1次绝妙的长效药呀</t>
+          <t>&gt; 战斗中非助战弑君者累计使用8次烽烟行刑场&gt; 3星通关主题曲4-8；必须编入非助战弑君者并上场，且使用2次烽烟行刑场</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="7" t="inlineStr">
         <is>
-          <t>引星棘刺</t>
+          <t>忍冬</t>
         </is>
       </c>
       <c r="B376" s="7" t="inlineStr">
         <is>
-          <t>OF-7</t>
+          <t>S2-3</t>
         </is>
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战引星棘刺累计使用20次解构涌潮&gt; 3星通关别传OF-7；必须编入非助战引星棘刺并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 由非助战忍冬累计造成80000点伤害&gt; 3星通关主题曲S2-3；必须编入非助战忍冬并上场，且使用忍冬击败至少24名敌人</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="7" t="inlineStr">
         <is>
-          <t>行箸</t>
+          <t>荒芜拉普兰德</t>
         </is>
       </c>
       <c r="B377" s="7" t="inlineStr">
         <is>
-          <t>3-2</t>
+          <t>IS-8</t>
         </is>
       </c>
       <c r="C377" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战行箸累计使用8次食不厌精&gt; 3星通关主题曲3-2；必须编入非助战行箸并上场，且所有干员不能被击倒</t>
+          <t>&gt; 由非助战荒芜拉普兰德累计造成150000点伤害&gt; 3星通关别传IS-8；必须编入非助战荒芜拉普兰德并上场，且荒芜拉普兰德使用至少2次逐猎狂飙或终幕·浩劫</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="7" t="inlineStr">
         <is>
-          <t>寻澜</t>
+          <t>瑰盐</t>
         </is>
       </c>
       <c r="B378" s="7" t="inlineStr">
         <is>
-          <t>3-5</t>
+          <t>4-6</t>
         </is>
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战寻澜并上场，且使用寻澜歼灭至少3个敌人&gt; 3星通关主题曲3-5；必须编入非助战寻澜并上场，且至少使用2次洞悉</t>
+          <t>&gt; 战斗中非助战瑰盐累计使用绝妙的长效药呀8次&gt; 3星通关主题曲4-6；必须编入非助战瑰盐并上场，且至少使用1次绝妙的长效药呀</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="7" t="inlineStr">
         <is>
-          <t>诺威尔</t>
+          <t>特克诺</t>
         </is>
       </c>
       <c r="B379" s="7" t="inlineStr">
         <is>
-          <t>5-7</t>
+          <t>DH-6</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战诺威尔并上场，且每次战斗至少释放1次生命不息&gt; 3星通关主题曲5-7；必须编入非助战诺威尔并上场，且队伍中不能有其他医疗干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战特克诺并上场，且每次战斗至少释放1次“恣意挥洒”&gt; 3星通关插曲DH-6，必须编入非助战特克诺并上场，其他成员仅可编入7名干员</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="7" t="inlineStr">
         <is>
-          <t>隐德来希</t>
+          <t>引星棘刺</t>
         </is>
       </c>
       <c r="B380" s="7" t="inlineStr">
         <is>
-          <t>10-12</t>
+          <t>OF-7</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战隐德来希累计造成100000点伤害&gt; 3星通关主题曲10-12标准实战环境；必须编入非助战隐德来希并上场，且隐德来希至少使用3次灵与欲的惜别</t>
+          <t>&gt; 战斗中非助战引星棘刺累计使用20次解构涌潮&gt; 3星通关别传OF-7；必须编入非助战引星棘刺并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="7" t="inlineStr">
         <is>
-          <t>钼铅</t>
+          <t>行箸</t>
         </is>
       </c>
       <c r="B381" s="7" t="inlineStr">
         <is>
-          <t>9-6</t>
+          <t>3-2</t>
         </is>
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战钼铅累计部署矿石“杀手”30个&gt; 3星通关主题曲9-6标准实战环境；必须编入非助战钼铅并上场，且使用钼铅至少击败1名深池重甲卫士</t>
+          <t>&gt; 使用非助战行箸累计使用8次食不厌精&gt; 3星通关主题曲3-2；必须编入非助战行箸并上场，且所有干员不能被击倒</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="7" t="inlineStr">
         <is>
-          <t>骋风</t>
+          <t>寻澜</t>
         </is>
       </c>
       <c r="B382" s="7" t="inlineStr">
         <is>
-          <t>SN-2</t>
+          <t>3-5</t>
         </is>
       </c>
       <c r="C382" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战骋风并上场，且每次战斗至少释放1次招无虚发&gt; 3星通关插曲SN-2；必须编入非助战骋风并上场，且使用2次招无虚发</t>
+          <t>&gt; 完成5次战斗；必须编入非助战寻澜并上场，且使用寻澜歼灭至少3个敌人&gt; 3星通关主题曲3-5；必须编入非助战寻澜并上场，且至少使用2次洞悉</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="7" t="inlineStr">
         <is>
-          <t>阿兰娜</t>
+          <t>诺威尔</t>
         </is>
       </c>
       <c r="B383" s="7" t="inlineStr">
         <is>
-          <t>7-14</t>
+          <t>5-7</t>
         </is>
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战阿兰娜累计部署15个“支援装置”&gt; 3星通关主题曲7-14；必须编入非助战阿兰娜并上场，且至少使用2次“万斤顶”</t>
+          <t>&gt; 完成5次战斗；必须编入非助战诺威尔并上场，且每次战斗至少释放1次生命不息&gt; 3星通关主题曲5-7；必须编入非助战诺威尔并上场，且队伍中不能有其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="7" t="inlineStr">
         <is>
-          <t>信仰搅拌机</t>
+          <t>隐德来希</t>
         </is>
       </c>
       <c r="B384" s="7" t="inlineStr">
         <is>
-          <t>14-5</t>
+          <t>10-12</t>
         </is>
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战信仰搅拌机并上场，且每次战斗至少释放1次退休前布道&gt; 3星通关主题曲14-5标准实战环境；必须编入非助战信仰搅拌机并上场，且使用信仰搅拌机歼灭至少10名敌人</t>
+          <t>&gt; 使用非助战隐德来希累计造成100000点伤害&gt; 3星通关主题曲10-12标准实战环境；必须编入非助战隐德来希并上场，且隐德来希至少使用3次灵与欲的惜别</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="7" t="inlineStr">
         <is>
-          <t>蕾缪安</t>
+          <t>钼铅</t>
         </is>
       </c>
       <c r="B385" s="7" t="inlineStr">
         <is>
-          <t>13-13</t>
+          <t>9-6</t>
         </is>
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>&gt; 由非助战蕾缪安累计造成30歼灭数&gt; 3星通关主题曲13-13标准实战环境；必须编入非助战蕾缪安并上场，且蕾缪安歼灭至少2个萨卡兹骸骨鞭笞者</t>
+          <t>&gt; 战斗中非助战钼铅累计部署矿石“杀手”30个&gt; 3星通关主题曲9-6标准实战环境；必须编入非助战钼铅并上场，且使用钼铅至少击败1名深池重甲卫士</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="7" t="inlineStr">
         <is>
+          <t>死芒</t>
+        </is>
+      </c>
+      <c r="B386" s="7" t="inlineStr">
+        <is>
+          <t>4-8</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>&gt; 完成5次战斗；必须编入非助战死芒并上场，且每次战斗至少释放2次“冠死以冕”&gt; 3星通关主题曲4-8，必须编入非助战死芒并上场，其他成员仅可编入辅助干员</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="7" t="inlineStr">
+        <is>
+          <t>骋风</t>
+        </is>
+      </c>
+      <c r="B387" s="7" t="inlineStr">
+        <is>
+          <t>SN-2</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>&gt; 完成5次战斗；必须编入非助战骋风并上场，且每次战斗至少释放1次招无虚发&gt; 3星通关插曲SN-2；必须编入非助战骋风并上场，且使用2次招无虚发</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="7" t="inlineStr">
+        <is>
+          <t>阿兰娜</t>
+        </is>
+      </c>
+      <c r="B388" s="7" t="inlineStr">
+        <is>
+          <t>7-14</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>&gt; 使用非助战阿兰娜累计部署15个“支援装置”&gt; 3星通关主题曲7-14；必须编入非助战阿兰娜并上场，且至少使用2次“万斤顶”</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="7" t="inlineStr">
+        <is>
+          <t>信仰搅拌机</t>
+        </is>
+      </c>
+      <c r="B389" s="7" t="inlineStr">
+        <is>
+          <t>14-5</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>&gt; 完成5次战斗；必须编入非助战信仰搅拌机并上场，且每次战斗至少释放1次退休前布道&gt; 3星通关主题曲14-5标准实战环境；必须编入非助战信仰搅拌机并上场，且使用信仰搅拌机歼灭至少10名敌人</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="7" t="inlineStr">
+        <is>
+          <t>蕾缪安</t>
+        </is>
+      </c>
+      <c r="B390" s="7" t="inlineStr">
+        <is>
+          <t>13-13</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>&gt; 由非助战蕾缪安累计造成30歼灭数&gt; 3星通关主题曲13-13标准实战环境；必须编入非助战蕾缪安并上场，且蕾缪安歼灭至少2个萨卡兹骸骨鞭笞者</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="7" t="inlineStr">
+        <is>
           <t>新约能天使</t>
         </is>
       </c>
-      <c r="B386" s="7" t="inlineStr">
+      <c r="B391" s="7" t="inlineStr">
         <is>
           <t>GA-EX-5</t>
         </is>
       </c>
-      <c r="C386" t="inlineStr">
+      <c r="C391" t="inlineStr">
         <is>
           <t>&gt; 战斗中非助战新约能天使累计使用开火成瘾症8次&gt; 3星通关插曲GA-EX-5；必须编入非助战新约能天使并上场，且使用2次开火成瘾症</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="7" t="inlineStr">
+        <is>
+          <t>酒神</t>
+        </is>
+      </c>
+      <c r="B392" s="7" t="inlineStr">
+        <is>
+          <t>9-6</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>&gt; 使用非助战酒神累计造成60000点神经损伤&gt; 3星通关主题曲9-6标准实战环境，必须编入非助战酒神并上场，且酒神使用至少2次“空剧场”</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
CI: Auto Update Data (#208)
Co-authored-by: ntgmc <ntgmc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Excel/模组任务.xlsx
+++ b/Excel/模组任务.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA394"/>
+  <dimension ref="A1:AA398"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
@@ -478,7 +478,7 @@
     <row r="1">
       <c r="A1" s="7" t="inlineStr">
         <is>
-          <t>更新日期：2025.06.29 13:23:12</t>
+          <t>更新日期：2025.07.11 13:25:31</t>
         </is>
       </c>
     </row>
@@ -4886,51 +4886,51 @@
     <row r="241">
       <c r="A241" s="7" t="inlineStr">
         <is>
-          <t>见行者</t>
+          <t>澄闪</t>
         </is>
       </c>
       <c r="B241" s="7" t="inlineStr">
         <is>
-          <t>GA-EX-1</t>
+          <t>4-7</t>
         </is>
       </c>
       <c r="C241" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战见行者并上场，且每次战斗至少释放2次惊爆射击&gt; 3星通关别传GA-EX-1；必须编入非助战见行者，且本场战斗至少使3个寻路者精锐狙击手坠落地穴</t>
+          <t>&gt; 战斗中非助战澄闪累计使用“澄净闪耀”10次&gt; 3星通关主题曲4-7；必须编入非助战澄闪并上场，其他成员仅可编入5名干员</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="7" t="inlineStr">
         <is>
-          <t>风丸</t>
+          <t>见行者</t>
         </is>
       </c>
       <c r="B242" s="7" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>GA-EX-1</t>
         </is>
       </c>
       <c r="C242" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战风丸累计使用纸艺·双影10次&gt; 3星通关主题曲3-1；必须编入非助战风丸并上场，且使用风丸歼灭至少30名敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战见行者并上场，且每次战斗至少释放2次惊爆射击&gt; 3星通关别传GA-EX-1；必须编入非助战见行者，且本场战斗至少使3个寻路者精锐狙击手坠落地穴</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="7" t="inlineStr">
         <is>
-          <t>菲亚梅塔</t>
+          <t>风丸</t>
         </is>
       </c>
       <c r="B243" s="7" t="inlineStr">
         <is>
-          <t>GA-4</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="C243" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战菲亚梅塔并上场，且使用菲亚梅塔歼灭至少10个敌人&gt; 3星通关别传GA-4；必须编入非助战菲亚梅塔并上场，且队伍中不能有其他狙击干员</t>
+          <t>&gt; 由非助战风丸累计使用纸艺·双影10次&gt; 3星通关主题曲3-1；必须编入非助战风丸并上场，且使用风丸歼灭至少30名敌人</t>
         </is>
       </c>
     </row>
@@ -4942,80 +4942,80 @@
       </c>
       <c r="B244" s="7" t="inlineStr">
         <is>
-          <t>S5-9</t>
+          <t>GA-4</t>
         </is>
       </c>
       <c r="C244" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战菲亚梅塔累计造成180000点伤害&gt; 3星通关主题曲S5-9；必须编入非助战菲亚梅塔并上场，且使用菲亚梅塔造成至少60000点伤害</t>
+          <t>&gt; 完成5次战斗；必须编入非助战菲亚梅塔并上场，且使用菲亚梅塔歼灭至少10个敌人&gt; 3星通关别传GA-4；必须编入非助战菲亚梅塔并上场，且队伍中不能有其他狙击干员</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="7" t="inlineStr">
         <is>
-          <t>褐果</t>
+          <t>菲亚梅塔</t>
         </is>
       </c>
       <c r="B245" s="7" t="inlineStr">
         <is>
-          <t>SV-3</t>
+          <t>S5-9</t>
         </is>
       </c>
       <c r="C245" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战褐果并上场，且每次战斗至少释放1次厚土迸发&gt; 3星通关插曲SV-3；必须编入非助战褐果并上场，且不编入其他医疗干员</t>
+          <t>&gt; 由非助战菲亚梅塔累计造成180000点伤害&gt; 3星通关主题曲S5-9；必须编入非助战菲亚梅塔并上场，且使用菲亚梅塔造成至少60000点伤害</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="7" t="inlineStr">
         <is>
-          <t>海蒂</t>
+          <t>褐果</t>
         </is>
       </c>
       <c r="B246" s="7" t="inlineStr">
         <is>
-          <t>9-7</t>
+          <t>SV-3</t>
         </is>
       </c>
       <c r="C246" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战海蒂累计使用8次“虚构故事·怒士”&gt; 3星通关主题曲9-7标准实战环境；必须编入非助战海蒂并上场，且海蒂使用至少3次“虚构故事·锈城”</t>
+          <t>&gt; 完成5次战斗；必须编入非助战褐果并上场，且每次战斗至少释放1次厚土迸发&gt; 3星通关插曲SV-3；必须编入非助战褐果并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="7" t="inlineStr">
         <is>
-          <t>洛洛</t>
+          <t>海蒂</t>
         </is>
       </c>
       <c r="B247" s="7" t="inlineStr">
         <is>
-          <t>RI-EX-4</t>
+          <t>9-7</t>
         </is>
       </c>
       <c r="C247" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战洛洛累计使用自负此轭10次&gt; 3星通关别传RI-EX-4；必须编入非助战洛洛并上场，且使用洛洛歼灭至少2名提亚卡乌冠军</t>
+          <t>&gt; 战斗中非助战海蒂累计使用8次“虚构故事·怒士”&gt; 3星通关主题曲9-7标准实战环境；必须编入非助战海蒂并上场，且海蒂使用至少3次“虚构故事·锈城”</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="7" t="inlineStr">
         <is>
-          <t>号角</t>
+          <t>洛洛</t>
         </is>
       </c>
       <c r="B248" s="7" t="inlineStr">
         <is>
-          <t>7-15</t>
+          <t>RI-EX-4</t>
         </is>
       </c>
       <c r="C248" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战号角累计使用终极防线10次&gt; 3星通关主题曲7-15；必须编入非助战号角并上场，且使用号角至少歼灭10个敌人</t>
+          <t>&gt; 战斗中非助战洛洛累计使用自负此轭10次&gt; 3星通关别传RI-EX-4；必须编入非助战洛洛并上场，且使用洛洛歼灭至少2名提亚卡乌冠军</t>
         </is>
       </c>
     </row>
@@ -5027,46 +5027,46 @@
       </c>
       <c r="B249" s="7" t="inlineStr">
         <is>
-          <t>9-5</t>
+          <t>7-15</t>
         </is>
       </c>
       <c r="C249" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战号角累计造成100000点伤害&gt; 3星通关主题曲9-5标准实战环境；必须编入非助战号角并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 战斗中非助战号角累计使用终极防线10次&gt; 3星通关主题曲7-15；必须编入非助战号角并上场，且使用号角至少歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="7" t="inlineStr">
         <is>
-          <t>掠风</t>
+          <t>号角</t>
         </is>
       </c>
       <c r="B250" s="7" t="inlineStr">
         <is>
-          <t>11-9</t>
+          <t>9-5</t>
         </is>
       </c>
       <c r="C250" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战掠风累计使用此身为源10次&gt; 3星通关主题曲11-9标准实战环境；必须编入非助战掠风并上场，其他成员仅可编入术师、重装与医疗干员</t>
+          <t>&gt; 由非助战号角累计造成100000点伤害&gt; 3星通关主题曲9-5标准实战环境；必须编入非助战号角并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="7" t="inlineStr">
         <is>
-          <t>流明</t>
+          <t>掠风</t>
         </is>
       </c>
       <c r="B251" s="7" t="inlineStr">
         <is>
-          <t>6-9</t>
+          <t>11-9</t>
         </is>
       </c>
       <c r="C251" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战流明并上场，且每次战斗至少释放2次灯火不灭&gt; 3星通关主题曲6-9；且仅可编入非助战流明1名医疗干员并上场</t>
+          <t>&gt; 战斗中非助战掠风累计使用此身为源10次&gt; 3星通关主题曲11-9标准实战环境；必须编入非助战掠风并上场，其他成员仅可编入术师、重装与医疗干员</t>
         </is>
       </c>
     </row>
@@ -5078,29 +5078,29 @@
       </c>
       <c r="B252" s="7" t="inlineStr">
         <is>
-          <t>OF-5</t>
+          <t>6-9</t>
         </is>
       </c>
       <c r="C252" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战流明累计使用沛霖10次&gt; 3星通关别传OF-5；必须编入非助战流明并上场，且不编入其他医疗干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战流明并上场，且每次战斗至少释放2次灯火不灭&gt; 3星通关主题曲6-9；且仅可编入非助战流明1名医疗干员并上场</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="7" t="inlineStr">
         <is>
-          <t>艾丽妮</t>
+          <t>流明</t>
         </is>
       </c>
       <c r="B253" s="7" t="inlineStr">
         <is>
-          <t>SV-EX-1</t>
+          <t>OF-5</t>
         </is>
       </c>
       <c r="C253" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战艾丽妮累计造成100000点伤害&gt; 3星通关插曲SV-EX-1；必须编入非助战艾丽妮并上场，且使用2次判决</t>
+          <t>&gt; 战斗中非助战流明累计使用沛霖10次&gt; 3星通关别传OF-5；必须编入非助战流明并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
@@ -5112,29 +5112,29 @@
       </c>
       <c r="B254" s="7" t="inlineStr">
         <is>
-          <t>SV-4</t>
+          <t>SV-EX-1</t>
         </is>
       </c>
       <c r="C254" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战艾丽妮使用技能累计造成50歼灭数&gt; 3星通关插曲SV-4；必须编入非助战艾丽妮并上场，且使用艾丽妮歼灭15个敌人</t>
+          <t>&gt; 由非助战艾丽妮累计造成100000点伤害&gt; 3星通关插曲SV-EX-1；必须编入非助战艾丽妮并上场，且使用2次判决</t>
         </is>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="7" t="inlineStr">
         <is>
-          <t>归溟幽灵鲨</t>
+          <t>艾丽妮</t>
         </is>
       </c>
       <c r="B255" s="7" t="inlineStr">
         <is>
-          <t>SV-EX-1</t>
+          <t>SV-4</t>
         </is>
       </c>
       <c r="C255" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战归溟幽灵鲨累计造成30歼灭数&gt; 3星通关插曲SV-EX-1；必须编入非助战归溟幽灵鲨并上场，且使用归溟幽灵鲨歼灭至少1个囊海爬行者</t>
+          <t>&gt; 由非助战艾丽妮使用技能累计造成50歼灭数&gt; 3星通关插曲SV-4；必须编入非助战艾丽妮并上场，且使用艾丽妮歼灭15个敌人</t>
         </is>
       </c>
     </row>
@@ -5146,63 +5146,63 @@
       </c>
       <c r="B256" s="7" t="inlineStr">
         <is>
-          <t>S4-1</t>
+          <t>SV-EX-1</t>
         </is>
       </c>
       <c r="C256" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战归溟幽灵鲨并上场，且每次战斗至少释放1次生存的重压&gt; 3星通关主题曲S4-1；必须编入非助战归溟幽灵鲨并上场，且使用归溟幽灵鲨歼灭10个敌人</t>
+          <t>&gt; 由非助战归溟幽灵鲨累计造成30歼灭数&gt; 3星通关插曲SV-EX-1；必须编入非助战归溟幽灵鲨并上场，且使用归溟幽灵鲨歼灭至少1个囊海爬行者</t>
         </is>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="7" t="inlineStr">
         <is>
-          <t>埃拉托</t>
+          <t>归溟幽灵鲨</t>
         </is>
       </c>
       <c r="B257" s="7" t="inlineStr">
         <is>
-          <t>S5-9</t>
+          <t>S4-1</t>
         </is>
       </c>
       <c r="C257" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战埃拉托累计使用英雄赞歌5次&gt; 3星通关主题曲S5-9；必须编入非助战埃拉托并上场，其他成员不可编入狙击干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战归溟幽灵鲨并上场，且每次战斗至少释放1次生存的重压&gt; 3星通关主题曲S4-1；必须编入非助战归溟幽灵鲨并上场，且使用归溟幽灵鲨歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="7" t="inlineStr">
         <is>
-          <t>濯尘芙蓉</t>
+          <t>埃拉托</t>
         </is>
       </c>
       <c r="B258" s="7" t="inlineStr">
         <is>
-          <t>LE-4</t>
+          <t>S5-9</t>
         </is>
       </c>
       <c r="C258" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战濯尘芙蓉累计使用抚业之触10次&gt; 3星通关别传LE-4；必须编入非助战濯尘芙蓉并上场，且至少使用2次抚业之触</t>
+          <t>&gt; 战斗中非助战埃拉托累计使用英雄赞歌5次&gt; 3星通关主题曲S5-9；必须编入非助战埃拉托并上场，其他成员不可编入狙击干员</t>
         </is>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="7" t="inlineStr">
         <is>
-          <t>黑键</t>
+          <t>濯尘芙蓉</t>
         </is>
       </c>
       <c r="B259" s="7" t="inlineStr">
         <is>
-          <t>3-7</t>
+          <t>LE-4</t>
         </is>
       </c>
       <c r="C259" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战黑键累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲3-7；必须编入非助战黑键并上场，且使用黑键歼灭至少1个重装防御组长</t>
+          <t>&gt; 战斗中非助战濯尘芙蓉累计使用抚业之触10次&gt; 3星通关别传LE-4；必须编入非助战濯尘芙蓉并上场，且至少使用2次抚业之触</t>
         </is>
       </c>
     </row>
@@ -5214,12 +5214,12 @@
       </c>
       <c r="B260" s="7" t="inlineStr">
         <is>
-          <t>3-6</t>
+          <t>3-7</t>
         </is>
       </c>
       <c r="C260" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战黑键并上场，且使用黑键歼灭至少6个敌人&gt; 3星通关主题曲3-6；必须编入非助战黑键并上场，且使用黑键歼灭屠宰老手</t>
+          <t>&gt; 由非助战黑键累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲3-7；必须编入非助战黑键并上场，且使用黑键歼灭至少1个重装防御组长</t>
         </is>
       </c>
     </row>
@@ -5231,63 +5231,63 @@
       </c>
       <c r="B261" s="7" t="inlineStr">
         <is>
-          <t>11-12</t>
+          <t>3-6</t>
         </is>
       </c>
       <c r="C261" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战黑键累计使用寂静之声10次&gt; 3星通关主题曲11-12标准实战环境；必须编入非助战黑键并上场，且使用黑键歼灭至少2名伦蒂尼姆城防自行炮</t>
+          <t>&gt; 完成5次战斗；必须编入非助战黑键并上场，且使用黑键歼灭至少6个敌人&gt; 3星通关主题曲3-6；必须编入非助战黑键并上场，且使用黑键歼灭屠宰老手</t>
         </is>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="7" t="inlineStr">
         <is>
-          <t>星源</t>
+          <t>黑键</t>
         </is>
       </c>
       <c r="B262" s="7" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>11-12</t>
         </is>
       </c>
       <c r="C262" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战星源累计造成40歼灭数&gt; 3星通关主题曲4-3；必须编入非助战星源并上场，其他成员仅可编入重装干员</t>
+          <t>&gt; 战斗中非助战黑键累计使用寂静之声10次&gt; 3星通关主题曲11-12标准实战环境；必须编入非助战黑键并上场，且使用黑键歼灭至少2名伦蒂尼姆城防自行炮</t>
         </is>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="7" t="inlineStr">
         <is>
-          <t>承曦格雷伊</t>
+          <t>星源</t>
         </is>
       </c>
       <c r="B263" s="7" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C263" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战承曦格雷伊累计使用晨曦信标10次&gt; 3星通关主题曲1-3；必须编入非助战承曦格雷伊并上场，其他成员仅可编入先锋干员</t>
+          <t>&gt; 由非助战星源累计造成40歼灭数&gt; 3星通关主题曲4-3；必须编入非助战星源并上场，其他成员仅可编入重装干员</t>
         </is>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="7" t="inlineStr">
         <is>
-          <t>多萝西</t>
+          <t>承曦格雷伊</t>
         </is>
       </c>
       <c r="B264" s="7" t="inlineStr">
         <is>
-          <t>MB-EX-1</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="C264" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战多萝西累计造成120000点伤害&gt; 3星通关插曲MB-EX-1，必须编入非助战多萝西并上场，其他成员仅可编入近卫干员</t>
+          <t>&gt; 战斗中非助战承曦格雷伊累计使用晨曦信标10次&gt; 3星通关主题曲1-3；必须编入非助战承曦格雷伊并上场，其他成员仅可编入先锋干员</t>
         </is>
       </c>
     </row>
@@ -5299,63 +5299,63 @@
       </c>
       <c r="B265" s="7" t="inlineStr">
         <is>
-          <t>4-5</t>
+          <t>MB-EX-1</t>
         </is>
       </c>
       <c r="C265" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战多萝西累计部署共振装置50个&gt; 3星通关主题曲4-5；必须编入非助战多萝西并上场，其他成员仅可编入3名干员</t>
+          <t>&gt; 由非助战多萝西累计造成120000点伤害&gt; 3星通关插曲MB-EX-1，必须编入非助战多萝西并上场，其他成员仅可编入近卫干员</t>
         </is>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="7" t="inlineStr">
         <is>
-          <t>至简</t>
+          <t>多萝西</t>
         </is>
       </c>
       <c r="B266" s="7" t="inlineStr">
         <is>
-          <t>IC-8</t>
+          <t>4-5</t>
         </is>
       </c>
       <c r="C266" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战至简累计使用神工意匠20次&gt; 3星通关别传IC-8；必须编入非助战至简并上场，且使用至简歼灭至少2名蜜酿级醒酒助手</t>
+          <t>&gt; 战斗中非助战多萝西累计部署共振装置50个&gt; 3星通关主题曲4-5；必须编入非助战多萝西并上场，其他成员仅可编入3名干员</t>
         </is>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="7" t="inlineStr">
         <is>
-          <t>晓歌</t>
+          <t>至简</t>
         </is>
       </c>
       <c r="B267" s="7" t="inlineStr">
         <is>
-          <t>5-3</t>
+          <t>IC-8</t>
         </is>
       </c>
       <c r="C267" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中累计部署非助战晓歌12次&gt; 3星通关主题曲5-3；必须编入非助战晓歌并上场，且使用晓歌歼灭至少3个特战术师或特战术师组长</t>
+          <t>&gt; 战斗中非助战至简累计使用神工意匠20次&gt; 3星通关别传IC-8；必须编入非助战至简并上场，且使用至简歼灭至少2名蜜酿级醒酒助手</t>
         </is>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="7" t="inlineStr">
         <is>
-          <t>鸿雪</t>
+          <t>晓歌</t>
         </is>
       </c>
       <c r="B268" s="7" t="inlineStr">
         <is>
-          <t>9-7</t>
+          <t>5-3</t>
         </is>
       </c>
       <c r="C268" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战鸿雪并上场，且每次战斗至少释放1次锐笔速写&gt; 3星通关主题曲9-7标准实战环境，必须编入非助战鸿雪并上场，且使用鸿雪歼灭至少10名敌人，其中包括至少1个深池重甲卫士</t>
+          <t>&gt; 战斗中累计部署非助战晓歌12次&gt; 3星通关主题曲5-3；必须编入非助战晓歌并上场，且使用晓歌歼灭至少3个特战术师或特战术师组长</t>
         </is>
       </c>
     </row>
@@ -5367,716 +5367,716 @@
       </c>
       <c r="B269" s="7" t="inlineStr">
         <is>
-          <t>2-10</t>
+          <t>9-7</t>
         </is>
       </c>
       <c r="C269" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中累计部署非助战鸿雪的“打字机”10次&gt; 3星通关主题曲2-10；必须编入非助战鸿雪并上场，且使用鸿雪或“打字机”歼灭碎骨</t>
+          <t>&gt; 完成5次战斗；必须编入非助战鸿雪并上场，且每次战斗至少释放1次锐笔速写&gt; 3星通关主题曲9-7标准实战环境，必须编入非助战鸿雪并上场，且使用鸿雪歼灭至少10名敌人，其中包括至少1个深池重甲卫士</t>
         </is>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="7" t="inlineStr">
         <is>
-          <t>百炼嘉维尔</t>
+          <t>鸿雪</t>
         </is>
       </c>
       <c r="B270" s="7" t="inlineStr">
         <is>
-          <t>9-2</t>
+          <t>2-10</t>
         </is>
       </c>
       <c r="C270" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战百炼嘉维尔累计使用链锯强袭10次&gt; 3星通关主题曲9-2标准实战环境；必须编入非助战百炼嘉维尔并上场，且使用百炼嘉维尔至少歼灭15个敌人</t>
+          <t>&gt; 战斗中累计部署非助战鸿雪的“打字机”10次&gt; 3星通关主题曲2-10；必须编入非助战鸿雪并上场，且使用鸿雪或“打字机”歼灭碎骨</t>
         </is>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="7" t="inlineStr">
         <is>
-          <t>但书</t>
+          <t>百炼嘉维尔</t>
         </is>
       </c>
       <c r="B271" s="7" t="inlineStr">
         <is>
-          <t>4-7</t>
+          <t>9-2</t>
         </is>
       </c>
       <c r="C271" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战但书累计使用致胜立论14次&gt; 3星通关主题曲4-7；必须编入非助战但书并上场，且使用但书至少歼灭3只高能源石虫</t>
+          <t>&gt; 战斗中非助战百炼嘉维尔累计使用链锯强袭10次&gt; 3星通关主题曲9-2标准实战环境；必须编入非助战百炼嘉维尔并上场，且使用百炼嘉维尔至少歼灭15个敌人</t>
         </is>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="7" t="inlineStr">
         <is>
-          <t>玛恩纳</t>
+          <t>百炼嘉维尔</t>
         </is>
       </c>
       <c r="B272" s="7" t="inlineStr">
         <is>
-          <t>11-15</t>
+          <t>RI-9</t>
         </is>
       </c>
       <c r="C272" s="9" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战玛恩纳累计造成120000点伤害&gt; 3星通关主题曲11-15标准实战环境；必须编入非助战玛恩纳并上场，且使用2次未照耀的荣光</t>
+          <t>&gt; 由非助战百炼嘉维尔累计造成40歼灭数&gt; 3星通关插曲RI-9；必须编入非助战百炼嘉维尔并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="7" t="inlineStr">
         <is>
-          <t>罗小黑</t>
+          <t>但书</t>
         </is>
       </c>
       <c r="B273" s="7" t="inlineStr">
         <is>
-          <t>IW-4</t>
+          <t>4-7</t>
         </is>
       </c>
       <c r="C273" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战罗小黑并上场，且每次战斗至少释放1次碎金为刃&gt; 3星通关别传IW-4；必须编入非助战罗小黑并上场，其他成员仅可编入6名干员</t>
+          <t>&gt; 战斗中非助战但书累计使用致胜立论14次&gt; 3星通关主题曲4-7；必须编入非助战但书并上场，且使用但书至少歼灭3只高能源石虫</t>
         </is>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="7" t="inlineStr">
         <is>
-          <t>海沫</t>
+          <t>玛恩纳</t>
         </is>
       </c>
       <c r="B274" s="7" t="inlineStr">
         <is>
-          <t>SN-2</t>
+          <t>11-15</t>
         </is>
       </c>
       <c r="C274" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战海沫并上场，且使用海沫造成至少12000点伤害&gt; 3星通关插曲SN-2；必须携带并部署非助战海沫，其他成员仅可编入2名干员</t>
+          <t>&gt; 使用非助战玛恩纳累计造成120000点伤害&gt; 3星通关主题曲11-15标准实战环境；必须编入非助战玛恩纳并上场，且使用2次未照耀的荣光</t>
         </is>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="7" t="inlineStr">
         <is>
-          <t>铅踝</t>
+          <t>罗小黑</t>
         </is>
       </c>
       <c r="B275" s="7" t="inlineStr">
         <is>
-          <t>S3-5</t>
+          <t>IW-4</t>
         </is>
       </c>
       <c r="C275" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战铅踝累计造成30歼灭数&gt; 3星通关主题曲S3-5；必须编入非助战铅踝并上场，且使用铅踝歼灭至少2个隐形弩手</t>
+          <t>&gt; 完成5次战斗；必须编入非助战罗小黑并上场，且每次战斗至少释放1次碎金为刃&gt; 3星通关别传IW-4；必须编入非助战罗小黑并上场，其他成员仅可编入6名干员</t>
         </is>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="7" t="inlineStr">
         <is>
-          <t>达格达</t>
+          <t>海沫</t>
         </is>
       </c>
       <c r="B276" s="7" t="inlineStr">
         <is>
-          <t>11-5</t>
+          <t>SN-2</t>
         </is>
       </c>
       <c r="C276" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战达格达累计造成30歼灭数&gt; 3星通关主题曲11-5标准实战环境；必须编入非助战达格达并上场，且使用达格达至少歼灭10个敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战海沫并上场，且使用海沫造成至少12000点伤害&gt; 3星通关插曲SN-2；必须携带并部署非助战海沫，其他成员仅可编入2名干员</t>
         </is>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="7" t="inlineStr">
         <is>
-          <t>白铁</t>
+          <t>铅踝</t>
         </is>
       </c>
       <c r="B277" s="7" t="inlineStr">
         <is>
-          <t>11-6</t>
+          <t>S3-5</t>
         </is>
       </c>
       <c r="C277" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战白铁累计部署支援装置25个&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战白铁并上场，且使用白铁或白铁的支援装置歼灭至少15名萨卡兹枯朽战士</t>
+          <t>&gt; 由非助战铅踝累计造成30歼灭数&gt; 3星通关主题曲S3-5；必须编入非助战铅踝并上场，且使用铅踝歼灭至少2个隐形弩手</t>
         </is>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="7" t="inlineStr">
         <is>
-          <t>白铁</t>
+          <t>达格达</t>
         </is>
       </c>
       <c r="B278" s="7" t="inlineStr">
         <is>
-          <t>9-6</t>
+          <t>11-5</t>
         </is>
       </c>
       <c r="C278" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战白铁累计使用8次“铁钳号·原型机”&gt; 3星通关主题曲9-6标准实战环境；必须编入非助战白铁并上场，且使用白铁至少歼灭10个敌人</t>
+          <t>&gt; 由非助战达格达累计造成30歼灭数&gt; 3星通关主题曲11-5标准实战环境；必须编入非助战达格达并上场，且使用达格达至少歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="7" t="inlineStr">
         <is>
-          <t>石英</t>
+          <t>白铁</t>
         </is>
       </c>
       <c r="B279" s="7" t="inlineStr">
         <is>
-          <t>DH-4</t>
+          <t>11-6</t>
         </is>
       </c>
       <c r="C279" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成3次战斗；必须编入非助战石英并上场，且每次战斗至少释放1次全力相搏&gt; 3星通关别传DH-4；必须编入非助战石英并上场，并使用石英至少击败2名控潮术师</t>
+          <t>&gt; 战斗中非助战白铁累计部署支援装置25个&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战白铁并上场，且使用白铁或白铁的支援装置歼灭至少15名萨卡兹枯朽战士</t>
         </is>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="7" t="inlineStr">
         <is>
-          <t>雪绒</t>
+          <t>白铁</t>
         </is>
       </c>
       <c r="B280" s="7" t="inlineStr">
         <is>
-          <t>2-3</t>
+          <t>9-6</t>
         </is>
       </c>
       <c r="C280" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战雪绒累计使用坠雪10次&gt; 3星通关主题曲2-3；必须编入非助战雪绒并上场，且使用雪绒歼灭至少2名重装防御者</t>
+          <t>&gt; 战斗中非助战白铁累计使用8次“铁钳号·原型机”&gt; 3星通关主题曲9-6标准实战环境；必须编入非助战白铁并上场，且使用白铁至少歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="7" t="inlineStr">
         <is>
-          <t>子月</t>
+          <t>石英</t>
         </is>
       </c>
       <c r="B281" s="7" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>DH-4</t>
         </is>
       </c>
       <c r="C281" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战子月累计造成30歼灭数&gt; 3星通关主题曲2-5；必须编入非助战子月并上场，且使用子月歼灭至少2个高阶术师</t>
+          <t>&gt; 完成3次战斗；必须编入非助战石英并上场，且每次战斗至少释放1次全力相搏&gt; 3星通关别传DH-4；必须编入非助战石英并上场，并使用石英至少击败2名控潮术师</t>
         </is>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="7" t="inlineStr">
         <is>
-          <t>伺夜</t>
+          <t>雪绒</t>
         </is>
       </c>
       <c r="B282" s="7" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="C282" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战伺夜并上场，且每次战斗至少释放1次领袖的尊严&gt; 3星通关主题曲3-8；必须编入非助战伺夜并上场，且使用伺夜歼灭碎骨</t>
+          <t>&gt; 战斗中非助战雪绒累计使用坠雪10次&gt; 3星通关主题曲2-3；必须编入非助战雪绒并上场，且使用雪绒歼灭至少2名重装防御者</t>
         </is>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="7" t="inlineStr">
         <is>
-          <t>伺夜</t>
+          <t>子月</t>
         </is>
       </c>
       <c r="B283" s="7" t="inlineStr">
         <is>
-          <t>IS-6</t>
+          <t>2-5</t>
         </is>
       </c>
       <c r="C283" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战伺夜，并确定第一位部署的干员是伺夜&gt; 3星通关别传IS-6；必须编入非助战伺夜并上场，且至少使用3次领袖的尊严</t>
+          <t>&gt; 由非助战子月累计造成30歼灭数&gt; 3星通关主题曲2-5；必须编入非助战子月并上场，且使用子月歼灭至少2个高阶术师</t>
         </is>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="7" t="inlineStr">
         <is>
-          <t>斥罪</t>
+          <t>伺夜</t>
         </is>
       </c>
       <c r="B284" s="7" t="inlineStr">
         <is>
-          <t>CB-4</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C284" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战斥罪累计造成40歼灭数&gt; 3星通关别传CB-4；必须携带并部署非助战斥罪，其他成员仅可编入4名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战伺夜并上场，且每次战斗至少释放1次领袖的尊严&gt; 3星通关主题曲3-8；必须编入非助战伺夜并上场，且使用伺夜歼灭碎骨</t>
         </is>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="7" t="inlineStr">
         <is>
-          <t>斥罪</t>
+          <t>伺夜</t>
         </is>
       </c>
       <c r="B285" s="7" t="inlineStr">
         <is>
-          <t>IS-7</t>
+          <t>IS-6</t>
         </is>
       </c>
       <c r="C285" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战斥罪累计使用披荆斩棘5次&gt; 3星通关别传IS-7；必须编入非助战斥罪并上场，且不编入其他医疗干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战伺夜，并确定第一位部署的干员是伺夜&gt; 3星通关别传IS-6；必须编入非助战伺夜并上场，且至少使用3次领袖的尊严</t>
         </is>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="7" t="inlineStr">
         <is>
-          <t>缄默德克萨斯</t>
+          <t>斥罪</t>
         </is>
       </c>
       <c r="B286" s="7" t="inlineStr">
         <is>
-          <t>CB-8</t>
+          <t>CB-4</t>
         </is>
       </c>
       <c r="C286" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战缄默德克萨斯累计歼灭10个精英或领袖敌人&gt; 3星通关别传CB-8；必须编入非助战缄默德克萨斯并上场，且使用缄默德克萨斯歼灭至少2个灰尾</t>
+          <t>&gt; 由非助战斥罪累计造成40歼灭数&gt; 3星通关别传CB-4；必须携带并部署非助战斥罪，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="7" t="inlineStr">
         <is>
-          <t>谜图</t>
+          <t>斥罪</t>
         </is>
       </c>
       <c r="B287" s="7" t="inlineStr">
         <is>
-          <t>9-4</t>
+          <t>IS-7</t>
         </is>
       </c>
       <c r="C287" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战谜图并上场，且使用谜图歼灭至少3个敌人&gt; 3星通关主题曲9-4标准实战环境；必须编入非助战谜图并上场，其他成员不可编入先锋干员</t>
+          <t>&gt; 战斗中非助战斥罪累计使用披荆斩棘5次&gt; 3星通关别传IS-7；必须编入非助战斥罪并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="7" t="inlineStr">
         <is>
-          <t>和弦</t>
+          <t>缄默德克萨斯</t>
         </is>
       </c>
       <c r="B288" s="7" t="inlineStr">
         <is>
-          <t>6-5</t>
+          <t>CB-8</t>
         </is>
       </c>
       <c r="C288" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战和弦并上场，且每次战斗至少释放一次沉溺之灾&gt; 3星通关主题曲6-5；必须编入非助战和弦并上场，且使用和弦歼灭至少2个宿主重装士兵</t>
+          <t>&gt; 由非助战缄默德克萨斯累计歼灭10个精英或领袖敌人&gt; 3星通关别传CB-8；必须编入非助战缄默德克萨斯并上场，且使用缄默德克萨斯歼灭至少2个灰尾</t>
         </is>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="7" t="inlineStr">
         <is>
-          <t>焰影苇草</t>
+          <t>谜图</t>
         </is>
       </c>
       <c r="B289" s="7" t="inlineStr">
         <is>
-          <t>11-6</t>
+          <t>9-4</t>
         </is>
       </c>
       <c r="C289" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战焰影苇草累计使用枯荣共息10次&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战焰影苇草并上场，且使用焰影苇草至少歼灭40个敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战谜图并上场，且使用谜图歼灭至少3个敌人&gt; 3星通关主题曲9-4标准实战环境；必须编入非助战谜图并上场，其他成员不可编入先锋干员</t>
         </is>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="7" t="inlineStr">
         <is>
-          <t>截云</t>
+          <t>和弦</t>
         </is>
       </c>
       <c r="B290" s="7" t="inlineStr">
         <is>
-          <t>S2-2</t>
+          <t>6-5</t>
         </is>
       </c>
       <c r="C290" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战截云累计造成100000点伤害&gt; 3星通关主题曲S2-2；必须编入非助战截云并上场，且使用截云至少歼灭10名敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战和弦并上场，且每次战斗至少释放一次沉溺之灾&gt; 3星通关主题曲6-5；必须编入非助战和弦并上场，且使用和弦歼灭至少2个宿主重装士兵</t>
         </is>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="7" t="inlineStr">
         <is>
-          <t>火哨</t>
+          <t>焰影苇草</t>
         </is>
       </c>
       <c r="B291" s="7" t="inlineStr">
         <is>
-          <t>S4-6</t>
+          <t>11-6</t>
         </is>
       </c>
       <c r="C291" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战火哨累计使用焦土8次&gt; 3星通关主题曲S4-6；必须携带并部署非助战火哨，其他成员仅可编入远程位干员</t>
+          <t>&gt; 战斗中非助战焰影苇草累计使用枯荣共息10次&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战焰影苇草并上场，且使用焰影苇草至少歼灭40个敌人</t>
         </is>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="7" t="inlineStr">
         <is>
-          <t>林</t>
+          <t>截云</t>
         </is>
       </c>
       <c r="B292" s="7" t="inlineStr">
         <is>
-          <t>11-6</t>
+          <t>S2-2</t>
         </is>
       </c>
       <c r="C292" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战林累计歼灭80个敌人&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战林并上场，且不编入重装干员</t>
+          <t>&gt; 由非助战截云累计造成100000点伤害&gt; 3星通关主题曲S2-2；必须编入非助战截云并上场，且使用截云至少歼灭10名敌人</t>
         </is>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="7" t="inlineStr">
         <is>
-          <t>林</t>
+          <t>火哨</t>
         </is>
       </c>
       <c r="B293" s="7" t="inlineStr">
         <is>
-          <t>6-5</t>
+          <t>S4-6</t>
         </is>
       </c>
       <c r="C293" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战林并上场，且每次战斗至少释放1次流光乍裂&gt; 3星通关主题曲6-5；必须携带且部署非助战林，且至少释放3次流光乍裂</t>
+          <t>&gt; 战斗中非助战火哨累计使用焦土8次&gt; 3星通关主题曲S4-6；必须携带并部署非助战火哨，其他成员仅可编入远程位干员</t>
         </is>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="7" t="inlineStr">
         <is>
-          <t>重岳</t>
+          <t>林</t>
         </is>
       </c>
       <c r="B294" s="7" t="inlineStr">
         <is>
-          <t>WB-7</t>
+          <t>11-6</t>
         </is>
       </c>
       <c r="C294" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战重岳累计造成120000点伤害&gt; 3星通关别传WB-7；必须携带并部署非助战重岳，其他成员仅可编入4名干员</t>
+          <t>&gt; 由非助战林累计歼灭80个敌人&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战林并上场，且不编入重装干员</t>
         </is>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="7" t="inlineStr">
         <is>
-          <t>重岳</t>
+          <t>林</t>
         </is>
       </c>
       <c r="B295" s="7" t="inlineStr">
         <is>
-          <t>GA-5</t>
+          <t>6-5</t>
         </is>
       </c>
       <c r="C295" s="9" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战重岳累计使用50次我无&gt; 3星通关别传GA-5；必须携带且部署非助战重岳，其他成员仅可编入4名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战林并上场，且每次战斗至少释放1次流光乍裂&gt; 3星通关主题曲6-5；必须携带且部署非助战林，且至少释放3次流光乍裂</t>
         </is>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="7" t="inlineStr">
         <is>
-          <t>铎铃</t>
+          <t>重岳</t>
         </is>
       </c>
       <c r="B296" s="7" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>WB-7</t>
         </is>
       </c>
       <c r="C296" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战铎铃累计使用乡心无改6次&gt; 3星通关主题曲2-1；必须编入非助战铎铃并上场，且使用3次乡心无改</t>
+          <t>&gt; 由非助战重岳累计造成120000点伤害&gt; 3星通关别传WB-7；必须携带并部署非助战重岳，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="7" t="inlineStr">
         <is>
-          <t>仇白</t>
+          <t>重岳</t>
         </is>
       </c>
       <c r="B297" s="7" t="inlineStr">
         <is>
-          <t>WB-7</t>
+          <t>GA-5</t>
         </is>
       </c>
       <c r="C297" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战仇白累计造成40歼灭数&gt; 3星通关别传WB-7；必须编入非助战仇白并上场，并使用仇白至少击败3名“破坚”</t>
+          <t>&gt; 使用非助战重岳累计使用50次我无&gt; 3星通关别传GA-5；必须携带且部署非助战重岳，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="7" t="inlineStr">
         <is>
-          <t>火龙S黑角</t>
+          <t>铎铃</t>
         </is>
       </c>
       <c r="B298" s="7" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="C298" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战火龙S黑角累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲3-8；必须编入非助战火龙S黑角并上场，且使用火龙S黑角歼灭碎骨</t>
+          <t>&gt; 战斗中非助战铎铃累计使用乡心无改6次&gt; 3星通关主题曲2-1；必须编入非助战铎铃并上场，且使用3次乡心无改</t>
         </is>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="7" t="inlineStr">
         <is>
-          <t>麒麟R夜刀</t>
+          <t>仇白</t>
         </is>
       </c>
       <c r="B299" s="7" t="inlineStr">
         <is>
-          <t>3-7</t>
+          <t>WB-7</t>
         </is>
       </c>
       <c r="C299" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；每次战斗至少部署3次非助战的麒麟R夜刀&gt; 3星通关主题曲3-7；必须编入非助战麒麟R夜刀并上场，且使用麒麟R夜刀歼灭至少2名炮手</t>
+          <t>&gt; 由非助战仇白累计造成40歼灭数&gt; 3星通关别传WB-7；必须编入非助战仇白并上场，并使用仇白至少击败3名“破坚”</t>
         </is>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="7" t="inlineStr">
         <is>
-          <t>休谟斯</t>
+          <t>火龙S黑角</t>
         </is>
       </c>
       <c r="B300" s="7" t="inlineStr">
         <is>
-          <t>7-8</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C300" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战休谟斯并上场，且每次战斗至少释放1次高效处理&gt; 3星通关主题曲7-8；必须编入非助战休谟斯并上场，其他成员仅可编入近战位干员</t>
+          <t>&gt; 由非助战火龙S黑角累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲3-8；必须编入非助战火龙S黑角并上场，且使用火龙S黑角歼灭碎骨</t>
         </is>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="7" t="inlineStr">
         <is>
-          <t>摩根</t>
+          <t>麒麟R夜刀</t>
         </is>
       </c>
       <c r="B301" s="7" t="inlineStr">
         <is>
-          <t>4-5</t>
+          <t>3-7</t>
         </is>
       </c>
       <c r="C301" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战摩根累计造成80000点伤害&gt; 3星通关主题曲4-5，必须编入非助战摩根并上场，且使用摩根至少歼灭10名敌人</t>
+          <t>&gt; 完成5次战斗；每次战斗至少部署3次非助战的麒麟R夜刀&gt; 3星通关主题曲3-7；必须编入非助战麒麟R夜刀并上场，且使用麒麟R夜刀歼灭至少2名炮手</t>
         </is>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="7" t="inlineStr">
         <is>
-          <t>洋灰</t>
+          <t>休谟斯</t>
         </is>
       </c>
       <c r="B302" s="7" t="inlineStr">
         <is>
-          <t>IW-EX-6</t>
+          <t>7-8</t>
         </is>
       </c>
       <c r="C302" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战洋灰并上场，且每次战斗至少释放1次结构加固&gt; 3星通关别传IW-EX-6，必须编入非助战洋灰并上场，且不编入其他重装干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战休谟斯并上场，且每次战斗至少释放1次高效处理&gt; 3星通关主题曲7-8；必须编入非助战休谟斯并上场，其他成员仅可编入近战位干员</t>
         </is>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="7" t="inlineStr">
         <is>
-          <t>伊内丝</t>
+          <t>摩根</t>
         </is>
       </c>
       <c r="B303" s="7" t="inlineStr">
         <is>
-          <t>12-12</t>
+          <t>4-5</t>
         </is>
       </c>
       <c r="C303" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中累计部署非助战伊内丝12次&gt; 3星通关主题曲12-12标准实战环境；必须编入非助战伊内丝并上场，且至少使用3次暗夜无明</t>
+          <t>&gt; 由非助战摩根累计造成80000点伤害&gt; 3星通关主题曲4-5，必须编入非助战摩根并上场，且使用摩根至少歼灭10名敌人</t>
         </is>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="7" t="inlineStr">
         <is>
-          <t>玫拉</t>
+          <t>洋灰</t>
         </is>
       </c>
       <c r="B304" s="7" t="inlineStr">
         <is>
-          <t>S3-5</t>
+          <t>IW-EX-6</t>
         </is>
       </c>
       <c r="C304" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战玫拉并上场，且每次战斗至少释放1次临界爆发&gt; 3星通关主题曲S3-5；必须编入非助战玫拉并上场，其他成员仅可编入6名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战洋灰并上场，且每次战斗至少释放1次结构加固&gt; 3星通关别传IW-EX-6，必须编入非助战洋灰并上场，且不编入其他重装干员</t>
         </is>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="7" t="inlineStr">
         <is>
-          <t>淬羽赫默</t>
+          <t>伊内丝</t>
         </is>
       </c>
       <c r="B305" s="7" t="inlineStr">
         <is>
-          <t>6-3</t>
+          <t>12-12</t>
         </is>
       </c>
       <c r="C305" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战淬羽赫默累计使用无畏者协议8次&gt; 3星通关主题曲6-3；必须编入非助战淬羽赫默并上场，且所有干员不被击倒</t>
+          <t>&gt; 战斗中累计部署非助战伊内丝12次&gt; 3星通关主题曲12-12标准实战环境；必须编入非助战伊内丝并上场，且至少使用3次暗夜无明</t>
         </is>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="7" t="inlineStr">
         <is>
-          <t>淬羽赫默</t>
+          <t>玫拉</t>
         </is>
       </c>
       <c r="B306" s="7" t="inlineStr">
         <is>
-          <t>WB-5</t>
+          <t>S3-5</t>
         </is>
       </c>
       <c r="C306" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战淬羽赫默并上场，且每次战斗至少释放1次无畏者协议&gt; 3星通关插曲WB-5；必须编入非助战淬羽赫默并上场，且所有干员不被击倒</t>
+          <t>&gt; 完成5次战斗；必须编入非助战玫拉并上场，且每次战斗至少释放1次临界爆发&gt; 3星通关主题曲S3-5；必须编入非助战玫拉并上场，其他成员仅可编入6名干员</t>
         </is>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="7" t="inlineStr">
         <is>
-          <t>霍尔海雅</t>
+          <t>淬羽赫默</t>
         </is>
       </c>
       <c r="B307" s="7" t="inlineStr">
         <is>
-          <t>OF-7</t>
+          <t>6-3</t>
         </is>
       </c>
       <c r="C307" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战霍尔海雅累计造成120000点伤害&gt; 3星通关别传OF-7；必须编入非助战霍尔海雅并上场，且至少使用2次博览者的狂语</t>
+          <t>&gt; 战斗中非助战淬羽赫默累计使用无畏者协议8次&gt; 3星通关主题曲6-3；必须编入非助战淬羽赫默并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="7" t="inlineStr">
         <is>
-          <t>霍尔海雅</t>
+          <t>淬羽赫默</t>
         </is>
       </c>
       <c r="B308" s="7" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>WB-5</t>
         </is>
       </c>
       <c r="C308" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战霍尔海雅并上场，且每次战斗至少释放1次博览者的狂语&gt; 3星通关主题曲4-3；必须编入非助战霍尔海雅并上场，且使用霍尔海雅至少歼灭10个敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战淬羽赫默并上场，且每次战斗至少释放1次无畏者协议&gt; 3星通关插曲WB-5；必须编入非助战淬羽赫默并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="7" t="inlineStr">
         <is>
-          <t>缪尔赛思</t>
+          <t>霍尔海雅</t>
         </is>
       </c>
       <c r="B309" s="7" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>OF-7</t>
         </is>
       </c>
       <c r="C309" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战缪尔赛思，并确定第一位部署的干员是缪尔赛思&gt; 3星通关主题曲3-4；必须编入非助战缪尔赛思并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 由非助战霍尔海雅累计造成120000点伤害&gt; 3星通关别传OF-7；必须编入非助战霍尔海雅并上场，且至少使用2次博览者的狂语</t>
         </is>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="7" t="inlineStr">
         <is>
-          <t>缪尔赛思</t>
+          <t>霍尔海雅</t>
         </is>
       </c>
       <c r="B310" s="7" t="inlineStr">
         <is>
-          <t>6-12</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C310" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战缪尔赛思并上场，且每次战斗至少释放1次生态耦合&gt; 3星通关主题曲6-12；必须编入非助战缪尔赛思并上场，且使用2次生态耦合</t>
+          <t>&gt; 完成5次战斗；必须编入非助战霍尔海雅并上场，且每次战斗至少释放1次博览者的狂语&gt; 3星通关主题曲4-3；必须编入非助战霍尔海雅并上场，且使用霍尔海雅至少歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="7" t="inlineStr">
         <is>
-          <t>隐现</t>
+          <t>缪尔赛思</t>
         </is>
       </c>
       <c r="B311" s="7" t="inlineStr">
@@ -6086,1418 +6086,1486 @@
       </c>
       <c r="C311" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战隐现累计造成30歼灭数&gt; 3星通关主题曲3-4；必须编入非助战隐现并上场，且不编入其他狙击干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战缪尔赛思，并确定第一位部署的干员是缪尔赛思&gt; 3星通关主题曲3-4；必须编入非助战缪尔赛思并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="7" t="inlineStr">
         <is>
-          <t>空构</t>
+          <t>缪尔赛思</t>
         </is>
       </c>
       <c r="B312" s="7" t="inlineStr">
         <is>
-          <t>DM-2</t>
+          <t>6-12</t>
         </is>
       </c>
       <c r="C312" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战空构累计造成60000点伤害&gt; 3星通关插曲DM-2；必须编入非助战空构并上场，且至少使用1次临场铳械改装</t>
+          <t>&gt; 完成5次战斗；必须编入非助战缪尔赛思并上场，且每次战斗至少释放1次生态耦合&gt; 3星通关主题曲6-12；必须编入非助战缪尔赛思并上场，且使用2次生态耦合</t>
         </is>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="7" t="inlineStr">
         <is>
-          <t>圣约送葬人</t>
+          <t>隐现</t>
         </is>
       </c>
       <c r="B313" s="7" t="inlineStr">
         <is>
-          <t>7-14</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="C313" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战圣约送葬人累计造成80000点伤害&gt; 3星通关主题曲7-14；必须编入非助战圣约送葬人并上场，且使用圣约送葬人歼灭至少2名游击队盾卫</t>
+          <t>&gt; 由非助战隐现累计造成30歼灭数&gt; 3星通关主题曲3-4；必须编入非助战隐现并上场，且不编入其他狙击干员</t>
         </is>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="7" t="inlineStr">
         <is>
-          <t>寒檀</t>
+          <t>空构</t>
         </is>
       </c>
       <c r="B314" s="7" t="inlineStr">
         <is>
-          <t>BI-2</t>
+          <t>DM-2</t>
         </is>
       </c>
       <c r="C314" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战寒檀并上场，且每次战斗至少释放1次“女巫之泪”&gt; 3星通关别传BI-2；必须编入非助战寒檀并上场，且使用寒檀至少歼灭8个敌人</t>
+          <t>&gt; 由非助战空构累计造成60000点伤害&gt; 3星通关插曲DM-2；必须编入非助战空构并上场，且至少使用1次临场铳械改装</t>
         </is>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="7" t="inlineStr">
         <is>
-          <t>提丰</t>
+          <t>圣约送葬人</t>
         </is>
       </c>
       <c r="B315" s="7" t="inlineStr">
         <is>
-          <t>S2-1</t>
+          <t>7-14</t>
         </is>
       </c>
       <c r="C315" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战提丰累计造成120000点伤害&gt; 3星通关主题曲S2-1；必须编入非助战提丰并上场，其他成员仅可编入近战位干员</t>
+          <t>&gt; 由非助战圣约送葬人累计造成80000点伤害&gt; 3星通关主题曲7-14；必须编入非助战圣约送葬人并上场，且使用圣约送葬人歼灭至少2名游击队盾卫</t>
         </is>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="7" t="inlineStr">
         <is>
-          <t>凛视</t>
+          <t>寒檀</t>
         </is>
       </c>
       <c r="B316" s="7" t="inlineStr">
         <is>
-          <t>7-13</t>
+          <t>BI-2</t>
         </is>
       </c>
       <c r="C316" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战凛视累计造成30次凋亡爆发&gt; 3星通关主题曲7-13；必须编入非助战凛视并上场，且凛视造成至少1次凋亡爆发</t>
+          <t>&gt; 完成5次战斗；必须编入非助战寒檀并上场，且每次战斗至少释放1次“女巫之泪”&gt; 3星通关别传BI-2；必须编入非助战寒檀并上场，且使用寒檀至少歼灭8个敌人</t>
         </is>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="7" t="inlineStr">
         <is>
-          <t>苍苔</t>
+          <t>提丰</t>
         </is>
       </c>
       <c r="B317" s="7" t="inlineStr">
         <is>
-          <t>9-3</t>
+          <t>S2-1</t>
         </is>
       </c>
       <c r="C317" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战苍苔并上场，且每次战斗至少释放1次土石的恒心&gt; 3星通关主题曲9-3标准实战环境；必须编入非助战苍苔并上场，且所有干员不被击倒</t>
+          <t>&gt; 由非助战提丰累计造成120000点伤害&gt; 3星通关主题曲S2-1；必须编入非助战提丰并上场，其他成员仅可编入近战位干员</t>
         </is>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="7" t="inlineStr">
         <is>
-          <t>青枳</t>
+          <t>提丰</t>
         </is>
       </c>
       <c r="B318" s="7" t="inlineStr">
         <is>
-          <t>OF-5</t>
+          <t>4-8</t>
         </is>
       </c>
       <c r="C318" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战青枳，并确定第一位部署的干员是青枳&gt; 3星通关别传OF-5；必须编入非助战青枳并上场，且不编入其他先锋干员</t>
+          <t>&gt; 由非助战提丰累计造成30歼灭数&gt; 3星通关主题曲4-8；必须编入非助战提丰并上场，且不编入其他狙击干员</t>
         </is>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="7" t="inlineStr">
         <is>
-          <t>琳琅诗怀雅</t>
+          <t>凛视</t>
         </is>
       </c>
       <c r="B319" s="7" t="inlineStr">
         <is>
-          <t>5-2</t>
+          <t>7-13</t>
         </is>
       </c>
       <c r="C319" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战琳琅诗怀雅累计造成60000点伤害※香槟炸弹造成的伤害也会参与计数&gt; 3星通关主题曲5-2；必须编入非助战琳琅诗怀雅并上场，且使用琳琅诗怀雅至少歼灭15个敌人</t>
+          <t>&gt; 由非助战凛视累计造成30次凋亡爆发&gt; 3星通关主题曲7-13；必须编入非助战凛视并上场，且凛视造成至少1次凋亡爆发</t>
         </is>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="7" t="inlineStr">
         <is>
-          <t>琳琅诗怀雅</t>
+          <t>苍苔</t>
         </is>
       </c>
       <c r="B320" s="7" t="inlineStr">
         <is>
-          <t>11-16</t>
+          <t>9-3</t>
         </is>
       </c>
       <c r="C320" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战琳琅诗怀雅累计造成40歼灭数&gt; 3星通关主题曲11-16标准实战环境；必须编入非助战琳琅诗怀雅并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战苍苔并上场，且每次战斗至少释放1次土石的恒心&gt; 3星通关主题曲9-3标准实战环境；必须编入非助战苍苔并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="7" t="inlineStr">
         <is>
-          <t>纯烬艾雅法拉</t>
+          <t>青枳</t>
         </is>
       </c>
       <c r="B321" s="7" t="inlineStr">
         <is>
-          <t>FC-5</t>
+          <t>OF-5</t>
         </is>
       </c>
       <c r="C321" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战纯烬艾雅法拉并上场，且每次战斗至少释放1次火山回响&gt; 3星通关别传FC-5；必须编入非助战纯烬艾雅法拉并上场，且不编入其他医疗干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战青枳，并确定第一位部署的干员是青枳&gt; 3星通关别传OF-5；必须编入非助战青枳并上场，且不编入其他先锋干员</t>
         </is>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="7" t="inlineStr">
         <is>
-          <t>冰酿</t>
+          <t>琳琅诗怀雅</t>
         </is>
       </c>
       <c r="B322" s="7" t="inlineStr">
         <is>
-          <t>S3-3</t>
+          <t>5-2</t>
         </is>
       </c>
       <c r="C322" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战冰酿累计造成80000伤害&gt; 3星通关主题曲S3-3；必须编入非助战冰酿并上场，且使用冰酿至少歼灭8个敌人</t>
+          <t>&gt; 由非助战琳琅诗怀雅累计造成60000点伤害※香槟炸弹造成的伤害也会参与计数&gt; 3星通关主题曲5-2；必须编入非助战琳琅诗怀雅并上场，且使用琳琅诗怀雅至少歼灭15个敌人</t>
         </is>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="7" t="inlineStr">
         <is>
-          <t>杏仁</t>
+          <t>琳琅诗怀雅</t>
         </is>
       </c>
       <c r="B323" s="7" t="inlineStr">
         <is>
-          <t>BI-2</t>
+          <t>11-16</t>
         </is>
       </c>
       <c r="C323" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战杏仁累计使用强力牵引10次&gt; 3星通关别传BI-2；必须编入非助战杏仁并上场，且至少使用2次强力牵引</t>
+          <t>&gt; 由非助战琳琅诗怀雅累计造成40歼灭数&gt; 3星通关主题曲11-16标准实战环境；必须编入非助战琳琅诗怀雅并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="7" t="inlineStr">
         <is>
-          <t>涤火杰西卡</t>
+          <t>纯烬艾雅法拉</t>
         </is>
       </c>
       <c r="B324" s="7" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>FC-5</t>
         </is>
       </c>
       <c r="C324" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战涤火杰西卡累计造成30歼灭数&gt; 3星通关主题曲3-8；必须编入非助战涤火杰西卡并上场，且使用涤火杰西卡歼灭碎骨</t>
+          <t>&gt; 完成5次战斗；必须编入非助战纯烬艾雅法拉并上场，且每次战斗至少释放1次火山回响&gt; 3星通关别传FC-5；必须编入非助战纯烬艾雅法拉并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="7" t="inlineStr">
         <is>
-          <t>维荻</t>
+          <t>冰酿</t>
         </is>
       </c>
       <c r="B325" s="7" t="inlineStr">
         <is>
-          <t>9-3</t>
+          <t>S3-3</t>
         </is>
       </c>
       <c r="C325" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战维荻累计造成60000点伤害&gt; 3星通关主题曲9-3标准实战环境；必须编入非助战维荻并上场，且至少使用2次双刃毒藤</t>
+          <t>&gt; 由非助战冰酿累计造成80000伤害&gt; 3星通关主题曲S3-3；必须编入非助战冰酿并上场，且使用冰酿至少歼灭8个敌人</t>
         </is>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="7" t="inlineStr">
         <is>
-          <t>戴菲恩</t>
+          <t>杏仁</t>
         </is>
       </c>
       <c r="B326" s="7" t="inlineStr">
         <is>
-          <t>WD-6</t>
+          <t>BI-2</t>
         </is>
       </c>
       <c r="C326" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战戴菲恩累计造成30歼灭数&gt; 3星通关插曲WD-6；必须携带且部署非助战戴菲恩，且至少使用2次抢攻</t>
+          <t>&gt; 战斗中非助战杏仁累计使用强力牵引10次&gt; 3星通关别传BI-2；必须编入非助战杏仁并上场，且至少使用2次强力牵引</t>
         </is>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="7" t="inlineStr">
         <is>
-          <t>刺玫</t>
+          <t>涤火杰西卡</t>
         </is>
       </c>
       <c r="B327" s="7" t="inlineStr">
         <is>
-          <t>IC-2</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C327" s="9" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战刺玫累计使用荆藤庇荫10次&gt; 3星通关别传IC-2；必须编入非助战刺玫并上场，且不编入其他医疗干员</t>
+          <t>&gt; 由非助战涤火杰西卡累计造成30歼灭数&gt; 3星通关主题曲3-8；必须编入非助战涤火杰西卡并上场，且使用涤火杰西卡歼灭碎骨</t>
         </is>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="7" t="inlineStr">
         <is>
-          <t>赫德雷</t>
+          <t>维荻</t>
         </is>
       </c>
       <c r="B328" s="7" t="inlineStr">
         <is>
-          <t>IW-7</t>
+          <t>9-3</t>
         </is>
       </c>
       <c r="C328" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战赫德雷累计歼灭5个精英或领袖敌人&gt; 3星通关别传IW-7；必须编入非助战赫德雷并上场，并使用赫德雷至少击败2名沉沙</t>
+          <t>&gt; 由非助战维荻累计造成60000点伤害&gt; 3星通关主题曲9-3标准实战环境；必须编入非助战维荻并上场，且至少使用2次双刃毒藤</t>
         </is>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="7" t="inlineStr">
         <is>
-          <t>深律</t>
+          <t>戴菲恩</t>
         </is>
       </c>
       <c r="B329" s="7" t="inlineStr">
         <is>
-          <t>LE-4</t>
+          <t>WD-6</t>
         </is>
       </c>
       <c r="C329" s="9" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战深律并上场，且每次战斗至少释放1次沉音宁神&gt; 3星通关别传LE-4；必须编入非助战深律并上场，且所有干员不被击倒</t>
+          <t>&gt; 由非助战戴菲恩累计造成30歼灭数&gt; 3星通关插曲WD-6；必须携带且部署非助战戴菲恩，且至少使用2次抢攻</t>
         </is>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="7" t="inlineStr">
         <is>
-          <t>止颂</t>
+          <t>刺玫</t>
         </is>
       </c>
       <c r="B330" s="7" t="inlineStr">
         <is>
-          <t>7-11</t>
+          <t>IC-2</t>
         </is>
       </c>
       <c r="C330" s="9" t="inlineStr">
         <is>
-          <t>&gt; 由非助战止颂累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲7-11；必须编入非助战止颂并上场，且使用止颂歼灭至少2名雇佣军萨卡兹战士</t>
+          <t>&gt; 战斗中非助战刺玫累计使用荆藤庇荫10次&gt; 3星通关别传IC-2；必须编入非助战刺玫并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="6" t="inlineStr">
         <is>
-          <t>止颂</t>
+          <t>赫德雷</t>
         </is>
       </c>
       <c r="B331" s="6" t="inlineStr">
         <is>
-          <t>TW-5</t>
+          <t>IW-7</t>
         </is>
       </c>
       <c r="C331" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战止颂累计造成120000点伤害&gt; 3星通关别传TW-5；必须编入非助战止颂并上场，且使用止颂击败至少6名敌人</t>
+          <t>&gt; 由非助战赫德雷累计歼灭5个精英或领袖敌人&gt; 3星通关别传IW-7；必须编入非助战赫德雷并上场，并使用赫德雷至少击败2名沉沙</t>
         </is>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="6" t="inlineStr">
         <is>
-          <t>薇薇安娜</t>
+          <t>深律</t>
         </is>
       </c>
       <c r="B332" s="6" t="inlineStr">
         <is>
-          <t>MN-3</t>
+          <t>LE-4</t>
         </is>
       </c>
       <c r="C332" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战薇薇安娜累计歼灭10个精英或领袖敌人&gt; 3星通关别传MN-3；必须编入非助战薇薇安娜并上场，且使用薇薇安娜歼灭“锈铜”奥尔默·英格拉</t>
+          <t>&gt; 完成5次战斗；必须编入非助战深律并上场，且每次战斗至少释放1次沉音宁神&gt; 3星通关别传LE-4；必须编入非助战深律并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="6" t="inlineStr">
         <is>
-          <t>塑心</t>
+          <t>止颂</t>
         </is>
       </c>
       <c r="B333" s="6" t="inlineStr">
         <is>
-          <t>GA-7</t>
+          <t>7-11</t>
         </is>
       </c>
       <c r="C333" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战塑心累计造成75000点凋亡损伤&gt; 3星通关别传GA-7；必须编入非助战塑心并上场，且塑心造成至少15000点凋亡损伤</t>
+          <t>&gt; 由非助战止颂累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲7-11；必须编入非助战止颂并上场，且使用止颂歼灭至少2名雇佣军萨卡兹战士</t>
         </is>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="6" t="inlineStr">
         <is>
-          <t>哈洛德</t>
+          <t>止颂</t>
         </is>
       </c>
       <c r="B334" s="6" t="inlineStr">
         <is>
-          <t>9-13</t>
+          <t>TW-5</t>
         </is>
       </c>
       <c r="C334" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战哈洛德累计使用重症优先8次&gt; 3星通关主题曲9-13标准实战环境；必须编入非助战哈洛德并上场，且所有干员不被击倒</t>
+          <t>&gt; 由非助战止颂累计造成120000点伤害&gt; 3星通关别传TW-5；必须编入非助战止颂并上场，且使用止颂击败至少6名敌人</t>
         </is>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="6" t="inlineStr">
         <is>
-          <t>烈夏</t>
+          <t>薇薇安娜</t>
         </is>
       </c>
       <c r="B335" s="6" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>MN-3</t>
         </is>
       </c>
       <c r="C335" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战烈夏累计造成30歼灭数&gt; 3星通关主题曲4-3；必须编入非助战烈夏并上场，且不编入其他近卫干员</t>
+          <t>&gt; 由非助战薇薇安娜累计歼灭10个精英或领袖敌人&gt; 3星通关别传MN-3；必须编入非助战薇薇安娜并上场，且使用薇薇安娜歼灭“锈铜”奥尔默·英格拉</t>
         </is>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="6" t="inlineStr">
         <is>
-          <t>锏</t>
+          <t>塑心</t>
         </is>
       </c>
       <c r="B336" s="6" t="inlineStr">
         <is>
-          <t>BI-6</t>
+          <t>GA-7</t>
         </is>
       </c>
       <c r="C336" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战锏并上场，且每次战斗至少释放1次归于宁静&gt; 3星通关别传BI-6；必须编入非助战锏并上场，且使用锏至少歼灭10个敌人</t>
+          <t>&gt; 由非助战塑心累计造成75000点凋亡损伤&gt; 3星通关别传GA-7；必须编入非助战塑心并上场，且塑心造成至少15000点凋亡损伤</t>
         </is>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="6" t="inlineStr">
         <is>
-          <t>莱伊</t>
+          <t>哈洛德</t>
         </is>
       </c>
       <c r="B337" s="6" t="inlineStr">
         <is>
-          <t>S9-1</t>
+          <t>9-13</t>
         </is>
       </c>
       <c r="C337" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战莱伊累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲S9-1标准实战环境；必须编入非助战莱伊并上场，且使用莱伊使用至少2次“得见光芒”</t>
+          <t>&gt; 战斗中非助战哈洛德累计使用重症优先8次&gt; 3星通关主题曲9-13标准实战环境；必须编入非助战哈洛德并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="6" t="inlineStr">
         <is>
-          <t>万顷</t>
+          <t>烈夏</t>
         </is>
       </c>
       <c r="B338" s="6" t="inlineStr">
         <is>
-          <t>9-13</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C338" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战万顷累计使用支援号令·γ型10次&gt; 3星通关主题曲9-13标准实战环境；必须编入非助战万顷并上场，且至少使用2次应东风</t>
+          <t>&gt; 由非助战烈夏累计造成30歼灭数&gt; 3星通关主题曲4-3；必须编入非助战烈夏并上场，且不编入其他近卫干员</t>
         </is>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="6" t="inlineStr">
         <is>
-          <t>小满</t>
+          <t>锏</t>
         </is>
       </c>
       <c r="B339" s="6" t="inlineStr">
         <is>
-          <t>9-11</t>
+          <t>BI-6</t>
         </is>
       </c>
       <c r="C339" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战小满累计造成60000点伤害&gt; 3星通关主题曲9-11标准实战环境；必须编入非助战小满并上场，且至少使用2次乡音沉沉</t>
+          <t>&gt; 完成5次战斗；必须编入非助战锏并上场，且每次战斗至少释放1次归于宁静&gt; 3星通关别传BI-6；必须编入非助战锏并上场，且使用锏至少歼灭10个敌人</t>
         </is>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="6" t="inlineStr">
         <is>
-          <t>左乐</t>
+          <t>莱伊</t>
         </is>
       </c>
       <c r="B340" s="6" t="inlineStr">
         <is>
-          <t>WB-5</t>
+          <t>S9-1</t>
         </is>
       </c>
       <c r="C340" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战左乐累计造成40歼灭数&gt; 3星通关别传WB-5；必须编入非助战左乐并上场，且使用左乐至少歼灭8个敌人</t>
+          <t>&gt; 由非助战莱伊累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲S9-1标准实战环境；必须编入非助战莱伊并上场，且使用莱伊使用至少2次“得见光芒”</t>
         </is>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="6" t="inlineStr">
         <is>
-          <t>左乐</t>
+          <t>万顷</t>
         </is>
       </c>
       <c r="B341" s="6" t="inlineStr">
         <is>
-          <t>RI-7</t>
+          <t>9-13</t>
         </is>
       </c>
       <c r="C341" s="3" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战左乐累计造成100000点伤害&gt; 3星通关别传RI-7；必须携带且部署非助战左乐，且至少释放3次佑序有炎</t>
+          <t>&gt; 战斗中非助战万顷累计使用支援号令·γ型10次&gt; 3星通关主题曲9-13标准实战环境；必须编入非助战万顷并上场，且至少使用2次应东风</t>
         </is>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="6" t="inlineStr">
         <is>
-          <t>黍</t>
+          <t>小满</t>
         </is>
       </c>
       <c r="B342" s="6" t="inlineStr">
         <is>
-          <t>11-11</t>
+          <t>9-11</t>
         </is>
       </c>
       <c r="C342" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战黍并上场，且每次战斗至少释放1次离离枯荣&gt; 3星通关主题曲11-11标准实战环境；必须编入非助战黍并上场，且所有干员不被击倒</t>
+          <t>&gt; 由非助战小满累计造成60000点伤害&gt; 3星通关主题曲9-11标准实战环境；必须编入非助战小满并上场，且至少使用2次乡音沉沉</t>
         </is>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="6" t="inlineStr">
         <is>
-          <t>红隼</t>
+          <t>左乐</t>
         </is>
       </c>
       <c r="B343" s="6" t="inlineStr">
         <is>
-          <t>11-18</t>
+          <t>WB-5</t>
         </is>
       </c>
       <c r="C343" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战红隼并上场，且每次战斗至少释放2次醉刃乱舞&gt; 3星通关主题曲11-18标准实战环境；必须编入非助战红隼，且第一位部署红隼、红隼全程不撤退或被击倒</t>
+          <t>&gt; 由非助战左乐累计造成40歼灭数&gt; 3星通关别传WB-5；必须编入非助战左乐并上场，且使用左乐至少歼灭8个敌人</t>
         </is>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="6" t="inlineStr">
         <is>
-          <t>导火索</t>
+          <t>左乐</t>
         </is>
       </c>
       <c r="B344" s="6" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>RI-7</t>
         </is>
       </c>
       <c r="C344" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战导火索累计造成80000点伤害&gt; 3星通关主题曲3-1；必须编入非助战导火索并上场，且使用导火索至少歼灭30个敌人</t>
+          <t>&gt; 使用非助战左乐累计造成100000点伤害&gt; 3星通关别传RI-7；必须携带且部署非助战左乐，且至少释放3次佑序有炎</t>
         </is>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="6" t="inlineStr">
         <is>
-          <t>双月</t>
+          <t>黍</t>
         </is>
       </c>
       <c r="B345" s="6" t="inlineStr">
         <is>
-          <t>3-7</t>
+          <t>11-11</t>
         </is>
       </c>
       <c r="C345" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战双月累计使用全知者的战术10次&gt; 3星通关主题曲3-7；必须编入非助战双月并上场，且至少使用2次全知者的战术</t>
+          <t>&gt; 完成5次战斗；必须编入非助战黍并上场，且每次战斗至少释放1次离离枯荣&gt; 3星通关主题曲11-11标准实战环境；必须编入非助战黍并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="6" t="inlineStr">
         <is>
-          <t>医生</t>
+          <t>红隼</t>
         </is>
       </c>
       <c r="B346" s="6" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>11-18</t>
         </is>
       </c>
       <c r="C346" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战医生累计使用激素手枪8次&gt; 3星通关主题曲2-5；必须编入非助战医生并上场，且不编入医疗干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战红隼并上场，且每次战斗至少释放2次醉刃乱舞&gt; 3星通关主题曲11-18标准实战环境；必须编入非助战红隼，且第一位部署红隼、红隼全程不撤退或被击倒</t>
         </is>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="6" t="inlineStr">
         <is>
-          <t>艾拉</t>
+          <t>导火索</t>
         </is>
       </c>
       <c r="B347" s="6" t="inlineStr">
         <is>
-          <t>DM-EX-1</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="C347" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战艾拉累计部署雷鸣地雷30个&gt; 3星通关插曲DM-EX-1；必须编入非助战艾拉并上场，且使用艾拉歼灭至少2名萨卡兹穿刺手</t>
+          <t>&gt; 由非助战导火索累计造成80000点伤害&gt; 3星通关主题曲3-1；必须编入非助战导火索并上场，且使用导火索至少歼灭30个敌人</t>
         </is>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="6" t="inlineStr">
         <is>
-          <t>露托</t>
+          <t>双月</t>
         </is>
       </c>
       <c r="B348" s="6" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>3-7</t>
         </is>
       </c>
       <c r="C348" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战露托累计使用强磁防卫8次&gt; 3星通关主题曲3-1；必须编入非助战露托并上场，且不编入其他重装干员</t>
+          <t>&gt; 战斗中非助战双月累计使用全知者的战术10次&gt; 3星通关主题曲3-7；必须编入非助战双月并上场，且至少使用2次全知者的战术</t>
         </is>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="6" t="inlineStr">
         <is>
-          <t>奥达</t>
+          <t>医生</t>
         </is>
       </c>
       <c r="B349" s="6" t="inlineStr">
         <is>
-          <t>S3-6</t>
+          <t>2-5</t>
         </is>
       </c>
       <c r="C349" s="3" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战奥达累计使用4次锻锤之力&gt; 3星通关主题曲S3-6；必须携带且部署非助战奥达，其他成员仅可编入4名干员</t>
+          <t>&gt; 战斗中非助战医生累计使用激素手枪8次&gt; 3星通关主题曲2-5；必须编入非助战医生并上场，且不编入医疗干员</t>
         </is>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="6" t="inlineStr">
         <is>
-          <t>阿罗玛</t>
+          <t>艾拉</t>
         </is>
       </c>
       <c r="B350" s="6" t="inlineStr">
         <is>
-          <t>GT-HX-3</t>
+          <t>DM-EX-1</t>
         </is>
       </c>
       <c r="C350" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战阿罗玛并上场，且每次战斗至少释放1次小心地滑&gt; 3星通关别传GT-HX-3；必须编入非助战阿罗玛并上场，且使用阿罗玛至少歼灭20个敌人</t>
+          <t>&gt; 战斗中非助战艾拉累计部署雷鸣地雷30个&gt; 3星通关插曲DM-EX-1；必须编入非助战艾拉并上场，且使用艾拉歼灭至少2名萨卡兹穿刺手</t>
         </is>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="6" t="inlineStr">
         <is>
-          <t>阿斯卡纶</t>
+          <t>露托</t>
         </is>
       </c>
       <c r="B351" s="6" t="inlineStr">
         <is>
-          <t>11-6</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="C351" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战阿斯卡纶累计造成180000点伤害&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战阿斯卡纶并上场，且使用阿斯卡纶至少歼灭30个敌人</t>
+          <t>&gt; 战斗中非助战露托累计使用强磁防卫8次&gt; 3星通关主题曲3-1；必须编入非助战露托并上场，且不编入其他重装干员</t>
         </is>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="6" t="inlineStr">
         <is>
-          <t>阿斯卡纶</t>
+          <t>奥达</t>
         </is>
       </c>
       <c r="B352" s="6" t="inlineStr">
         <is>
-          <t>5-10</t>
+          <t>S3-6</t>
         </is>
       </c>
       <c r="C352" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战阿斯卡纶累计使用“降临”5次&gt; 3星通关主题曲5-10，必须编入非助战阿斯卡纶并上场，其他成员不可编入特种干员</t>
+          <t>&gt; 使用非助战奥达累计使用4次锻锤之力&gt; 3星通关主题曲S3-6；必须携带且部署非助战奥达，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="6" t="inlineStr">
         <is>
-          <t>历阵锐枪芬</t>
+          <t>阿罗玛</t>
         </is>
       </c>
       <c r="B353" s="6" t="inlineStr">
         <is>
-          <t>4-2</t>
+          <t>GT-HX-3</t>
         </is>
       </c>
       <c r="C353" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战历阵锐枪芬，并确定第一位部署的干员是历阵锐枪芬&gt; 3星通关主题曲4-2；必须编入非助战历阵锐枪芬并上场，且不编入其他先锋干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战阿罗玛并上场，且每次战斗至少释放1次小心地滑&gt; 3星通关别传GT-HX-3；必须编入非助战阿罗玛并上场，且使用阿罗玛至少歼灭20个敌人</t>
         </is>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="6" t="inlineStr">
         <is>
-          <t>魔王</t>
+          <t>阿斯卡纶</t>
         </is>
       </c>
       <c r="B354" s="6" t="inlineStr">
         <is>
-          <t>14-5</t>
+          <t>11-6</t>
         </is>
       </c>
       <c r="C354" s="3" t="inlineStr">
         <is>
-          <t>&gt; 携带非助战魔王完成5次战斗，且每次战斗至少发动一次“编织重构现世”&gt; 3星通关主题曲14-5标准实战环境；必须编入非助战魔王并上场，其他成员仅可编入近战位干员</t>
+          <t>&gt; 由非助战阿斯卡纶累计造成180000点伤害&gt; 3星通关主题曲11-6标准实战环境；必须编入非助战阿斯卡纶并上场，且使用阿斯卡纶至少歼灭30个敌人</t>
         </is>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="6" t="inlineStr">
         <is>
-          <t>逻各斯</t>
+          <t>阿斯卡纶</t>
         </is>
       </c>
       <c r="B355" s="6" t="inlineStr">
         <is>
-          <t>14-9</t>
+          <t>5-10</t>
         </is>
       </c>
       <c r="C355" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战逻各斯累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲14-9标准实战环境；必须编入非助战逻各斯并上场，且使用逻各斯至少歼灭7个敌人</t>
+          <t>&gt; 战斗中非助战阿斯卡纶累计使用“降临”5次&gt; 3星通关主题曲5-10，必须编入非助战阿斯卡纶并上场，其他成员不可编入特种干员</t>
         </is>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="6" t="inlineStr">
         <is>
-          <t>逻各斯</t>
+          <t>历阵锐枪芬</t>
         </is>
       </c>
       <c r="B356" s="6" t="inlineStr">
         <is>
-          <t>11-6</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="C356" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战逻各斯累计造成100000点伤害&gt; 3星通关主题曲11-6标准实战环境，必须编入非助战逻各斯并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 完成5次战斗；必须编入非助战历阵锐枪芬，并确定第一位部署的干员是历阵锐枪芬&gt; 3星通关主题曲4-2；必须编入非助战历阵锐枪芬并上场，且不编入其他先锋干员</t>
         </is>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="6" t="inlineStr">
         <is>
-          <t>维什戴尔</t>
+          <t>魔王</t>
         </is>
       </c>
       <c r="B357" s="6" t="inlineStr">
         <is>
-          <t>DM-5</t>
+          <t>14-5</t>
         </is>
       </c>
       <c r="C357" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战维什戴尔累计造成120000伤害&gt; 3星通关插曲DM-5；必须编入非助战维什戴尔并上场，且使用维什戴尔至少歼灭20个敌人</t>
+          <t>&gt; 携带非助战魔王完成5次战斗，且每次战斗至少发动一次“编织重构现世”&gt; 3星通关主题曲14-5标准实战环境；必须编入非助战魔王并上场，其他成员仅可编入近战位干员</t>
         </is>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="6" t="inlineStr">
         <is>
-          <t>阿米娅(医疗)</t>
+          <t>逻各斯</t>
         </is>
       </c>
       <c r="B358" s="6" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>14-9</t>
         </is>
       </c>
       <c r="C358" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战医疗职业的阿米娅累计使用慈悲愿景5次&gt; 3星通关主题曲3-8；必须编入非助战医疗职业的阿米娅并上场，且不编入其他医疗干员</t>
+          <t>&gt; 由非助战逻各斯累计歼灭10个精英或领袖敌人&gt; 3星通关主题曲14-9标准实战环境；必须编入非助战逻各斯并上场，且使用逻各斯至少歼灭7个敌人</t>
         </is>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="6" t="inlineStr">
         <is>
-          <t>深巡</t>
+          <t>逻各斯</t>
         </is>
       </c>
       <c r="B359" s="6" t="inlineStr">
         <is>
-          <t>SN-5</t>
+          <t>11-6</t>
         </is>
       </c>
       <c r="C359" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战深巡累计使用行动能力剥夺8次&gt; 3星通关插曲SN-5，必须编入非助战深巡并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 由非助战逻各斯累计造成100000点伤害&gt; 3星通关主题曲11-6标准实战环境，必须编入非助战逻各斯并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="6" t="inlineStr">
         <is>
-          <t>海霓</t>
+          <t>维什戴尔</t>
         </is>
       </c>
       <c r="B360" s="6" t="inlineStr">
         <is>
-          <t>SV-4</t>
+          <t>DM-5</t>
         </is>
       </c>
       <c r="C360" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战海霓累计使用阻滞性显色剂8次&gt; 3星通关插曲SV-4；必须编入非助战海霓并上场，且不编入其他辅助干员</t>
+          <t>&gt; 由非助战维什戴尔累计造成120000伤害&gt; 3星通关插曲DM-5；必须编入非助战维什戴尔并上场，且使用维什戴尔至少歼灭20个敌人</t>
         </is>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="6" t="inlineStr">
         <is>
-          <t>乌尔比安</t>
+          <t>阿米娅(医疗)</t>
         </is>
       </c>
       <c r="B361" s="6" t="inlineStr">
         <is>
-          <t>SV-6</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C361" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战乌尔比安累计使用必须开辟的通路10次&gt; 3星通关插曲SV-6；必须编入非助战乌尔比安并上场，并使用乌尔比安至少击败2名囊海爬行者</t>
+          <t>&gt; 战斗中非助战医疗职业的阿米娅累计使用慈悲愿景5次&gt; 3星通关主题曲3-8；必须编入非助战医疗职业的阿米娅并上场，且不编入其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="6" t="inlineStr">
         <is>
-          <t>渡桥</t>
+          <t>深巡</t>
         </is>
       </c>
       <c r="B362" s="6" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>SN-5</t>
         </is>
       </c>
       <c r="C362" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战渡桥累计使用承压功率8次&gt; 3星通关主题曲3-1；必须编入非助战渡桥并上场，且至少使用3次承压功率</t>
+          <t>&gt; 战斗中非助战深巡累计使用行动能力剥夺8次&gt; 3星通关插曲SN-5，必须编入非助战深巡并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="6" t="inlineStr">
         <is>
-          <t>锡人</t>
+          <t>海霓</t>
         </is>
       </c>
       <c r="B363" s="6" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>SV-4</t>
         </is>
       </c>
       <c r="C363" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战锡人累计使用8次“大拉里”&gt; 3星通关主题曲4-3，必须编入非助战锡人并上场，且队伍中不能有其他医疗干员</t>
+          <t>&gt; 战斗中非助战海霓累计使用阻滞性显色剂8次&gt; 3星通关插曲SV-4；必须编入非助战海霓并上场，且不编入其他辅助干员</t>
         </is>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="6" t="inlineStr">
         <is>
-          <t>衡沙</t>
+          <t>乌尔比安</t>
         </is>
       </c>
       <c r="B364" s="6" t="inlineStr">
         <is>
-          <t>DV-2</t>
+          <t>SV-6</t>
         </is>
       </c>
       <c r="C364" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中累计召唤非助战衡沙的召唤物20回&gt; 3星通关别传DV-2；必须编入非助战衡沙并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 战斗中非助战乌尔比安累计使用必须开辟的通路10次&gt; 3星通关插曲SV-6；必须编入非助战乌尔比安并上场，并使用乌尔比安至少击败2名囊海爬行者</t>
         </is>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="6" t="inlineStr">
         <is>
-          <t>佩佩</t>
+          <t>渡桥</t>
         </is>
       </c>
       <c r="B365" s="6" t="inlineStr">
         <is>
-          <t>3-8</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="C365" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战佩佩累计造成40歼灭数&gt; 3星通关主题曲3-8；必须编入非助战佩佩并上场，且使用佩佩歼灭碎骨</t>
+          <t>&gt; 战斗中非助战渡桥累计使用承压功率8次&gt; 3星通关主题曲3-1；必须编入非助战渡桥并上场，且至少使用3次承压功率</t>
         </is>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="6" t="inlineStr">
         <is>
-          <t>森西</t>
+          <t>锡人</t>
         </is>
       </c>
       <c r="B366" s="6" t="inlineStr">
         <is>
-          <t>1-12</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C366" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战森西累计使用团体魔物大餐6次&gt; 3星通关主题曲1-12；必须编入非助战森西并上场，且所有干员不被击倒</t>
+          <t>&gt; 战斗中非助战锡人累计使用8次“大拉里”&gt; 3星通关主题曲4-3，必须编入非助战锡人并上场，且队伍中不能有其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="6" t="inlineStr">
         <is>
-          <t>齐尔查克</t>
+          <t>衡沙</t>
         </is>
       </c>
       <c r="B367" s="6" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>DV-2</t>
         </is>
       </c>
       <c r="C367" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战齐尔查克累计使用随机应变6次&gt; 3星通关主题曲4-3；必须编入非助战齐尔查克并上场，其他成员不可编入先锋干员</t>
+          <t>&gt; 战斗中累计召唤非助战衡沙的召唤物20回&gt; 3星通关别传DV-2；必须编入非助战衡沙并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="6" t="inlineStr">
         <is>
-          <t>莱欧斯</t>
+          <t>佩佩</t>
         </is>
       </c>
       <c r="B368" s="6" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>3-8</t>
         </is>
       </c>
       <c r="C368" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战莱欧斯并上场，且每次战斗至少释放1次威吓战法&gt; 3星通关主题曲2-4；必须编入非助战莱欧斯并上场，并使用莱欧斯至少击败1名高阶术师</t>
+          <t>&gt; 由非助战佩佩累计造成40歼灭数&gt; 3星通关主题曲3-8；必须编入非助战佩佩并上场，且使用佩佩歼灭碎骨</t>
         </is>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="6" t="inlineStr">
         <is>
-          <t>玛露西尔</t>
+          <t>森西</t>
         </is>
       </c>
       <c r="B369" s="6" t="inlineStr">
         <is>
-          <t>5-10</t>
+          <t>1-12</t>
         </is>
       </c>
       <c r="C369" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战玛露西尔累计造成100000点伤害&gt; 3星通关主题曲5-10；必须编入非助战玛露西尔并上场，且使用玛露西尔至少歼灭10名敌人</t>
+          <t>&gt; 战斗中非助战森西累计使用团体魔物大餐6次&gt; 3星通关主题曲1-12；必须编入非助战森西并上场，且所有干员不被击倒</t>
         </is>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="6" t="inlineStr">
         <is>
-          <t>凯瑟琳</t>
+          <t>齐尔查克</t>
         </is>
       </c>
       <c r="B370" s="6" t="inlineStr">
         <is>
-          <t>11-7</t>
+          <t>4-3</t>
         </is>
       </c>
       <c r="C370" s="3" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战凯瑟琳累计部署15个“支援装置”&gt; 3星通关主题曲11-7标准实战环境；必须编入非助战凯瑟琳并上场，且凯瑟琳使用至少2次“战火淬炼”</t>
+          <t>&gt; 战斗中非助战齐尔查克累计使用随机应变6次&gt; 3星通关主题曲4-3；必须编入非助战齐尔查克并上场，其他成员不可编入先锋干员</t>
         </is>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="6" t="inlineStr">
         <is>
-          <t>波卜</t>
+          <t>莱欧斯</t>
         </is>
       </c>
       <c r="B371" s="6" t="inlineStr">
         <is>
-          <t>4-8</t>
+          <t>2-4</t>
         </is>
       </c>
       <c r="C371" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战波卜累计造成30次灼燃爆发&gt; 3星通关主题曲4-8；必须编入非助战波卜并上场，且波卜使用至少2次“此路不通”</t>
+          <t>&gt; 完成5次战斗；必须编入非助战莱欧斯并上场，且每次战斗至少释放1次威吓战法&gt; 3星通关主题曲2-4；必须编入非助战莱欧斯并上场，并使用莱欧斯至少击败1名高阶术师</t>
         </is>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="6" t="inlineStr">
         <is>
-          <t>维娜·维多利亚</t>
+          <t>玛露西尔</t>
         </is>
       </c>
       <c r="B372" s="6" t="inlineStr">
         <is>
-          <t>9-5</t>
+          <t>5-10</t>
         </is>
       </c>
       <c r="C372" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战维娜·维多利亚累计造成120000点伤害&gt; 3星通关主题曲9-5标准实战环境；必须编入非助战维娜·维多利亚并上场，其他成员仅可编入5名干员</t>
+          <t>&gt; 由非助战玛露西尔累计造成100000点伤害&gt; 3星通关主题曲5-10；必须编入非助战玛露西尔并上场，且使用玛露西尔至少歼灭10名敌人</t>
         </is>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="6" t="inlineStr">
         <is>
-          <t>裁度</t>
+          <t>凯瑟琳</t>
         </is>
       </c>
       <c r="B373" s="6" t="inlineStr">
         <is>
-          <t>5-8</t>
+          <t>11-7</t>
         </is>
       </c>
       <c r="C373" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战裁度并部署至少2次，且使用裁度击败至少4名敌人&gt; 3星通关主题曲5-8；必须编入非助战裁度并上场，且至少束缚12次敌人</t>
+          <t>&gt; 使用非助战凯瑟琳累计部署15个“支援装置”&gt; 3星通关主题曲11-7标准实战环境；必须编入非助战凯瑟琳并上场，且凯瑟琳使用至少2次“战火淬炼”</t>
         </is>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="6" t="inlineStr">
         <is>
-          <t>弑君者</t>
+          <t>波卜</t>
         </is>
       </c>
       <c r="B374" s="6" t="inlineStr">
         <is>
-          <t>4-4</t>
+          <t>4-8</t>
         </is>
       </c>
       <c r="C374" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；每次战斗至少部署3次非助战弑君者&gt; 3星通关主题曲4-4；必须编入非助战弑君者并上场，且不编入其他特种干员</t>
+          <t>&gt; 由非助战波卜累计造成30次灼燃爆发&gt; 3星通关主题曲4-8；必须编入非助战波卜并上场，且波卜使用至少2次“此路不通”</t>
         </is>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="6" t="inlineStr">
         <is>
-          <t>弑君者</t>
+          <t>维娜·维多利亚</t>
         </is>
       </c>
       <c r="B375" s="6" t="inlineStr">
         <is>
-          <t>4-8</t>
+          <t>9-5</t>
         </is>
       </c>
       <c r="C375" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战弑君者累计使用8次烽烟行刑场&gt; 3星通关主题曲4-8；必须编入非助战弑君者并上场，且使用2次烽烟行刑场</t>
+          <t>&gt; 由非助战维娜·维多利亚累计造成120000点伤害&gt; 3星通关主题曲9-5标准实战环境；必须编入非助战维娜·维多利亚并上场，其他成员仅可编入5名干员</t>
         </is>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="6" t="inlineStr">
         <is>
-          <t>忍冬</t>
+          <t>裁度</t>
         </is>
       </c>
       <c r="B376" s="6" t="inlineStr">
         <is>
-          <t>S2-3</t>
+          <t>5-8</t>
         </is>
       </c>
       <c r="C376" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战忍冬累计造成80000点伤害&gt; 3星通关主题曲S2-3；必须编入非助战忍冬并上场，且使用忍冬击败至少24名敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战裁度并部署至少2次，且使用裁度击败至少4名敌人&gt; 3星通关主题曲5-8；必须编入非助战裁度并上场，且至少束缚12次敌人</t>
         </is>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="6" t="inlineStr">
         <is>
-          <t>荒芜拉普兰德</t>
+          <t>弑君者</t>
         </is>
       </c>
       <c r="B377" s="6" t="inlineStr">
         <is>
-          <t>IS-8</t>
+          <t>4-4</t>
         </is>
       </c>
       <c r="C377" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战荒芜拉普兰德累计造成150000点伤害&gt; 3星通关别传IS-8；必须编入非助战荒芜拉普兰德并上场，且荒芜拉普兰德使用至少2次逐猎狂飙或终幕·浩劫</t>
+          <t>&gt; 完成5次战斗；每次战斗至少部署3次非助战弑君者&gt; 3星通关主题曲4-4；必须编入非助战弑君者并上场，且不编入其他特种干员</t>
         </is>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="6" t="inlineStr">
         <is>
-          <t>瑰盐</t>
+          <t>弑君者</t>
         </is>
       </c>
       <c r="B378" s="6" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>4-8</t>
         </is>
       </c>
       <c r="C378" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战瑰盐累计使用绝妙的长效药呀8次&gt; 3星通关主题曲4-6；必须编入非助战瑰盐并上场，且至少使用1次绝妙的长效药呀</t>
+          <t>&gt; 战斗中非助战弑君者累计使用8次烽烟行刑场&gt; 3星通关主题曲4-8；必须编入非助战弑君者并上场，且使用2次烽烟行刑场</t>
         </is>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="6" t="inlineStr">
         <is>
-          <t>瑰盐</t>
+          <t>忍冬</t>
         </is>
       </c>
       <c r="B379" s="6" t="inlineStr">
         <is>
-          <t>4-6</t>
+          <t>S2-3</t>
         </is>
       </c>
       <c r="C379" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战瑰盐累计使用绝妙的长效药呀8次&gt; 3星通关主题曲4-6；必须编入非助战瑰盐并上场，且至少使用1次绝妙的长效药呀</t>
+          <t>&gt; 由非助战忍冬累计造成80000点伤害&gt; 3星通关主题曲S2-3；必须编入非助战忍冬并上场，且使用忍冬击败至少24名敌人</t>
         </is>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="6" t="inlineStr">
         <is>
-          <t>特克诺</t>
+          <t>荒芜拉普兰德</t>
         </is>
       </c>
       <c r="B380" s="6" t="inlineStr">
         <is>
-          <t>DH-6</t>
+          <t>IS-8</t>
         </is>
       </c>
       <c r="C380" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战特克诺并上场，且每次战斗至少释放1次“恣意挥洒”&gt; 3星通关插曲DH-6，必须编入非助战特克诺并上场，其他成员仅可编入7名干员</t>
+          <t>&gt; 由非助战荒芜拉普兰德累计造成150000点伤害&gt; 3星通关别传IS-8；必须编入非助战荒芜拉普兰德并上场，且荒芜拉普兰德使用至少2次逐猎狂飙或终幕·浩劫</t>
         </is>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="6" t="inlineStr">
         <is>
-          <t>特克诺</t>
+          <t>瑰盐</t>
         </is>
       </c>
       <c r="B381" s="6" t="inlineStr">
         <is>
-          <t>DH-6</t>
+          <t>4-6</t>
         </is>
       </c>
       <c r="C381" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战特克诺并上场，且每次战斗至少释放1次“恣意挥洒”&gt; 3星通关插曲DH-6，必须编入非助战特克诺并上场，其他成员仅可编入7名干员</t>
+          <t>&gt; 战斗中非助战瑰盐累计使用绝妙的长效药呀8次&gt; 3星通关主题曲4-6；必须编入非助战瑰盐并上场，且至少使用1次绝妙的长效药呀</t>
         </is>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="6" t="inlineStr">
         <is>
-          <t>引星棘刺</t>
+          <t>瑰盐</t>
         </is>
       </c>
       <c r="B382" s="6" t="inlineStr">
         <is>
-          <t>OF-7</t>
+          <t>4-6</t>
         </is>
       </c>
       <c r="C382" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战引星棘刺累计使用20次解构涌潮&gt; 3星通关别传OF-7；必须编入非助战引星棘刺并上场，其他成员仅可编入4名干员</t>
+          <t>&gt; 战斗中非助战瑰盐累计使用绝妙的长效药呀8次&gt; 3星通关主题曲4-6；必须编入非助战瑰盐并上场，且至少使用1次绝妙的长效药呀</t>
         </is>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="6" t="inlineStr">
         <is>
-          <t>行箸</t>
+          <t>特克诺</t>
         </is>
       </c>
       <c r="B383" s="6" t="inlineStr">
         <is>
-          <t>3-2</t>
+          <t>DH-6</t>
         </is>
       </c>
       <c r="C383" s="3" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战行箸累计使用8次食不厌精&gt; 3星通关主题曲3-2；必须编入非助战行箸并上场，且所有干员不能被击倒</t>
+          <t>&gt; 完成5次战斗；必须编入非助战特克诺并上场，且每次战斗至少释放1次“恣意挥洒”&gt; 3星通关插曲DH-6，必须编入非助战特克诺并上场，其他成员仅可编入7名干员</t>
         </is>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="6" t="inlineStr">
         <is>
-          <t>寻澜</t>
+          <t>引星棘刺</t>
         </is>
       </c>
       <c r="B384" s="6" t="inlineStr">
         <is>
-          <t>3-5</t>
+          <t>OF-7</t>
         </is>
       </c>
       <c r="C384" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战寻澜并上场，且使用寻澜歼灭至少3个敌人&gt; 3星通关主题曲3-5；必须编入非助战寻澜并上场，且至少使用2次洞悉</t>
+          <t>&gt; 战斗中非助战引星棘刺累计使用20次解构涌潮&gt; 3星通关别传OF-7；必须编入非助战引星棘刺并上场，其他成员仅可编入4名干员</t>
         </is>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="6" t="inlineStr">
         <is>
-          <t>诺威尔</t>
+          <t>行箸</t>
         </is>
       </c>
       <c r="B385" s="6" t="inlineStr">
         <is>
-          <t>5-7</t>
+          <t>3-2</t>
         </is>
       </c>
       <c r="C385" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战诺威尔并上场，且每次战斗至少释放1次生命不息&gt; 3星通关主题曲5-7；必须编入非助战诺威尔并上场，且队伍中不能有其他医疗干员</t>
+          <t>&gt; 使用非助战行箸累计使用8次食不厌精&gt; 3星通关主题曲3-2；必须编入非助战行箸并上场，且所有干员不能被击倒</t>
         </is>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="6" t="inlineStr">
         <is>
-          <t>隐德来希</t>
+          <t>寻澜</t>
         </is>
       </c>
       <c r="B386" s="6" t="inlineStr">
         <is>
-          <t>10-12</t>
+          <t>3-5</t>
         </is>
       </c>
       <c r="C386" s="3" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战隐德来希累计造成100000点伤害&gt; 3星通关主题曲10-12标准实战环境；必须编入非助战隐德来希并上场，且隐德来希至少使用3次灵与欲的惜别</t>
+          <t>&gt; 完成5次战斗；必须编入非助战寻澜并上场，且使用寻澜歼灭至少3个敌人&gt; 3星通关主题曲3-5；必须编入非助战寻澜并上场，且至少使用2次洞悉</t>
         </is>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="6" t="inlineStr">
         <is>
-          <t>钼铅</t>
+          <t>诺威尔</t>
         </is>
       </c>
       <c r="B387" s="6" t="inlineStr">
         <is>
-          <t>9-6</t>
+          <t>5-7</t>
         </is>
       </c>
       <c r="C387" s="3" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战钼铅累计部署矿石“杀手”30个&gt; 3星通关主题曲9-6标准实战环境；必须编入非助战钼铅并上场，且使用钼铅至少击败1名深池重甲卫士</t>
+          <t>&gt; 完成5次战斗；必须编入非助战诺威尔并上场，且每次战斗至少释放1次生命不息&gt; 3星通关主题曲5-7；必须编入非助战诺威尔并上场，且队伍中不能有其他医疗干员</t>
         </is>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="6" t="inlineStr">
         <is>
-          <t>死芒</t>
+          <t>隐德来希</t>
         </is>
       </c>
       <c r="B388" s="6" t="inlineStr">
         <is>
-          <t>4-8</t>
+          <t>10-12</t>
         </is>
       </c>
       <c r="C388" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战死芒并上场，且每次战斗至少释放2次“冠死以冕”&gt; 3星通关主题曲4-8，必须编入非助战死芒并上场，其他成员仅可编入辅助干员</t>
+          <t>&gt; 使用非助战隐德来希累计造成100000点伤害&gt; 3星通关主题曲10-12标准实战环境；必须编入非助战隐德来希并上场，且隐德来希至少使用3次灵与欲的惜别</t>
         </is>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="6" t="inlineStr">
         <is>
-          <t>骋风</t>
+          <t>钼铅</t>
         </is>
       </c>
       <c r="B389" s="6" t="inlineStr">
         <is>
-          <t>SN-2</t>
+          <t>9-6</t>
         </is>
       </c>
       <c r="C389" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战骋风并上场，且每次战斗至少释放1次招无虚发&gt; 3星通关插曲SN-2；必须编入非助战骋风并上场，且使用2次招无虚发</t>
+          <t>&gt; 战斗中非助战钼铅累计部署矿石“杀手”30个&gt; 3星通关主题曲9-6标准实战环境；必须编入非助战钼铅并上场，且使用钼铅至少击败1名深池重甲卫士</t>
         </is>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="6" t="inlineStr">
         <is>
-          <t>阿兰娜</t>
+          <t>死芒</t>
         </is>
       </c>
       <c r="B390" s="6" t="inlineStr">
         <is>
-          <t>7-14</t>
+          <t>4-8</t>
         </is>
       </c>
       <c r="C390" s="3" t="inlineStr">
         <is>
-          <t>&gt; 使用非助战阿兰娜累计部署15个“支援装置”&gt; 3星通关主题曲7-14；必须编入非助战阿兰娜并上场，且至少使用2次“万斤顶”</t>
+          <t>&gt; 完成5次战斗；必须编入非助战死芒并上场，且每次战斗至少释放2次“冠死以冕”&gt; 3星通关主题曲4-8，必须编入非助战死芒并上场，其他成员仅可编入辅助干员</t>
         </is>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="6" t="inlineStr">
         <is>
-          <t>信仰搅拌机</t>
+          <t>骋风</t>
         </is>
       </c>
       <c r="B391" s="6" t="inlineStr">
         <is>
-          <t>14-5</t>
+          <t>SN-2</t>
         </is>
       </c>
       <c r="C391" s="3" t="inlineStr">
         <is>
-          <t>&gt; 完成5次战斗；必须编入非助战信仰搅拌机并上场，且每次战斗至少释放1次退休前布道&gt; 3星通关主题曲14-5标准实战环境；必须编入非助战信仰搅拌机并上场，且使用信仰搅拌机歼灭至少10名敌人</t>
+          <t>&gt; 完成5次战斗；必须编入非助战骋风并上场，且每次战斗至少释放1次招无虚发&gt; 3星通关插曲SN-2；必须编入非助战骋风并上场，且使用2次招无虚发</t>
         </is>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="6" t="inlineStr">
         <is>
-          <t>蕾缪安</t>
+          <t>阿兰娜</t>
         </is>
       </c>
       <c r="B392" s="6" t="inlineStr">
         <is>
-          <t>13-13</t>
+          <t>7-14</t>
         </is>
       </c>
       <c r="C392" s="3" t="inlineStr">
         <is>
-          <t>&gt; 由非助战蕾缪安累计造成30歼灭数&gt; 3星通关主题曲13-13标准实战环境；必须编入非助战蕾缪安并上场，且蕾缪安歼灭至少2个萨卡兹骸骨鞭笞者</t>
+          <t>&gt; 使用非助战阿兰娜累计部署15个“支援装置”&gt; 3星通关主题曲7-14；必须编入非助战阿兰娜并上场，且至少使用2次“万斤顶”</t>
         </is>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="10" t="inlineStr">
         <is>
-          <t>新约能天使</t>
+          <t>信仰搅拌机</t>
         </is>
       </c>
       <c r="B393" s="10" t="inlineStr">
         <is>
-          <t>GA-EX-5</t>
+          <t>14-5</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>&gt; 战斗中非助战新约能天使累计使用开火成瘾症8次&gt; 3星通关插曲GA-EX-5；必须编入非助战新约能天使并上场，且使用2次开火成瘾症</t>
+          <t>&gt; 完成5次战斗；必须编入非助战信仰搅拌机并上场，且每次战斗至少释放1次退休前布道&gt; 3星通关主题曲14-5标准实战环境；必须编入非助战信仰搅拌机并上场，且使用信仰搅拌机歼灭至少10名敌人</t>
         </is>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="10" t="inlineStr">
         <is>
+          <t>蕾缪安</t>
+        </is>
+      </c>
+      <c r="B394" s="10" t="inlineStr">
+        <is>
+          <t>13-13</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>&gt; 由非助战蕾缪安累计造成30歼灭数&gt; 3星通关主题曲13-13标准实战环境；必须编入非助战蕾缪安并上场，且蕾缪安歼灭至少2个萨卡兹骸骨鞭笞者</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="10" t="inlineStr">
+        <is>
+          <t>新约能天使</t>
+        </is>
+      </c>
+      <c r="B395" s="10" t="inlineStr">
+        <is>
+          <t>GA-EX-5</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>&gt; 战斗中非助战新约能天使累计使用开火成瘾症8次&gt; 3星通关插曲GA-EX-5；必须编入非助战新约能天使并上场，且使用2次开火成瘾症</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="10" t="inlineStr">
+        <is>
           <t>酒神</t>
         </is>
       </c>
-      <c r="B394" s="10" t="inlineStr">
+      <c r="B396" s="10" t="inlineStr">
         <is>
           <t>9-6</t>
         </is>
       </c>
-      <c r="C394" t="inlineStr">
+      <c r="C396" t="inlineStr">
         <is>
           <t>&gt; 使用非助战酒神累计造成60000点神经损伤&gt; 3星通关主题曲9-6标准实战环境，必须编入非助战酒神并上场，且酒神使用至少2次“空剧场”</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="10" t="inlineStr">
+        <is>
+          <t>录武官</t>
+        </is>
+      </c>
+      <c r="B397" s="10" t="inlineStr">
+        <is>
+          <t>HS-5</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>&gt; 战斗中非助战录武官累计使用“一点关窍”6次&gt; 3星通关插曲HS-5，必须编入非助战录武官并上场，且不编入其他医疗干员</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="10" t="inlineStr">
+        <is>
+          <t>司霆惊蛰</t>
+        </is>
+      </c>
+      <c r="B398" s="10" t="inlineStr">
+        <is>
+          <t>DV-7</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>&gt; 由非助战司霆惊蛰累计造成120000点伤害&gt; 3星通关插曲DV-7；必须编入非助战司霆惊蛰并上场，且使用1次“天地通明”</t>
         </is>
       </c>
     </row>

</xml_diff>